<commit_message>
Adjust water/sanitation urban/rural calculations
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B4DFE5-8608-9D4B-9B0F-0A0B870DFF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34714A6-5E0A-D846-B94E-1465CF8ADAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="174">
   <si>
     <t>uhc</t>
   </si>
@@ -512,9 +512,6 @@
     <t>NCD_BMI_PLUS2C</t>
   </si>
   <si>
-    <t>NCD_CCS_SatFat</t>
-  </si>
-  <si>
     <t>IHRSPAR_CAPACITY01</t>
   </si>
   <si>
@@ -552,13 +549,19 @@
   </si>
   <si>
     <t>IHRSPAR_CAPACITY13</t>
+  </si>
+  <si>
+    <t>UHCTRANSFATS</t>
+  </si>
+  <si>
+    <t>WSH_SANITATION_SAFELY_MANAGED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -578,12 +581,6 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF586E75"/>
-      <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -619,13 +616,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -633,13 +629,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -710,6 +699,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -727,9 +723,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F64" totalsRowShown="0">
   <autoFilter ref="A1:F64" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
@@ -1003,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1185,7 +1181,7 @@
         <v>98</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
@@ -1201,7 +1197,7 @@
         <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
@@ -1217,7 +1213,7 @@
         <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
@@ -1233,7 +1229,7 @@
         <v>101</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
@@ -1249,7 +1245,7 @@
         <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
@@ -1265,7 +1261,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
@@ -1281,7 +1277,7 @@
         <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
@@ -1297,7 +1293,7 @@
         <v>105</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="2"/>
@@ -1313,7 +1309,7 @@
         <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
@@ -1329,7 +1325,7 @@
         <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
@@ -1345,7 +1341,7 @@
         <v>108</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
@@ -1361,7 +1357,7 @@
         <v>109</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
@@ -1377,7 +1373,7 @@
         <v>110</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
@@ -1392,7 +1388,6 @@
       <c r="B24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="3"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2">
@@ -1406,7 +1401,6 @@
       <c r="B25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="3"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2">
@@ -1420,7 +1414,6 @@
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="3"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
@@ -1482,7 +1475,7 @@
       <c r="B30" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="1" t="s">
         <v>135</v>
       </c>
       <c r="D30" s="2">
@@ -1498,7 +1491,6 @@
       <c r="B31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="3"/>
       <c r="D31" s="2">
         <v>1</v>
       </c>
@@ -1528,7 +1520,7 @@
       <c r="B33" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1546,7 +1538,7 @@
       <c r="B34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D34" s="2"/>
@@ -1562,7 +1554,7 @@
       <c r="B35" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="2"/>
@@ -1578,7 +1570,7 @@
       <c r="B36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D36" s="2"/>
@@ -1594,7 +1586,7 @@
       <c r="B37" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D37" s="2"/>
@@ -1610,7 +1602,7 @@
       <c r="B38" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="1" t="s">
         <v>152</v>
       </c>
       <c r="D38" s="2"/>
@@ -1626,7 +1618,7 @@
       <c r="B39" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="1" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2"/>
@@ -1754,7 +1746,7 @@
       <c r="B47" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D47" s="2">
@@ -1917,7 +1909,7 @@
         <v>118</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2">
@@ -1933,7 +1925,7 @@
         <v>121</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2">
@@ -1949,7 +1941,7 @@
         <v>122</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2">
@@ -2028,8 +2020,8 @@
       <c r="B64" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>159</v>
+      <c r="C64" s="5" t="s">
+        <v>172</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2">
@@ -2040,7 +2032,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D2:F64">
-    <cfRule type="containsText" dxfId="0" priority="133" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="3" priority="133" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2053,6 +2045,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
@@ -2144,15 +2145,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2373,6 +2365,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2385,14 +2385,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Implement load_billions_data to access data stored on the xMart
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87781A8-6CD7-764B-905E-680CEDD499F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B57367-FB49-544A-BED6-7AD954FE9559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="185">
   <si>
     <t>uhc</t>
   </si>
@@ -242,9 +242,6 @@
     <t>fpg</t>
   </si>
   <si>
-    <t>ihr</t>
-  </si>
-  <si>
     <t>beds</t>
   </si>
   <si>
@@ -329,45 +326,6 @@
     <t>polio</t>
   </si>
   <si>
-    <t>ihr1</t>
-  </si>
-  <si>
-    <t>ihr2</t>
-  </si>
-  <si>
-    <t>ihr3</t>
-  </si>
-  <si>
-    <t>ihr4</t>
-  </si>
-  <si>
-    <t>ihr5</t>
-  </si>
-  <si>
-    <t>ihr6</t>
-  </si>
-  <si>
-    <t>ihr7</t>
-  </si>
-  <si>
-    <t>ihr8</t>
-  </si>
-  <si>
-    <t>ihr9</t>
-  </si>
-  <si>
-    <t>ihr10</t>
-  </si>
-  <si>
-    <t>ihr11</t>
-  </si>
-  <si>
-    <t>ihr12</t>
-  </si>
-  <si>
-    <t>ihr13</t>
-  </si>
-  <si>
     <t>respond</t>
   </si>
   <si>
@@ -555,6 +513,81 @@
   </si>
   <si>
     <t>WSH_SANITATION_SAFELY_MANAGED</t>
+  </si>
+  <si>
+    <t>yellow_fever_campaign</t>
+  </si>
+  <si>
+    <t>yellow_fever_routine</t>
+  </si>
+  <si>
+    <t>cholera_campaign</t>
+  </si>
+  <si>
+    <t>cholera_campaign_denom</t>
+  </si>
+  <si>
+    <t>meningitis_routine</t>
+  </si>
+  <si>
+    <t>meningitis_campaign</t>
+  </si>
+  <si>
+    <t>meningitis_campaign_denom</t>
+  </si>
+  <si>
+    <t>measles_routine</t>
+  </si>
+  <si>
+    <t>yellow_fever_campaign_denom</t>
+  </si>
+  <si>
+    <t>polio_routine</t>
+  </si>
+  <si>
+    <t>surviving_infants</t>
+  </si>
+  <si>
+    <t>espar10</t>
+  </si>
+  <si>
+    <t>espar11</t>
+  </si>
+  <si>
+    <t>espar12</t>
+  </si>
+  <si>
+    <t>espar13</t>
+  </si>
+  <si>
+    <t>espar01</t>
+  </si>
+  <si>
+    <t>espar02</t>
+  </si>
+  <si>
+    <t>espar03</t>
+  </si>
+  <si>
+    <t>espar04</t>
+  </si>
+  <si>
+    <t>espar05</t>
+  </si>
+  <si>
+    <t>espar06</t>
+  </si>
+  <si>
+    <t>espar07</t>
+  </si>
+  <si>
+    <t>espar08</t>
+  </si>
+  <si>
+    <t>espar09</t>
+  </si>
+  <si>
+    <t>espar</t>
   </si>
 </sst>
 </file>
@@ -616,13 +649,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -720,8 +754,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F64" totalsRowShown="0">
-  <autoFilter ref="A1:F64" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F75" totalsRowShown="0">
+  <autoFilter ref="A1:F75" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="6">
     <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
@@ -997,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1035,7 +1069,7 @@
         <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -1044,7 +1078,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1052,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
@@ -1062,11 +1096,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="2"/>
@@ -1076,11 +1108,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
@@ -1091,10 +1121,10 @@
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -1105,10 +1135,10 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
@@ -1119,10 +1149,10 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
@@ -1133,10 +1163,10 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
@@ -1146,11 +1176,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>96</v>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
@@ -1161,10 +1189,10 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
@@ -1174,48 +1202,36 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>165</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>166</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
         <v>1</v>
@@ -1223,15 +1239,13 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
         <v>1</v>
@@ -1239,15 +1253,13 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
         <v>1</v>
@@ -1255,47 +1267,37 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
         <v>1</v>
@@ -1303,13 +1305,13 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
@@ -1319,13 +1321,13 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
@@ -1335,13 +1337,13 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
@@ -1351,13 +1353,13 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>109</v>
+        <v>178</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
@@ -1367,13 +1369,13 @@
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>110</v>
+        <v>179</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
@@ -1383,12 +1385,15 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2">
         <v>1</v>
@@ -1396,12 +1401,15 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>181</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2">
         <v>1</v>
@@ -1409,12 +1417,15 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
         <v>1</v>
@@ -1422,188 +1433,168 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>22</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>131</v>
+      <c r="A29" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>132</v>
+      <c r="A30" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="2">
-        <v>1</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
+      <c r="A32" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>151</v>
+        <v>97</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="2">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
+      <c r="A33" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="6"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="6"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="2">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="6"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="2">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
+      <c r="A37" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="2">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
+      <c r="A38" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2">
@@ -1611,31 +1602,31 @@
       </c>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>80</v>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2">
-        <v>1</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>38</v>
+      <c r="A40" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -1644,14 +1635,14 @@
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>39</v>
+      <c r="A41" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -1660,14 +1651,11 @@
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>139</v>
+      <c r="A42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -1675,305 +1663,305 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>63</v>
+        <v>30</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D44" s="2">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>66</v>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>64</v>
+      <c r="A46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>65</v>
+      <c r="A47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2">
+        <v>1</v>
+      </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>46</v>
+      <c r="A48" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>36</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="2">
-        <v>1</v>
-      </c>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2">
-        <v>1</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>88</v>
+        <v>40</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2">
-        <v>1</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>82</v>
+        <v>41</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2">
-        <v>1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2">
-        <v>1</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>120</v>
+        <v>43</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>118</v>
+        <v>44</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>121</v>
+        <v>45</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2">
-        <v>1</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>53</v>
+      <c r="A59" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2">
-        <v>1</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>83</v>
+        <v>47</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2">
-        <v>1</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+      <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
@@ -1981,31 +1969,33 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>84</v>
+        <v>184</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2">
-        <v>1</v>
-      </c>
-      <c r="F62" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2">
@@ -2015,13 +2005,13 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>172</v>
+        <v>87</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2">
@@ -2029,9 +2019,185 @@
       </c>
       <c r="F64" s="2"/>
     </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2">
+        <v>1</v>
+      </c>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2">
+        <v>1</v>
+      </c>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2">
+        <v>1</v>
+      </c>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2">
+        <v>1</v>
+      </c>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2">
+        <v>1</v>
+      </c>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2">
+        <v>1</v>
+      </c>
+      <c r="F75" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F64">
+  <conditionalFormatting sqref="D2:F75">
     <cfRule type="containsText" dxfId="3" priority="133" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
@@ -2045,109 +2211,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2364,7 +2427,129 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2381,29 +2566,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Allow argument passing to xmart4::xmart_table in `load_billion_data()`
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560AAF72-1BCF-E747-8862-11719CD47ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C619CFC-0827-FB49-89A5-DAF0A581D787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,7 +755,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F75" totalsRowShown="0">
-  <autoFilter ref="A1:F75" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
+  <autoFilter ref="A1:F75" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}">
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
@@ -1033,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1586,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
@@ -1602,7 +1608,7 @@
       </c>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>58</v>
       </c>
@@ -1618,7 +1624,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
@@ -1634,7 +1640,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>118</v>
       </c>
@@ -1650,7 +1656,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>29</v>
       </c>
@@ -1663,7 +1669,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>30</v>
       </c>
@@ -1679,7 +1685,7 @@
       </c>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>31</v>
       </c>
@@ -1697,7 +1703,7 @@
       </c>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>32</v>
       </c>
@@ -1713,7 +1719,7 @@
       </c>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>33</v>
       </c>
@@ -1729,7 +1735,7 @@
       </c>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>34</v>
       </c>
@@ -1745,7 +1751,7 @@
       </c>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>35</v>
       </c>
@@ -1761,7 +1767,7 @@
       </c>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>36</v>
       </c>
@@ -1777,7 +1783,7 @@
       </c>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>37</v>
       </c>
@@ -1793,7 +1799,7 @@
       </c>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>38</v>
       </c>
@@ -1809,7 +1815,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>39</v>
       </c>
@@ -1825,7 +1831,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>40</v>
       </c>
@@ -1841,7 +1847,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>41</v>
       </c>
@@ -1857,7 +1863,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>42</v>
       </c>
@@ -1873,7 +1879,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>43</v>
       </c>
@@ -1889,7 +1895,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>44</v>
       </c>
@@ -1905,7 +1911,7 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>45</v>
       </c>
@@ -1921,7 +1927,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>46</v>
       </c>
@@ -1937,7 +1943,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
@@ -1953,7 +1959,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>48</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>50</v>
       </c>
@@ -2003,7 +2009,7 @@
       </c>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -2019,7 +2025,7 @@
       </c>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>52</v>
       </c>
@@ -2035,7 +2041,7 @@
       </c>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>52</v>
       </c>
@@ -2051,7 +2057,7 @@
       </c>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>52</v>
       </c>
@@ -2067,7 +2073,7 @@
       </c>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>53</v>
       </c>
@@ -2083,7 +2089,7 @@
       </c>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>53</v>
       </c>
@@ -2099,7 +2105,7 @@
       </c>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>53</v>
       </c>
@@ -2115,7 +2121,7 @@
       </c>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>54</v>
       </c>
@@ -2131,7 +2137,7 @@
       </c>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>55</v>
       </c>
@@ -2147,7 +2153,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>56</v>
       </c>
@@ -2163,7 +2169,7 @@
       </c>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>57</v>
       </c>
@@ -2179,7 +2185,7 @@
       </c>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>59</v>
       </c>
@@ -2211,100 +2217,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2521,6 +2433,100 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2531,23 +2537,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2566,6 +2555,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Increase number of HEP indicators
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C619CFC-0827-FB49-89A5-DAF0A581D787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26149DDB-9D59-9641-8F49-0F5DFAD54224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="191">
   <si>
     <t>uhc</t>
   </si>
@@ -588,6 +588,24 @@
   </si>
   <si>
     <t>espar</t>
+  </si>
+  <si>
+    <t>meningitis_campaign_denom_sum</t>
+  </si>
+  <si>
+    <t>meningitis_campaign_sum</t>
+  </si>
+  <si>
+    <t>cholera_campaign_sum</t>
+  </si>
+  <si>
+    <t>cholera_campaign_denom_sum</t>
+  </si>
+  <si>
+    <t>yellow_fever_campaign_denom_sum</t>
+  </si>
+  <si>
+    <t>yellow_fever_campaign_sum</t>
   </si>
 </sst>
 </file>
@@ -662,7 +680,28 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -733,13 +772,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -754,18 +786,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F75" totalsRowShown="0">
-  <autoFilter ref="A1:F75" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F81" totalsRowShown="0">
+  <autoFilter ref="A1:F81" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
@@ -1037,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,11 +1152,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -1140,11 +1164,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
@@ -1155,10 +1177,10 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
@@ -1169,10 +1191,10 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
@@ -1182,9 +1204,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>167</v>
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
@@ -1195,10 +1219,10 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
@@ -1209,8 +1233,8 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
-        <v>164</v>
+      <c r="B11" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
@@ -1220,9 +1244,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -1234,7 +1260,7 @@
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
@@ -1244,11 +1270,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
@@ -1258,11 +1282,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -1272,11 +1294,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -1286,9 +1306,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>169</v>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
@@ -1298,9 +1318,11 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>170</v>
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
@@ -1311,15 +1333,13 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
         <v>1</v>
@@ -1327,47 +1347,37 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
         <v>1</v>
@@ -1375,13 +1385,13 @@
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
@@ -1391,13 +1401,13 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="2"/>
@@ -1407,13 +1417,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
@@ -1423,13 +1433,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
@@ -1439,13 +1449,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="2"/>
@@ -1455,13 +1465,13 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="2"/>
@@ -1471,13 +1481,13 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="2"/>
@@ -1487,13 +1497,13 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
@@ -1503,13 +1513,13 @@
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="2"/>
@@ -1519,12 +1529,15 @@
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2">
         <v>1</v>
@@ -1532,47 +1545,59 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" s="6"/>
+      <c r="A36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2">
@@ -1581,10 +1606,10 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1592,190 +1617,165 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="2">
-        <v>1</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="D48" s="2">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2">
-        <v>1</v>
-      </c>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2">
@@ -1783,127 +1783,129 @@
       </c>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2">
+        <v>1</v>
+      </c>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="D56" s="2"/>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D53" s="2">
-        <v>1</v>
-      </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="D57" s="2">
         <v>1</v>
@@ -1911,15 +1913,15 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
@@ -1927,15 +1929,15 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>72</v>
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
@@ -1943,15 +1945,15 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D60" s="2">
         <v>1</v>
@@ -1959,15 +1961,15 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
@@ -1977,127 +1979,127 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2">
-        <v>1</v>
-      </c>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2">
-        <v>1</v>
-      </c>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2">
-        <v>1</v>
-      </c>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2">
-        <v>1</v>
-      </c>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2">
-        <v>1</v>
-      </c>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2">
@@ -2105,15 +2107,15 @@
       </c>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2">
@@ -2121,15 +2123,15 @@
       </c>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2">
@@ -2137,31 +2139,31 @@
       </c>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2">
+        <v>1</v>
+      </c>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2">
@@ -2169,15 +2171,15 @@
       </c>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2">
@@ -2185,15 +2187,15 @@
       </c>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>158</v>
+        <v>107</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2">
@@ -2201,11 +2203,117 @@
       </c>
       <c r="F75" s="2"/>
     </row>
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2">
+        <v>1</v>
+      </c>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2">
+        <v>1</v>
+      </c>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2">
+        <v>1</v>
+      </c>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2">
+        <v>1</v>
+      </c>
+      <c r="F81" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F75">
-    <cfRule type="containsText" dxfId="3" priority="133" operator="containsText" text="1">
+  <conditionalFormatting sqref="D2:F4 D7:F39 D42:F81">
+    <cfRule type="containsText" dxfId="2" priority="135" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:F6">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:F41">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2434,6 +2542,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
@@ -2527,15 +2644,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
@@ -2556,6 +2664,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2570,12 +2686,4 @@
     <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement HEP Billion pipeline
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26149DDB-9D59-9641-8F49-0F5DFAD54224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77EED74-8870-BA46-8582-D9D8611CADC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="185">
   <si>
     <t>uhc</t>
   </si>
@@ -588,24 +588,6 @@
   </si>
   <si>
     <t>espar</t>
-  </si>
-  <si>
-    <t>meningitis_campaign_denom_sum</t>
-  </si>
-  <si>
-    <t>meningitis_campaign_sum</t>
-  </si>
-  <si>
-    <t>cholera_campaign_sum</t>
-  </si>
-  <si>
-    <t>cholera_campaign_denom_sum</t>
-  </si>
-  <si>
-    <t>yellow_fever_campaign_denom_sum</t>
-  </si>
-  <si>
-    <t>yellow_fever_campaign_sum</t>
   </si>
 </sst>
 </file>
@@ -680,21 +662,7 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -786,12 +754,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F81" totalsRowShown="0">
-  <autoFilter ref="A1:F81" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F75" totalsRowShown="0">
+  <autoFilter ref="A1:F75" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
@@ -1063,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1152,9 +1120,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>187</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -1164,9 +1134,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>188</v>
+        <v>90</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
@@ -1177,10 +1149,10 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
@@ -1191,10 +1163,10 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
@@ -1204,11 +1176,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>91</v>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
@@ -1219,10 +1189,10 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
@@ -1233,8 +1203,8 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>167</v>
+      <c r="B11" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
@@ -1244,11 +1214,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -1260,7 +1228,7 @@
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
@@ -1270,9 +1238,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="B14" s="3" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
@@ -1282,9 +1252,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B15" s="3" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -1294,9 +1266,11 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -1306,9 +1280,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
-        <v>185</v>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
@@ -1318,11 +1292,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>94</v>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
@@ -1333,13 +1305,15 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
         <v>1</v>
@@ -1347,37 +1321,47 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
         <v>1</v>
@@ -1385,13 +1369,13 @@
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
@@ -1401,13 +1385,13 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="2"/>
@@ -1417,13 +1401,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
@@ -1433,13 +1417,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
@@ -1449,13 +1433,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="2"/>
@@ -1465,13 +1449,13 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="2"/>
@@ -1481,13 +1465,13 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="2"/>
@@ -1497,13 +1481,13 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
@@ -1513,13 +1497,13 @@
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="2"/>
@@ -1529,15 +1513,12 @@
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2">
         <v>1</v>
@@ -1545,59 +1526,47 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D34" s="3"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D35" s="3"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="6"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2">
@@ -1606,10 +1575,10 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1618,89 +1587,111 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C38" s="6"/>
+      <c r="A38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2">
-        <v>1</v>
-      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
+      <c r="A39" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="B39" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
       <c r="E39" s="2"/>
-      <c r="F39" s="2">
-        <v>1</v>
-      </c>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
+      <c r="A40" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="B40" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="2">
-        <v>1</v>
-      </c>
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
+      <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="B41" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
       <c r="E41" s="2"/>
-      <c r="F41" s="2">
-        <v>1</v>
-      </c>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="2"/>
+      <c r="A42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
       <c r="E42" s="2"/>
-      <c r="F42" s="2">
-        <v>1</v>
-      </c>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>28</v>
+      <c r="A43" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>99</v>
+        <v>73</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2">
-        <v>1</v>
-      </c>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>47</v>
+      <c r="A44" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E44" s="2">
         <v>1</v>
       </c>
@@ -1708,74 +1699,77 @@
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>61</v>
+        <v>32</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>117</v>
+      <c r="A46" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>118</v>
+      <c r="A47" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2">
+        <v>1</v>
+      </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>29</v>
+      <c r="A48" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2">
@@ -1783,129 +1777,127 @@
       </c>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D50" s="2"/>
       <c r="E50" s="2">
         <v>1</v>
       </c>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>32</v>
+      <c r="A51" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2">
-        <v>1</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>33</v>
+      <c r="A52" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2">
-        <v>1</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>76</v>
+      <c r="A53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2">
-        <v>1</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>77</v>
+        <v>41</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2">
-        <v>1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2">
-        <v>1</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>79</v>
+        <v>43</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>71</v>
+        <v>44</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D57" s="2">
         <v>1</v>
@@ -1915,13 +1907,13 @@
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>101</v>
+        <v>45</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
@@ -1930,14 +1922,14 @@
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>68</v>
+      <c r="A59" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
@@ -1947,13 +1939,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D60" s="2">
         <v>1</v>
@@ -1961,15 +1953,15 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
@@ -1979,127 +1971,127 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D62" s="2">
         <v>1</v>
       </c>
       <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="F62" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D63" s="2">
-        <v>1</v>
-      </c>
-      <c r="E63" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2">
+        <v>1</v>
+      </c>
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D64" s="2">
-        <v>1</v>
-      </c>
-      <c r="E64" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2">
+        <v>1</v>
+      </c>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>46</v>
+      <c r="A65" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D65" s="2">
-        <v>1</v>
-      </c>
-      <c r="E65" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2">
+        <v>1</v>
+      </c>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>102</v>
+        <v>52</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2">
+        <v>1</v>
+      </c>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2">
+        <v>1</v>
+      </c>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>184</v>
+        <v>104</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2">
-        <v>1</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2">
+        <v>1</v>
+      </c>
+      <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2">
@@ -2109,13 +2101,13 @@
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2">
@@ -2125,13 +2117,13 @@
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2">
@@ -2141,29 +2133,29 @@
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>105</v>
+        <v>55</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2">
-        <v>1</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2">
@@ -2173,13 +2165,13 @@
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2">
@@ -2189,13 +2181,13 @@
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>159</v>
+        <v>85</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2">
@@ -2203,117 +2195,11 @@
       </c>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2">
-        <v>1</v>
-      </c>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2">
-        <v>1</v>
-      </c>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2">
-        <v>1</v>
-      </c>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2">
-        <v>1</v>
-      </c>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F4 D7:F39 D42:F81">
-    <cfRule type="containsText" dxfId="2" priority="135" operator="containsText" text="1">
+  <conditionalFormatting sqref="D2:F75">
+    <cfRule type="containsText" dxfId="0" priority="135" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:F6">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40:F41">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2325,6 +2211,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2541,15 +2436,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2645,6 +2531,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2659,14 +2553,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update indicator_df to include HEP components dashboard IDs
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77EED74-8870-BA46-8582-D9D8611CADC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E141AB-5793-AB40-A5F6-68AD6D032B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="196">
   <si>
     <t>uhc</t>
   </si>
@@ -588,6 +588,39 @@
   </si>
   <si>
     <t>espar</t>
+  </si>
+  <si>
+    <t>HE_meningitis_Campign</t>
+  </si>
+  <si>
+    <t>HE_meningitis_CampignSize</t>
+  </si>
+  <si>
+    <t>HE_meningitis_Routine</t>
+  </si>
+  <si>
+    <t>HE_cholera_Campign</t>
+  </si>
+  <si>
+    <t>HE_cholera_CampignSize</t>
+  </si>
+  <si>
+    <t>HE_yellowfever_Campign</t>
+  </si>
+  <si>
+    <t>HE_yellowfever_CampignSize</t>
+  </si>
+  <si>
+    <t>HE_yellowfever_Routine</t>
+  </si>
+  <si>
+    <t>HE_polio_Routine</t>
+  </si>
+  <si>
+    <t>HE_surviving_infants</t>
+  </si>
+  <si>
+    <t>HE_measles_Routine</t>
   </si>
 </sst>
 </file>
@@ -664,13 +697,6 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -740,6 +766,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -757,9 +790,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F75" totalsRowShown="0">
   <autoFilter ref="A1:F75" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
@@ -1034,7 +1067,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1096,7 +1129,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>162</v>
       </c>
@@ -1108,7 +1143,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>163</v>
       </c>
@@ -1176,7 +1213,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>167</v>
       </c>
@@ -1202,7 +1241,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>164</v>
       </c>
@@ -1214,7 +1255,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>165</v>
       </c>
@@ -1226,7 +1269,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>166</v>
       </c>
@@ -1280,7 +1325,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>169</v>
       </c>
@@ -1292,7 +1339,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>170</v>
       </c>
@@ -1538,7 +1587,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="B34" s="2" t="s">
         <v>168</v>
       </c>
@@ -1550,7 +1601,9 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
+      <c r="A35" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>160</v>
       </c>
@@ -1562,7 +1615,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
+      <c r="A36" s="6" t="s">
+        <v>192</v>
+      </c>
       <c r="B36" s="2" t="s">
         <v>161</v>
       </c>
@@ -2198,7 +2253,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D2:F75">
-    <cfRule type="containsText" dxfId="0" priority="135" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="3" priority="135" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2211,6 +2266,100 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2219,7 +2368,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2436,101 +2585,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2538,7 +2610,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2555,21 +2627,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add covariate column to indicator_df and add IHR and pneumo_mort covariates as rows
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E141AB-5793-AB40-A5F6-68AD6D032B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEAF2E8-FAB0-8A44-9EB1-E4F7C3E4D0E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="224">
   <si>
     <t>uhc</t>
   </si>
@@ -621,6 +621,90 @@
   </si>
   <si>
     <t>HE_measles_Routine</t>
+  </si>
+  <si>
+    <t>ihr01</t>
+  </si>
+  <si>
+    <t>ihr02</t>
+  </si>
+  <si>
+    <t>ihr03</t>
+  </si>
+  <si>
+    <t>ihr04</t>
+  </si>
+  <si>
+    <t>ihr05</t>
+  </si>
+  <si>
+    <t>ihr06</t>
+  </si>
+  <si>
+    <t>ihr07</t>
+  </si>
+  <si>
+    <t>ihr08</t>
+  </si>
+  <si>
+    <t>ihr09</t>
+  </si>
+  <si>
+    <t>ihr10</t>
+  </si>
+  <si>
+    <t>ihr11</t>
+  </si>
+  <si>
+    <t>ihr12</t>
+  </si>
+  <si>
+    <t>ihr13</t>
+  </si>
+  <si>
+    <t>IHR01</t>
+  </si>
+  <si>
+    <t>IHR02</t>
+  </si>
+  <si>
+    <t>IHR03</t>
+  </si>
+  <si>
+    <t>IHR04</t>
+  </si>
+  <si>
+    <t>IHR05</t>
+  </si>
+  <si>
+    <t>IHR06</t>
+  </si>
+  <si>
+    <t>IHR07</t>
+  </si>
+  <si>
+    <t>IHR08</t>
+  </si>
+  <si>
+    <t>IHR09</t>
+  </si>
+  <si>
+    <t>IHR10</t>
+  </si>
+  <si>
+    <t>IHR11</t>
+  </si>
+  <si>
+    <t>IHR12</t>
+  </si>
+  <si>
+    <t>IHR13</t>
+  </si>
+  <si>
+    <t>covariate</t>
+  </si>
+  <si>
+    <t>pneumo_mort</t>
   </si>
 </sst>
 </file>
@@ -695,7 +779,28 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -766,13 +871,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -787,15 +885,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:F75" totalsRowShown="0">
-  <autoFilter ref="A1:F75" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
-  <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:G89" totalsRowShown="0">
+  <autoFilter ref="A1:G89" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
+  <tableColumns count="7">
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
+    <tableColumn id="2" xr3:uid="{32F342AE-BE8D-4C4B-B2A9-150E44FF0BA1}" name="covariate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1064,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1094,7 +1193,7 @@
     <col min="25" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1113,8 +1212,11 @@
       <c r="F1" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1128,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>188</v>
       </c>
@@ -1142,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>189</v>
       </c>
@@ -1156,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1170,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1184,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1198,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1212,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>195</v>
       </c>
@@ -1226,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1240,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>187</v>
       </c>
@@ -1254,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>185</v>
       </c>
@@ -1268,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>186</v>
       </c>
@@ -1282,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1296,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1310,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>193</v>
       </c>
@@ -1338,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>194</v>
       </c>
@@ -1352,222 +1454,238 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="3"/>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="3"/>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="3"/>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" s="3"/>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="3"/>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="3"/>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="3"/>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D26" s="3"/>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" s="3"/>
+      <c r="G26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D28" s="3"/>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D29" s="3"/>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="3"/>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D31" s="3"/>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2">
         <v>1</v>
@@ -1575,12 +1693,15 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2">
         <v>1</v>
@@ -1588,13 +1709,15 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
         <v>1</v>
@@ -1602,27 +1725,31 @@
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="2"/>
+      <c r="A36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="3"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2">
         <v>1</v>
@@ -1630,12 +1757,15 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2">
         <v>1</v>
@@ -1643,236 +1773,222 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>103</v>
+        <v>181</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>61</v>
+        <v>20</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="D39" s="3"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>117</v>
+      <c r="A40" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="D40" s="3"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>118</v>
+      <c r="A41" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D41" s="3"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="2">
-        <v>1</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="3"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>30</v>
+      <c r="A43" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>31</v>
+      <c r="A44" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="2">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" s="6"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="2">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="A48" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" s="6"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="2">
-        <v>1</v>
-      </c>
-      <c r="F48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="A49" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" s="6"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="2">
-        <v>1</v>
-      </c>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>37</v>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>38</v>
+      <c r="A51" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2">
+        <v>1</v>
+      </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>101</v>
+      <c r="A52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D52" s="2">
         <v>1</v>
@@ -1881,14 +1997,14 @@
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>68</v>
+      <c r="A53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
@@ -1896,15 +2012,15 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>63</v>
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
@@ -1913,14 +2029,11 @@
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>42</v>
+      <c r="A55" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="D55" s="2">
         <v>1</v>
@@ -1928,129 +2041,129 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>66</v>
+        <v>30</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
-      <c r="E56" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>64</v>
+        <v>31</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
-      <c r="E57" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1</v>
+      </c>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>65</v>
+      <c r="A58" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1</v>
-      </c>
-      <c r="E58" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2">
+        <v>1</v>
+      </c>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1</v>
-      </c>
-      <c r="E59" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2">
+        <v>1</v>
+      </c>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>102</v>
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D60" s="2">
-        <v>1</v>
-      </c>
-      <c r="E60" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2">
+        <v>1</v>
+      </c>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1</v>
-      </c>
-      <c r="E61" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2">
+        <v>1</v>
+      </c>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>184</v>
+        <v>78</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2">
+        <v>1</v>
+      </c>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2">
@@ -2060,141 +2173,140 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2">
-        <v>1</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2">
-        <v>1</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>105</v>
+        <v>40</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2">
-        <v>1</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>106</v>
+        <v>41</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2">
-        <v>1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>107</v>
+        <v>43</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>108</v>
+        <v>44</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2">
-        <v>1</v>
-      </c>
+    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
@@ -2202,59 +2314,295 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2">
+        <v>1</v>
+      </c>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2">
+        <v>1</v>
+      </c>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2">
+        <v>1</v>
+      </c>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2">
+        <v>1</v>
+      </c>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2">
+        <v>1</v>
+      </c>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2">
+        <v>1</v>
+      </c>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2">
-        <v>1</v>
-      </c>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
+      <c r="D87" s="2"/>
+      <c r="E87" s="2">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2">
-        <v>1</v>
-      </c>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
+      <c r="D88" s="2"/>
+      <c r="E88" s="2">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C89" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2">
-        <v>1</v>
-      </c>
-      <c r="F75" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+      <c r="F89" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F75">
-    <cfRule type="containsText" dxfId="3" priority="135" operator="containsText" text="1">
+  <conditionalFormatting sqref="D2:F89">
+    <cfRule type="containsText" dxfId="2" priority="137" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19:G31">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",G19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G71">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",G71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2360,15 +2708,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2585,6 +2924,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
   <ds:schemaRefs>
@@ -2603,14 +2951,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2627,4 +2967,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add eSPAR sub-sub-components to HEP indicators
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEAF2E8-FAB0-8A44-9EB1-E4F7C3E4D0E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B298E878-8087-BD46-B51F-C7208B308751}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="242">
   <si>
     <t>uhc</t>
   </si>
@@ -705,6 +705,60 @@
   </si>
   <si>
     <t>pneumo_mort</t>
+  </si>
+  <si>
+    <t>espar01_01</t>
+  </si>
+  <si>
+    <t>espar01_02</t>
+  </si>
+  <si>
+    <t>espar01_03</t>
+  </si>
+  <si>
+    <t>espar02_01</t>
+  </si>
+  <si>
+    <t>espar02_02</t>
+  </si>
+  <si>
+    <t>espar05_01</t>
+  </si>
+  <si>
+    <t>espar05_02</t>
+  </si>
+  <si>
+    <t>espar05_03</t>
+  </si>
+  <si>
+    <t>espar06_01</t>
+  </si>
+  <si>
+    <t>espar06_02</t>
+  </si>
+  <si>
+    <t>espar08_01</t>
+  </si>
+  <si>
+    <t>espar08_02</t>
+  </si>
+  <si>
+    <t>espar08_03</t>
+  </si>
+  <si>
+    <t>espar09_01</t>
+  </si>
+  <si>
+    <t>espar09_02</t>
+  </si>
+  <si>
+    <t>espar09_03</t>
+  </si>
+  <si>
+    <t>espar11_01</t>
+  </si>
+  <si>
+    <t>espar11_02</t>
   </si>
 </sst>
 </file>
@@ -781,27 +835,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -871,6 +904,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -885,12 +939,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:G89" totalsRowShown="0">
-  <autoFilter ref="A1:G89" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:G107" totalsRowShown="0">
+  <autoFilter ref="A1:G107" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="7">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
@@ -1163,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1692,15 +1746,11 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="6"/>
       <c r="D33" s="3"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2">
@@ -1708,15 +1758,11 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C34" s="6"/>
       <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
@@ -1724,15 +1770,11 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C35" s="6"/>
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2">
@@ -1741,13 +1783,13 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="2"/>
@@ -1756,15 +1798,11 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" s="6"/>
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2">
@@ -1772,15 +1810,11 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C38" s="6"/>
       <c r="D38" s="3"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2">
@@ -1789,13 +1823,13 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="2"/>
@@ -1805,13 +1839,13 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
@@ -1821,13 +1855,13 @@
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
@@ -1836,15 +1870,11 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C42" s="6"/>
       <c r="D42" s="3"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2">
@@ -1852,15 +1882,11 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>156</v>
-      </c>
+      <c r="A43" s="2"/>
+      <c r="B43" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C43" s="6"/>
       <c r="D43" s="3"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2">
@@ -1868,15 +1894,11 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44" s="6"/>
       <c r="D44" s="3"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2">
@@ -1885,39 +1907,39 @@
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="2"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="3"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>168</v>
+      <c r="A47" s="2"/>
+      <c r="B47" s="5" t="s">
+        <v>233</v>
       </c>
       <c r="C47" s="6"/>
-      <c r="D47" s="2"/>
+      <c r="D47" s="3"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2">
         <v>1</v>
@@ -1925,357 +1947,318 @@
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="3"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="2"/>
+      <c r="A49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="3"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" s="2"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="3"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
+      <c r="A52" s="2"/>
+      <c r="B52" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="3"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>117</v>
+      <c r="A53" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D53" s="2">
-        <v>1</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="D53" s="3"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1</v>
-      </c>
+      <c r="A54" s="2"/>
+      <c r="B54" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="3"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
+      <c r="A55" s="2"/>
+      <c r="B55" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="3"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2">
-        <v>1</v>
-      </c>
-      <c r="F56" s="2"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>31</v>
+      <c r="A57" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="2">
-        <v>1</v>
-      </c>
-      <c r="F57" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2">
-        <v>1</v>
-      </c>
-      <c r="F58" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2">
-        <v>1</v>
-      </c>
-      <c r="F59" s="2"/>
+      <c r="A59" s="2"/>
+      <c r="B59" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2">
-        <v>1</v>
-      </c>
-      <c r="F60" s="2"/>
+      <c r="A60" s="2"/>
+      <c r="B60" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>35</v>
+      <c r="A61" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>77</v>
+        <v>173</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2">
-        <v>1</v>
-      </c>
-      <c r="F61" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>36</v>
+      <c r="A62" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>78</v>
+        <v>174</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2">
-        <v>1</v>
-      </c>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>37</v>
+        <v>157</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D63" s="2"/>
-      <c r="E63" s="2">
-        <v>1</v>
-      </c>
-      <c r="F63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>38</v>
+      <c r="A64" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" s="2">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D65" s="2">
-        <v>1</v>
-      </c>
+      <c r="F64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>40</v>
+      <c r="F65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="2"/>
       <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>41</v>
+      <c r="F66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
+        <v>192</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="2"/>
       <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>42</v>
+      <c r="F67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>66</v>
+      <c r="F68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2">
+        <v>1</v>
+      </c>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>44</v>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
@@ -2283,30 +2266,31 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C71" s="6"/>
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>65</v>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
@@ -2314,15 +2298,12 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
@@ -2330,65 +2311,65 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>102</v>
+        <v>30</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D74" s="2">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2">
+        <v>1</v>
+      </c>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>62</v>
+        <v>31</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="2">
+        <v>1</v>
+      </c>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>49</v>
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>184</v>
+        <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D76" s="2">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>50</v>
+        <v>111</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2">
+        <v>1</v>
+      </c>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2">
@@ -2396,15 +2377,15 @@
       </c>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>51</v>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2">
@@ -2412,15 +2393,15 @@
       </c>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2">
@@ -2428,15 +2409,15 @@
       </c>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2">
@@ -2444,15 +2425,15 @@
       </c>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2">
@@ -2460,79 +2441,79 @@
       </c>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2">
-        <v>1</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2">
-        <v>1</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>108</v>
+        <v>40</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2">
-        <v>1</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>82</v>
+        <v>41</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2">
-        <v>1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>67</v>
+        <v>42</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D86" s="2">
         <v>1</v>
@@ -2540,69 +2521,358 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2">
+        <v>1</v>
+      </c>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2">
+        <v>1</v>
+      </c>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2">
+        <v>1</v>
+      </c>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2">
+        <v>1</v>
+      </c>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2">
+        <v>1</v>
+      </c>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2">
+        <v>1</v>
+      </c>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2">
+        <v>1</v>
+      </c>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2">
+        <v>1</v>
+      </c>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D104" s="2">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2">
-        <v>1</v>
-      </c>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
+      <c r="D105" s="2"/>
+      <c r="E105" s="2">
+        <v>1</v>
+      </c>
+      <c r="F105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2">
-        <v>1</v>
-      </c>
-      <c r="F88" s="2"/>
-    </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
+      <c r="D106" s="2"/>
+      <c r="E106" s="2">
+        <v>1</v>
+      </c>
+      <c r="F106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C107" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2">
+        <v>1</v>
+      </c>
+      <c r="F107" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F89">
-    <cfRule type="containsText" dxfId="2" priority="137" operator="containsText" text="1">
+  <conditionalFormatting sqref="D2:F107">
+    <cfRule type="containsText" dxfId="5" priority="137" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",G19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G71">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",G71)))</formula>
+  <conditionalFormatting sqref="G89">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",G89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2614,100 +2884,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2924,7 +3100,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2933,24 +3109,101 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2969,10 +3222,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add routine numerators to indicator_df
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B298E878-8087-BD46-B51F-C7208B308751}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A352B92-DB04-7448-9CDD-5F4C0D048BD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$100</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="255">
   <si>
     <t>uhc</t>
   </si>
@@ -759,6 +759,45 @@
   </si>
   <si>
     <t>espar11_02</t>
+  </si>
+  <si>
+    <t>HE_measles_Routine_num</t>
+  </si>
+  <si>
+    <t>measles_routine_num</t>
+  </si>
+  <si>
+    <t>meningitis_routine_num</t>
+  </si>
+  <si>
+    <t>HE_meningitis_Routine_num</t>
+  </si>
+  <si>
+    <t>cholera_campaign_num</t>
+  </si>
+  <si>
+    <t>meningitis_campaign_num</t>
+  </si>
+  <si>
+    <t>HE_meningitis_Campign_num</t>
+  </si>
+  <si>
+    <t>polio_routine_num</t>
+  </si>
+  <si>
+    <t>HE_polio_Routine_num</t>
+  </si>
+  <si>
+    <t>HE_yellowfever_Campign_num</t>
+  </si>
+  <si>
+    <t>yellow_fever_campaign_num</t>
+  </si>
+  <si>
+    <t>HE_yellowfever_Routine_num</t>
+  </si>
+  <si>
+    <t>yellow_fever_routine_num</t>
   </si>
 </sst>
 </file>
@@ -833,7 +872,77 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -904,27 +1013,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -939,12 +1027,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:G107" totalsRowShown="0">
-  <autoFilter ref="A1:G107" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:G114" totalsRowShown="0">
+  <autoFilter ref="A1:G114" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="7">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="10"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
@@ -1217,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:F60"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1300,10 +1388,10 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>163</v>
+        <v>246</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
@@ -1313,11 +1401,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -1328,10 +1416,10 @@
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
@@ -1342,10 +1430,10 @@
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
@@ -1356,10 +1444,10 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
@@ -1369,11 +1457,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>167</v>
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
@@ -1383,11 +1471,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>93</v>
+      <c r="A10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
@@ -1397,11 +1485,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>187</v>
+      <c r="A11" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>164</v>
+        <v>243</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
@@ -1411,11 +1499,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>185</v>
+      <c r="A12" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -1426,10 +1514,10 @@
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
@@ -1440,10 +1528,10 @@
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>245</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>244</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
@@ -1453,11 +1541,11 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
+      <c r="A15" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -1468,10 +1556,10 @@
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>248</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>96</v>
+        <v>247</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -1482,10 +1570,10 @@
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>169</v>
+        <v>186</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
@@ -1496,10 +1584,10 @@
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>170</v>
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
@@ -1509,97 +1597,82 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>209</v>
-      </c>
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
         <v>1</v>
       </c>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>210</v>
-      </c>
+      <c r="A20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
         <v>1</v>
       </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="B21" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>211</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="C21" s="3"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>212</v>
-      </c>
+      <c r="A22" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>213</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
         <v>1</v>
       </c>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1613,10 +1686,10 @@
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1630,10 +1703,10 @@
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1647,10 +1720,10 @@
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1664,10 +1737,10 @@
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1681,10 +1754,10 @@
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1698,10 +1771,10 @@
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1715,10 +1788,10 @@
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1730,89 +1803,110 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D32" s="3"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="3"/>
+      <c r="B33" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="3"/>
+      <c r="B34" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="3"/>
+      <c r="B35" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D36" s="3"/>
+      <c r="G35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C37" s="6"/>
+      <c r="G36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="3"/>
@@ -1821,47 +1915,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>147</v>
-      </c>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C39" s="6"/>
       <c r="D39" s="3"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>148</v>
-      </c>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C40" s="6"/>
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
@@ -1869,10 +1955,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="3"/>
@@ -1881,10 +1967,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="3"/>
@@ -1893,27 +1979,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C44" s="6"/>
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="2"/>
@@ -1921,22 +2011,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="C46" s="6"/>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="D46" s="3"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="3"/>
@@ -1945,16 +2039,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>151</v>
-      </c>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C48" s="6"/>
       <c r="D48" s="3"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2">
@@ -1962,15 +2052,11 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="6"/>
       <c r="D49" s="3"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2">
@@ -1978,11 +2064,15 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C50" s="6"/>
+      <c r="A50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="D50" s="3"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2">
@@ -1992,7 +2082,7 @@
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="3"/>
@@ -2004,7 +2094,7 @@
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="3"/>
@@ -2015,13 +2105,13 @@
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="2"/>
@@ -2030,11 +2120,15 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C54" s="6"/>
+      <c r="A54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="D54" s="3"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2">
@@ -2044,7 +2138,7 @@
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="3"/>
@@ -2056,7 +2150,7 @@
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="3"/>
@@ -2066,15 +2160,11 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="A57" s="2"/>
+      <c r="B57" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="6"/>
       <c r="D57" s="3"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2">
@@ -2083,13 +2173,13 @@
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="2"/>
@@ -2100,7 +2190,7 @@
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="3"/>
@@ -2112,7 +2202,7 @@
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="3"/>
@@ -2122,15 +2212,11 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>156</v>
-      </c>
+      <c r="A61" s="2"/>
+      <c r="B61" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C61" s="6"/>
       <c r="D61" s="3"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2">
@@ -2139,13 +2225,13 @@
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="2"/>
@@ -2155,39 +2241,39 @@
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" s="3"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D64" s="2"/>
+      <c r="A64" s="2"/>
+      <c r="B64" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="3"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>168</v>
+      <c r="A65" s="2"/>
+      <c r="B65" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="C65" s="6"/>
-      <c r="D65" s="2"/>
+      <c r="D65" s="3"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2">
         <v>1</v>
@@ -2195,27 +2281,31 @@
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" s="3"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="2"/>
+      <c r="A67" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="3"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2">
         <v>1</v>
@@ -2223,10 +2313,10 @@
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -2236,124 +2326,109 @@
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="D69" s="2"/>
-      <c r="E69" s="2">
-        <v>1</v>
-      </c>
-      <c r="F69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>58</v>
+        <v>191</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D70" s="2">
-        <v>1</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="2"/>
       <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+      <c r="F70" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>117</v>
+      <c r="A71" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="2"/>
       <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
+      <c r="F71" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1</v>
-      </c>
+      <c r="A72" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="2"/>
       <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>29</v>
+      <c r="A73" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" s="2">
-        <v>1</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="2"/>
       <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
+      <c r="F73" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="A74" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" s="6"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="2">
-        <v>1</v>
-      </c>
-      <c r="F74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>31</v>
+      <c r="A75" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="2">
-        <v>1</v>
-      </c>
-      <c r="F75" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2">
@@ -2363,77 +2438,74 @@
     </row>
     <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2">
-        <v>1</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>34</v>
+      <c r="A78" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2">
-        <v>1</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>35</v>
+      <c r="A79" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2">
-        <v>1</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
-        <v>36</v>
+      <c r="A80" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2">
-        <v>1</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2">
@@ -2443,140 +2515,143 @@
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="2">
+        <v>1</v>
+      </c>
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
-        <v>39</v>
+      <c r="A83" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-      <c r="E83" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2">
+        <v>1</v>
+      </c>
       <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>68</v>
+      <c r="A84" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D84" s="2">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2">
+        <v>1</v>
+      </c>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>63</v>
+    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D85" s="2">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
       <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D86" s="2">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2">
+        <v>1</v>
+      </c>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>66</v>
+        <v>36</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D87" s="2">
-        <v>1</v>
-      </c>
-      <c r="E87" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2">
+        <v>1</v>
+      </c>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>64</v>
+        <v>37</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D88" s="2">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2">
+        <v>1</v>
+      </c>
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C89" s="6"/>
+      <c r="A89" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
-      <c r="G89" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D90" s="2">
         <v>1</v>
@@ -2585,14 +2660,14 @@
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>72</v>
+      <c r="A91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D91" s="2">
         <v>1</v>
@@ -2602,13 +2677,13 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D92" s="2">
         <v>1</v>
@@ -2616,15 +2691,15 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D93" s="2">
         <v>1</v>
@@ -2634,143 +2709,142 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>184</v>
+        <v>43</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D94" s="2">
         <v>1</v>
       </c>
       <c r="E94" s="2"/>
-      <c r="F94" s="2">
-        <v>1</v>
-      </c>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>80</v>
+        <v>44</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2"/>
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2">
-        <v>1</v>
-      </c>
+      <c r="A96" s="2"/>
+      <c r="B96" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C96" s="6"/>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2"/>
       <c r="F96" s="2"/>
+      <c r="G96" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>81</v>
+        <v>45</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2">
-        <v>1</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2"/>
       <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
-        <v>52</v>
+      <c r="A98" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2">
-        <v>1</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>106</v>
+        <v>47</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2">
-        <v>1</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>104</v>
+        <v>48</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2">
-        <v>1</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D100" s="2">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>107</v>
+        <v>184</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2">
-        <v>1</v>
-      </c>
-      <c r="F101" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="D101" s="2">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2">
@@ -2780,13 +2854,13 @@
     </row>
     <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2">
@@ -2796,29 +2870,29 @@
     </row>
     <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D104" s="2">
-        <v>1</v>
-      </c>
-      <c r="E104" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2">
+        <v>1</v>
+      </c>
       <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2">
@@ -2828,13 +2902,13 @@
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2">
@@ -2844,13 +2918,13 @@
     </row>
     <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>158</v>
+        <v>104</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2">
@@ -2858,21 +2932,168 @@
       </c>
       <c r="F107" s="2"/>
     </row>
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2">
+        <v>1</v>
+      </c>
+      <c r="F108" s="2"/>
+    </row>
+    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2">
+        <v>1</v>
+      </c>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2">
+        <v>1</v>
+      </c>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D111" s="2">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+    </row>
+    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2">
+        <v>1</v>
+      </c>
+      <c r="F112" s="2"/>
+    </row>
+    <row r="113" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2">
+        <v>1</v>
+      </c>
+      <c r="F113" s="2"/>
+    </row>
+    <row r="114" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2">
+        <v>1</v>
+      </c>
+      <c r="F114" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F107">
-    <cfRule type="containsText" dxfId="5" priority="137" operator="containsText" text="1">
+  <conditionalFormatting sqref="D2:F2 D11:F12 D14:F15 D4:F9 D17:F20 D22:F70 D72:F72 D74:F114">
+    <cfRule type="containsText" dxfId="9" priority="144" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:G31">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",G19)))</formula>
+  <conditionalFormatting sqref="G24:G36">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",G24)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G89">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",G89)))</formula>
+  <conditionalFormatting sqref="G96">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",G96)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:F10">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:F13">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:F3">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:F16">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:F21">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71:F71">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D73:F73">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2884,6 +3105,109 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -3100,110 +3424,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3220,29 +3466,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust HEP functions to work with long format data
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562F4428-205C-B64E-AE21-D9C6A22AED51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D1AC2E-7428-A54F-97CC-424D406C82F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators!$A$1:$F$80</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="231">
   <si>
     <t>uhc</t>
   </si>
@@ -693,6 +693,39 @@
   </si>
   <si>
     <t>hpop_healthier_minus</t>
+  </si>
+  <si>
+    <t>measles_campaign</t>
+  </si>
+  <si>
+    <t>measles_campaign_num</t>
+  </si>
+  <si>
+    <t>measles_campaign_denom</t>
+  </si>
+  <si>
+    <t>ebola</t>
+  </si>
+  <si>
+    <t>ebola_campaign</t>
+  </si>
+  <si>
+    <t>ebola_campaign_num</t>
+  </si>
+  <si>
+    <t>ebola_campaign_denom</t>
+  </si>
+  <si>
+    <t>covid</t>
+  </si>
+  <si>
+    <t>covid_campaign</t>
+  </si>
+  <si>
+    <t>covid_campaign_num</t>
+  </si>
+  <si>
+    <t>covid_campaign_denom</t>
   </si>
 </sst>
 </file>
@@ -768,7 +801,7 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -798,25 +831,23 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -953,6 +984,29 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
@@ -1023,17 +1077,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:H88" totalsRowShown="0">
-  <autoFilter ref="A1:H88" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:H99" totalsRowShown="0">
+  <autoFilter ref="A1:H99" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="8">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="25"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
     <tableColumn id="2" xr3:uid="{32F342AE-BE8D-4C4B-B2A9-150E44FF0BA1}" name="covariate"/>
-    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1302,10 +1356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86:H88"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,11 +1561,9 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>93</v>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -1522,11 +1574,9 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>164</v>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
@@ -1537,11 +1587,9 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>200</v>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
@@ -1552,11 +1600,9 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>165</v>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -1567,11 +1613,9 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>203</v>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -1582,11 +1626,9 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>166</v>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
@@ -1597,11 +1639,9 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>94</v>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
@@ -1612,11 +1652,9 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>95</v>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
@@ -1627,11 +1665,9 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>96</v>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
@@ -1642,11 +1678,9 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>193</v>
-      </c>
+      <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="2"/>
@@ -1657,11 +1691,9 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>205</v>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="2"/>
@@ -1673,10 +1705,10 @@
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>170</v>
+        <v>9</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="2"/>
@@ -1687,16 +1719,14 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>13</v>
+      <c r="A24" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2">
         <v>1</v>
@@ -1705,15 +1735,13 @@
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2">
         <v>1</v>
@@ -1721,16 +1749,14 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>15</v>
+      <c r="A26" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>165</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
         <v>1</v>
@@ -1739,15 +1765,13 @@
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>203</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2">
         <v>1</v>
@@ -1755,16 +1779,14 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>17</v>
+      <c r="A28" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>166</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <v>1</v>
@@ -1773,15 +1795,13 @@
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2">
         <v>1</v>
@@ -1790,15 +1810,13 @@
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2">
         <v>1</v>
@@ -1807,15 +1825,13 @@
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2">
         <v>1</v>
@@ -1823,16 +1839,14 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" s="3"/>
+      <c r="A32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2">
         <v>1</v>
@@ -1841,15 +1855,13 @@
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2">
         <v>1</v>
@@ -1858,15 +1870,13 @@
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="3"/>
+        <v>194</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
         <v>1</v>
@@ -1875,13 +1885,13 @@
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
@@ -1892,13 +1902,13 @@
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="2"/>
@@ -1909,12 +1919,15 @@
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>177</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2">
         <v>1</v>
@@ -1923,12 +1936,15 @@
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="2"/>
+        <v>178</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="3"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2">
         <v>1</v>
@@ -1937,13 +1953,15 @@
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="3"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2">
         <v>1</v>
@@ -1952,13 +1970,15 @@
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>207</v>
+        <v>18</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="3"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2">
         <v>1</v>
@@ -1967,13 +1987,15 @@
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" s="3"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2">
         <v>1</v>
@@ -1981,14 +2003,16 @@
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>209</v>
+      <c r="A42" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" s="3"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2">
         <v>1</v>
@@ -1996,14 +2020,16 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="2"/>
+      <c r="A43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="3"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2">
         <v>1</v>
@@ -2012,12 +2038,15 @@
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="3"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2">
         <v>1</v>
@@ -2026,199 +2055,181 @@
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>103</v>
+        <v>172</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2">
+        <v>1</v>
+      </c>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="D46" s="3"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="F46" s="2">
+        <v>1</v>
+      </c>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>117</v>
+      <c r="A47" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="D47" s="3"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>118</v>
+      <c r="A48" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="F48" s="2">
+        <v>1</v>
+      </c>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="F49" s="2">
+        <v>1</v>
+      </c>
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="A50" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="6"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2">
+        <v>1</v>
+      </c>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>31</v>
+      <c r="A51" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="2">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2">
+        <v>1</v>
+      </c>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="6"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="2">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2">
+        <v>1</v>
+      </c>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>33</v>
+      <c r="A53" s="6" t="s">
+        <v>209</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>113</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="C53" s="6"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="2">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A54" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" s="6"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="2">
-        <v>1</v>
-      </c>
-      <c r="F54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>35</v>
+      <c r="A55" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D55" s="2"/>
-      <c r="E55" s="2">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>36</v>
+      <c r="A56" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2">
@@ -2227,32 +2238,32 @@
       <c r="F56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>79</v>
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2">
-        <v>1</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>38</v>
+      <c r="A58" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
@@ -2262,14 +2273,14 @@
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>39</v>
+      <c r="A59" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
@@ -2279,14 +2290,11 @@
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>125</v>
+      <c r="A60" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D60" s="2">
         <v>1</v>
@@ -2295,150 +2303,153 @@
       <c r="F60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>63</v>
+        <v>30</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1</v>
-      </c>
-      <c r="E61" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2">
+        <v>1</v>
+      </c>
       <c r="F61" s="2"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1</v>
+      </c>
       <c r="F62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>66</v>
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D63" s="2">
-        <v>1</v>
-      </c>
-      <c r="E63" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2">
+        <v>1</v>
+      </c>
       <c r="F63" s="2"/>
       <c r="H63" s="2"/>
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>64</v>
+      <c r="A64" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D64" s="2">
-        <v>1</v>
-      </c>
-      <c r="E64" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2">
+        <v>1</v>
+      </c>
       <c r="F64" s="2"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="2">
-        <v>1</v>
-      </c>
-      <c r="E65" s="2"/>
+      <c r="A65" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2">
+        <v>1</v>
+      </c>
       <c r="F65" s="2"/>
-      <c r="G65" s="2">
-        <v>1</v>
-      </c>
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>65</v>
+        <v>35</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2">
+        <v>1</v>
+      </c>
       <c r="F66" s="2"/>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>46</v>
+      <c r="A67" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2">
+        <v>1</v>
+      </c>
       <c r="F67" s="2"/>
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>102</v>
+        <v>37</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
-      <c r="E68" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2">
+        <v>1</v>
+      </c>
       <c r="F68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
@@ -2447,187 +2458,184 @@
       <c r="F69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
       </c>
       <c r="E70" s="2"/>
-      <c r="F70" s="2">
-        <v>1</v>
-      </c>
+      <c r="F70" s="2"/>
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>80</v>
+        <v>40</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2">
-        <v>1</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>87</v>
+        <v>41</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2">
-        <v>1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2">
-        <v>1</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>105</v>
+        <v>43</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="H74" s="2"/>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>106</v>
+        <v>44</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2">
-        <v>1</v>
-      </c>
+      <c r="A76" s="2"/>
+      <c r="B76" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2"/>
       <c r="F76" s="2"/>
+      <c r="G76" s="2">
+        <v>1</v>
+      </c>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>107</v>
+        <v>45</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2">
-        <v>1</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>53</v>
+      <c r="A78" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2">
-        <v>1</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>82</v>
+        <v>47</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2">
-        <v>1</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D80" s="2">
         <v>1</v>
@@ -2636,32 +2644,34 @@
       <c r="F80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2">
+        <v>1</v>
+      </c>
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2">
@@ -2672,13 +2682,13 @@
     </row>
     <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>158</v>
+        <v>87</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2">
@@ -2687,182 +2697,379 @@
       <c r="F83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
+    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2">
+        <v>1</v>
+      </c>
+      <c r="F84" s="2"/>
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2"/>
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2">
+        <v>1</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2"/>
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2"/>
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+      <c r="F89" s="2"/>
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2"/>
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="H91" s="2"/>
+    </row>
+    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2">
+        <v>1</v>
+      </c>
+      <c r="F92" s="2"/>
+      <c r="H92" s="2"/>
+    </row>
+    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2">
+        <v>1</v>
+      </c>
+      <c r="F93" s="2"/>
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2">
+        <v>1</v>
+      </c>
+      <c r="F94" s="2"/>
+      <c r="H94" s="2"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B95" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C84" s="6"/>
-      <c r="D84" s="2">
-        <v>1</v>
-      </c>
-      <c r="H84" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
+      <c r="C95" s="6"/>
+      <c r="D95" s="2">
+        <v>1</v>
+      </c>
+      <c r="H95" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B96" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C85" s="6"/>
-      <c r="D85" s="2">
-        <v>1</v>
-      </c>
-      <c r="H85" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="7" t="s">
+      <c r="C96" s="6"/>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+      <c r="H96" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B97" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C86" s="6"/>
-      <c r="E86" s="2">
-        <v>1</v>
-      </c>
-      <c r="H86" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7" t="s">
+      <c r="C97" s="6"/>
+      <c r="E97" s="2">
+        <v>1</v>
+      </c>
+      <c r="H97" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C87" s="6"/>
-      <c r="E87" s="2">
-        <v>1</v>
-      </c>
-      <c r="H87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="7"/>
-      <c r="B88" s="7" t="s">
+      <c r="C98" s="6"/>
+      <c r="E98" s="2">
+        <v>1</v>
+      </c>
+      <c r="H98" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="7"/>
+      <c r="B99" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="C88" s="6"/>
-      <c r="E88" s="2">
-        <v>1</v>
-      </c>
-      <c r="H88" s="2">
+      <c r="C99" s="6"/>
+      <c r="E99" s="2">
+        <v>1</v>
+      </c>
+      <c r="H99" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F2 D11:F12 D14:F15 D4:F9 D17:F20 D41:F41 D43:F83 D22:F39">
-    <cfRule type="containsText" dxfId="21" priority="156" operator="containsText" text="1">
+  <conditionalFormatting sqref="D2:F2 D25:F26 D4:F9 D28:F31 D52:F52 D54:F94 D33:F50 D11:F11 D21:F23 H11:H23 D15:E20">
+    <cfRule type="containsText" dxfId="23" priority="159" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G65">
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",G65)))</formula>
+  <conditionalFormatting sqref="G76">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",G76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:F13">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D13)))</formula>
+  <conditionalFormatting sqref="D24:F24">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F3">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:F16">
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D16)))</formula>
+  <conditionalFormatting sqref="D27:F27">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21:F21">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D21)))</formula>
+  <conditionalFormatting sqref="D32:F32">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40:F40">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D40)))</formula>
+  <conditionalFormatting sqref="D51:F51">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42:F42">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D42)))</formula>
+  <conditionalFormatting sqref="D53:F53">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2 H11:H12 H14:H15 H4:H9 H17:H20 H41 H43:H83 H22:H39">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="1">
+  <conditionalFormatting sqref="H2 H25:H26 H4:H9 H28:H31 H52 H54:H94 H33:H50">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",H13)))</formula>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",H16)))</formula>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",H21)))</formula>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",H40)))</formula>
+  <conditionalFormatting sqref="H51">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",H42)))</formula>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H53)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D84:D85">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D84)))</formula>
+  <conditionalFormatting sqref="D95:D96">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D95)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H84:H85">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",H84)))</formula>
+  <conditionalFormatting sqref="H95:H96">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H95)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H86:H88">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",H86)))</formula>
+  <conditionalFormatting sqref="H97:H99">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H97)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E86:E88">
+  <conditionalFormatting sqref="E97:E99">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",E97)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:F14">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:F20">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",E86)))</formula>
+      <formula>NOT(ISERROR(SEARCH("1",F15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2874,6 +3081,109 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -3090,110 +3400,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3210,29 +3442,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated indicator_df.xlsx with GHO code for measles_routine (WHS8_110).
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D1AC2E-7428-A54F-97CC-424D406C82F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AFEDB7-4ACA-4A70-8BFE-2E0D8C6B0B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="232">
   <si>
     <t>uhc</t>
   </si>
@@ -726,6 +726,9 @@
   </si>
   <si>
     <t>covid_campaign_denom</t>
+  </si>
+  <si>
+    <t>WHS8_110</t>
   </si>
 </sst>
 </file>
@@ -801,14 +804,7 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <fill>
         <patternFill>
@@ -1080,14 +1076,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:H99" totalsRowShown="0">
   <autoFilter ref="A1:H99" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="8">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="26"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="24"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
     <tableColumn id="2" xr3:uid="{32F342AE-BE8D-4C4B-B2A9-150E44FF0BA1}" name="covariate"/>
-    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1359,32 +1355,32 @@
   <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="21.1640625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="21.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="29.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="45.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="45.44140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="31.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" style="1" customWidth="1"/>
     <col min="17" max="17" width="192.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="178.5" style="1" customWidth="1"/>
-    <col min="19" max="19" width="23.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="178.44140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.109375" style="1" customWidth="1"/>
     <col min="20" max="21" width="35" style="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="1" customWidth="1"/>
     <col min="23" max="23" width="22.6640625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.83203125" style="1"/>
+    <col min="24" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1410,7 +1406,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1425,7 +1421,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>188</v>
       </c>
@@ -1440,7 +1436,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>188</v>
       </c>
@@ -1455,7 +1451,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>189</v>
       </c>
@@ -1470,7 +1466,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1485,7 +1481,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1500,7 +1496,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1515,14 +1511,14 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
@@ -1530,14 +1526,16 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>231</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2">
@@ -1545,7 +1543,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>198</v>
       </c>
@@ -1560,7 +1558,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>220</v>
@@ -1573,7 +1571,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>221</v>
@@ -1586,7 +1584,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>222</v>
@@ -1599,7 +1597,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>223</v>
@@ -1612,7 +1610,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>224</v>
@@ -1625,7 +1623,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>225</v>
@@ -1638,7 +1636,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>226</v>
@@ -1651,7 +1649,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>227</v>
@@ -1664,7 +1662,7 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>228</v>
@@ -1677,7 +1675,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>229</v>
@@ -1690,7 +1688,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>230</v>
@@ -1703,7 +1701,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1718,7 +1716,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>187</v>
       </c>
@@ -1733,7 +1731,7 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>201</v>
       </c>
@@ -1748,7 +1746,7 @@
       </c>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>185</v>
       </c>
@@ -1763,7 +1761,7 @@
       </c>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>204</v>
       </c>
@@ -1778,7 +1776,7 @@
       </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>186</v>
       </c>
@@ -1793,7 +1791,7 @@
       </c>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -1808,7 +1806,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -1823,7 +1821,7 @@
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
@@ -1838,7 +1836,7 @@
       </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>193</v>
       </c>
@@ -1853,7 +1851,7 @@
       </c>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>206</v>
       </c>
@@ -1868,7 +1866,7 @@
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>194</v>
       </c>
@@ -1883,7 +1881,7 @@
       </c>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
@@ -1900,7 +1898,7 @@
       </c>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1917,7 +1915,7 @@
       </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -1934,7 +1932,7 @@
       </c>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
@@ -1951,7 +1949,7 @@
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>17</v>
       </c>
@@ -1968,7 +1966,7 @@
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
@@ -1985,7 +1983,7 @@
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -2002,7 +2000,7 @@
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
@@ -2019,7 +2017,7 @@
       </c>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
@@ -2036,7 +2034,7 @@
       </c>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
@@ -2053,7 +2051,7 @@
       </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>23</v>
       </c>
@@ -2070,7 +2068,7 @@
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>24</v>
       </c>
@@ -2087,7 +2085,7 @@
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>25</v>
       </c>
@@ -2104,7 +2102,7 @@
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>26</v>
       </c>
@@ -2118,7 +2116,7 @@
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>27</v>
       </c>
@@ -2132,7 +2130,7 @@
       </c>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>191</v>
       </c>
@@ -2147,7 +2145,7 @@
       </c>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>207</v>
       </c>
@@ -2162,7 +2160,7 @@
       </c>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>190</v>
       </c>
@@ -2177,7 +2175,7 @@
       </c>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>209</v>
       </c>
@@ -2192,7 +2190,7 @@
       </c>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>192</v>
       </c>
@@ -2207,7 +2205,7 @@
       </c>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>28</v>
       </c>
@@ -2221,7 +2219,7 @@
       </c>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>47</v>
       </c>
@@ -2238,7 +2236,7 @@
       <c r="F56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -2255,7 +2253,7 @@
       <c r="F57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
@@ -2272,7 +2270,7 @@
       <c r="F58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>118</v>
       </c>
@@ -2289,7 +2287,7 @@
       <c r="F59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>29</v>
       </c>
@@ -2303,7 +2301,7 @@
       <c r="F60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>30</v>
       </c>
@@ -2320,7 +2318,7 @@
       <c r="F61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>31</v>
       </c>
@@ -2339,7 +2337,7 @@
       <c r="F62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>32</v>
       </c>
@@ -2356,7 +2354,7 @@
       <c r="F63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>33</v>
       </c>
@@ -2373,7 +2371,7 @@
       <c r="F64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>34</v>
       </c>
@@ -2390,7 +2388,7 @@
       <c r="F65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -2407,7 +2405,7 @@
       <c r="F66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>36</v>
       </c>
@@ -2424,7 +2422,7 @@
       <c r="F67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>37</v>
       </c>
@@ -2441,7 +2439,7 @@
       <c r="F68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>38</v>
       </c>
@@ -2458,7 +2456,7 @@
       <c r="F69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>39</v>
       </c>
@@ -2475,7 +2473,7 @@
       <c r="F70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>40</v>
       </c>
@@ -2492,7 +2490,7 @@
       <c r="F71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>41</v>
       </c>
@@ -2509,7 +2507,7 @@
       <c r="F72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>42</v>
       </c>
@@ -2526,7 +2524,7 @@
       <c r="F73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>43</v>
       </c>
@@ -2543,7 +2541,7 @@
       <c r="F74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>44</v>
       </c>
@@ -2560,7 +2558,7 @@
       <c r="F75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
         <v>197</v>
@@ -2576,7 +2574,7 @@
       </c>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>45</v>
       </c>
@@ -2593,7 +2591,7 @@
       <c r="F77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>46</v>
       </c>
@@ -2610,7 +2608,7 @@
       <c r="F78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>47</v>
       </c>
@@ -2627,7 +2625,7 @@
       <c r="F79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>48</v>
       </c>
@@ -2644,7 +2642,7 @@
       <c r="F80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>49</v>
       </c>
@@ -2663,7 +2661,7 @@
       </c>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>50</v>
       </c>
@@ -2680,7 +2678,7 @@
       <c r="F82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -2697,7 +2695,7 @@
       <c r="F83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>52</v>
       </c>
@@ -2714,7 +2712,7 @@
       <c r="F84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>52</v>
       </c>
@@ -2731,7 +2729,7 @@
       <c r="F85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>52</v>
       </c>
@@ -2748,7 +2746,7 @@
       <c r="F86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>53</v>
       </c>
@@ -2765,7 +2763,7 @@
       <c r="F87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>53</v>
       </c>
@@ -2782,7 +2780,7 @@
       <c r="F88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>53</v>
       </c>
@@ -2799,7 +2797,7 @@
       <c r="F89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>54</v>
       </c>
@@ -2816,7 +2814,7 @@
       <c r="F90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>55</v>
       </c>
@@ -2833,7 +2831,7 @@
       <c r="F91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>56</v>
       </c>
@@ -2850,7 +2848,7 @@
       <c r="F92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>57</v>
       </c>
@@ -2867,7 +2865,7 @@
       <c r="F93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>59</v>
       </c>
@@ -2884,7 +2882,7 @@
       <c r="F94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>212</v>
       </c>
@@ -2899,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>214</v>
       </c>
@@ -2914,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
         <v>216</v>
       </c>
@@ -2929,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7" t="s">
         <v>218</v>
@@ -2942,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="7"/>
       <c r="B99" s="7" t="s">
         <v>219</v>
@@ -2958,112 +2956,112 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D2:F2 D25:F26 D4:F9 D28:F31 D52:F52 D54:F94 D33:F50 D11:F11 D21:F23 H11:H23 D15:E20">
-    <cfRule type="containsText" dxfId="23" priority="159" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="22" priority="159" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",G76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:F24">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F3">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:F27">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:F32">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:F51">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53:F53">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2 H25:H26 H4:H9 H28:H31 H52 H54:H94 H33:H50">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D95:D96">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95:H96">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97:H99">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97:E99">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",E97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:F14">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D12)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added GHO code for polio_routine(WHS4_544) to indicator_df
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AFEDB7-4ACA-4A70-8BFE-2E0D8C6B0B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFC967-9096-48A3-B97F-6834E6DB3A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="233">
   <si>
     <t>uhc</t>
   </si>
@@ -729,6 +729,9 @@
   </si>
   <si>
     <t>WHS8_110</t>
+  </si>
+  <si>
+    <t>WHS4_544</t>
   </si>
 </sst>
 </file>
@@ -805,6 +808,99 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -966,99 +1062,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1076,14 +1079,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:H99" totalsRowShown="0">
   <autoFilter ref="A1:H99" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="8">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="25"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
     <tableColumn id="2" xr3:uid="{32F342AE-BE8D-4C4B-B2A9-150E44FF0BA1}" name="covariate"/>
-    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1354,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1843,7 +1846,9 @@
       <c r="B32" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>232</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2">
@@ -2956,117 +2961,117 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D2:F2 D25:F26 D4:F9 D28:F31 D52:F52 D54:F94 D33:F50 D11:F11 D21:F23 H11:H23 D15:E20">
-    <cfRule type="containsText" dxfId="22" priority="159" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="26" priority="159" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76">
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",G76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:F24">
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F3">
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:F27">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:F32">
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:F51">
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53:F53">
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2 H25:H26 H4:H9 H28:H31 H52 H54:H94 H33:H50">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D95:D96">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95:H96">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97:H99">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97:E99">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",E97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:F14">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F20">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",F15)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3079,109 +3084,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -3398,32 +3300,110 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3440,4 +3420,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update indicator_df with dbl_cntd variables
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WHO\billionaiRe\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFC967-9096-48A3-B97F-6834E6DB3A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49F8084-FE8A-CA4A-B47A-F90BBC4D3E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="236">
   <si>
     <t>uhc</t>
   </si>
@@ -732,6 +732,15 @@
   </si>
   <si>
     <t>WHS4_544</t>
+  </si>
+  <si>
+    <t>hpop_healthier_dbl_cntd</t>
+  </si>
+  <si>
+    <t>hpop_healthier_plus_dbl_cntd</t>
+  </si>
+  <si>
+    <t>hpop_healthier_minus_dbl_cntd</t>
   </si>
 </sst>
 </file>
@@ -807,97 +816,11 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="29">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1062,6 +985,106 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1079,14 +1102,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{783B6F54-F67A-6342-BA49-C3BF890CB76C}" name="Table1" displayName="Table1" ref="A1:H99" totalsRowShown="0">
   <autoFilter ref="A1:H99" xr:uid="{780BA2EC-B0C0-C940-BDAE-0AE14886CFC5}"/>
   <tableColumns count="8">
-    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{7DFA423E-8684-974A-98B5-EA0B00422A08}" name="dashboard_id" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{CBB65CF6-3ED2-664B-9889-9F562D1497A4}" name="analysis_code" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{3D4F0965-9F06-0149-883C-B2F7B6622A73}" name="gho_code" dataDxfId="26"/>
     <tableColumn id="10" xr3:uid="{FA2DED0D-DB40-B945-A6E8-15C35D79B548}" name="uhc"/>
     <tableColumn id="103" xr3:uid="{57C07A1E-73A9-4347-8790-620D9F865229}" name="hpop"/>
     <tableColumn id="11" xr3:uid="{00C0B48C-3F1F-6946-8E5A-1F94E497C7FB}" name="hep"/>
     <tableColumn id="2" xr3:uid="{32F342AE-BE8D-4C4B-B2A9-150E44FF0BA1}" name="covariate"/>
-    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{4FB9FBFA-F8CE-FE43-8AF4-B3FC217671DE}" name="calculated" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1355,35 +1378,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB31011-80E6-5F4A-A086-38DA0F50CFFC}">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="21.109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="21.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28.109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="45.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="45.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="31.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="192.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="178.44140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="23.109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="178.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.1640625" style="1" customWidth="1"/>
     <col min="20" max="21" width="35" style="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="1" customWidth="1"/>
     <col min="23" max="23" width="22.6640625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.77734375" style="1"/>
+    <col min="24" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1409,7 +1432,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1447,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>188</v>
       </c>
@@ -1439,7 +1462,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>188</v>
       </c>
@@ -1454,7 +1477,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>189</v>
       </c>
@@ -1469,7 +1492,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1484,7 +1507,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1499,7 +1522,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1537,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1529,7 +1552,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>195</v>
       </c>
@@ -1546,7 +1569,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>198</v>
       </c>
@@ -1561,7 +1584,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>220</v>
@@ -1574,7 +1597,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>221</v>
@@ -1587,7 +1610,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>222</v>
@@ -1600,7 +1623,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>223</v>
@@ -1613,7 +1636,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>224</v>
@@ -1626,7 +1649,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>225</v>
@@ -1639,7 +1662,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>226</v>
@@ -1652,7 +1675,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>227</v>
@@ -1665,7 +1688,7 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>228</v>
@@ -1678,7 +1701,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>229</v>
@@ -1691,7 +1714,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>230</v>
@@ -1704,7 +1727,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1719,7 +1742,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>187</v>
       </c>
@@ -1734,7 +1757,7 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>201</v>
       </c>
@@ -1749,7 +1772,7 @@
       </c>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>185</v>
       </c>
@@ -1764,7 +1787,7 @@
       </c>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>204</v>
       </c>
@@ -1779,7 +1802,7 @@
       </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>186</v>
       </c>
@@ -1794,7 +1817,7 @@
       </c>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -1809,7 +1832,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -1824,7 +1847,7 @@
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
@@ -1839,7 +1862,7 @@
       </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>193</v>
       </c>
@@ -1856,7 +1879,7 @@
       </c>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>206</v>
       </c>
@@ -1871,7 +1894,7 @@
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>194</v>
       </c>
@@ -1886,7 +1909,7 @@
       </c>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
@@ -1903,7 +1926,7 @@
       </c>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1920,7 +1943,7 @@
       </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -1937,7 +1960,7 @@
       </c>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
@@ -1954,7 +1977,7 @@
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>17</v>
       </c>
@@ -1971,7 +1994,7 @@
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
@@ -1988,7 +2011,7 @@
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -2005,7 +2028,7 @@
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
@@ -2022,7 +2045,7 @@
       </c>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
@@ -2039,7 +2062,7 @@
       </c>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
@@ -2056,7 +2079,7 @@
       </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>23</v>
       </c>
@@ -2073,7 +2096,7 @@
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>24</v>
       </c>
@@ -2090,7 +2113,7 @@
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>25</v>
       </c>
@@ -2107,7 +2130,7 @@
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>26</v>
       </c>
@@ -2121,7 +2144,7 @@
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>27</v>
       </c>
@@ -2135,7 +2158,7 @@
       </c>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>191</v>
       </c>
@@ -2150,7 +2173,7 @@
       </c>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>207</v>
       </c>
@@ -2165,7 +2188,7 @@
       </c>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>190</v>
       </c>
@@ -2180,7 +2203,7 @@
       </c>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>209</v>
       </c>
@@ -2195,7 +2218,7 @@
       </c>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>192</v>
       </c>
@@ -2210,7 +2233,7 @@
       </c>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>28</v>
       </c>
@@ -2224,7 +2247,7 @@
       </c>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>47</v>
       </c>
@@ -2241,7 +2264,7 @@
       <c r="F56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -2258,7 +2281,7 @@
       <c r="F57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
@@ -2275,7 +2298,7 @@
       <c r="F58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>118</v>
       </c>
@@ -2292,7 +2315,7 @@
       <c r="F59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>29</v>
       </c>
@@ -2306,7 +2329,7 @@
       <c r="F60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>30</v>
       </c>
@@ -2323,7 +2346,7 @@
       <c r="F61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>31</v>
       </c>
@@ -2342,7 +2365,7 @@
       <c r="F62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>32</v>
       </c>
@@ -2359,7 +2382,7 @@
       <c r="F63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>33</v>
       </c>
@@ -2376,7 +2399,7 @@
       <c r="F64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>34</v>
       </c>
@@ -2393,7 +2416,7 @@
       <c r="F65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -2410,7 +2433,7 @@
       <c r="F66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>36</v>
       </c>
@@ -2427,7 +2450,7 @@
       <c r="F67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>37</v>
       </c>
@@ -2444,7 +2467,7 @@
       <c r="F68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>38</v>
       </c>
@@ -2461,7 +2484,7 @@
       <c r="F69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>39</v>
       </c>
@@ -2478,7 +2501,7 @@
       <c r="F70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>40</v>
       </c>
@@ -2495,7 +2518,7 @@
       <c r="F71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>41</v>
       </c>
@@ -2512,7 +2535,7 @@
       <c r="F72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>42</v>
       </c>
@@ -2529,7 +2552,7 @@
       <c r="F73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>43</v>
       </c>
@@ -2546,7 +2569,7 @@
       <c r="F74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>44</v>
       </c>
@@ -2563,7 +2586,7 @@
       <c r="F75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
         <v>197</v>
@@ -2579,7 +2602,7 @@
       </c>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>45</v>
       </c>
@@ -2596,7 +2619,7 @@
       <c r="F77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>46</v>
       </c>
@@ -2613,7 +2636,7 @@
       <c r="F78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>47</v>
       </c>
@@ -2630,7 +2653,7 @@
       <c r="F79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>48</v>
       </c>
@@ -2647,7 +2670,7 @@
       <c r="F80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>49</v>
       </c>
@@ -2666,7 +2689,7 @@
       </c>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>50</v>
       </c>
@@ -2683,7 +2706,7 @@
       <c r="F82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -2700,7 +2723,7 @@
       <c r="F83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>52</v>
       </c>
@@ -2717,7 +2740,7 @@
       <c r="F84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>52</v>
       </c>
@@ -2734,7 +2757,7 @@
       <c r="F85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>52</v>
       </c>
@@ -2751,7 +2774,7 @@
       <c r="F86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>53</v>
       </c>
@@ -2768,7 +2791,7 @@
       <c r="F87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>53</v>
       </c>
@@ -2785,7 +2808,7 @@
       <c r="F88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>53</v>
       </c>
@@ -2802,7 +2825,7 @@
       <c r="F89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>54</v>
       </c>
@@ -2819,7 +2842,7 @@
       <c r="F90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>55</v>
       </c>
@@ -2836,7 +2859,7 @@
       <c r="F91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>56</v>
       </c>
@@ -2853,7 +2876,7 @@
       <c r="F92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>57</v>
       </c>
@@ -2870,7 +2893,7 @@
       <c r="F93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>59</v>
       </c>
@@ -2887,7 +2910,7 @@
       <c r="F94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>212</v>
       </c>
@@ -2902,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>214</v>
       </c>
@@ -2917,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>216</v>
       </c>
@@ -2932,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
       <c r="B98" s="7" t="s">
         <v>218</v>
@@ -2945,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="B99" s="7" t="s">
         <v>219</v>
@@ -2958,121 +2981,172 @@
         <v>1</v>
       </c>
     </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C100" s="6"/>
+      <c r="E100" s="2">
+        <v>1</v>
+      </c>
+      <c r="H100" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="7"/>
+      <c r="B101" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C101" s="6"/>
+      <c r="E101" s="2">
+        <v>1</v>
+      </c>
+      <c r="H101" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="7"/>
+      <c r="B102" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="E102" s="2">
+        <v>1</v>
+      </c>
+      <c r="H102" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D2:F2 D25:F26 D4:F9 D28:F31 D52:F52 D54:F94 D33:F50 D11:F11 D21:F23 H11:H23 D15:E20">
-    <cfRule type="containsText" dxfId="26" priority="159" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="24" priority="163" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",G76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:F24">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F3">
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:F27">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:F32">
-    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:F51">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53:F53">
-    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2 H25:H26 H4:H9 H28:H31 H52 H54:H94 H33:H50">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D95:D96">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95:H96">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97:H99">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97:E99">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",E97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:F14">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F20">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",F15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H100:H102">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",H100)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E100:E102">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",E100)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3084,6 +3158,109 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
+      <UserInfo>
+        <DisplayName>ROBSON, Alice</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SLOUP, Shalene</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BRILLANTES, Zoe</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BAHL, Navneet Kumar</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIONDI, Nelly</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>HO, Jessica Chi Ying</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIRKBY, Katherine</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PRASAD, Amit</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BIEHL, Molly</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ASMA, Samira</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ATIA, Sondos</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CHATTERJI, Somnath</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CALDWELL, Seth</DisplayName>
+        <AccountId>141</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MSEMBURI, William</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CAO, Bochen</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -3300,110 +3477,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bd879b36-96f5-4c4e-979a-9eb1cd712529">
-      <UserInfo>
-        <DisplayName>ROBSON, Alice</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SLOUP, Shalene</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BRILLANTES, Zoe</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BAHL, Navneet Kumar</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIONDI, Nelly</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>HO, Jessica Chi Ying</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIRKBY, Katherine</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PRASAD, Amit</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BIEHL, Molly</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BOUCHER, Philippe Jean-Pierre (fleap)</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ASMA, Samira</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ATIA, Sondos</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CHATTERJI, Somnath</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CALDWELL, Seth</DisplayName>
-        <AccountId>141</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUTENRIETH, Christine Sonja</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MSEMBURI, William</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CAO, Bochen</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069016DC-5E59-4E7E-9F07-D21FB652AB0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3420,29 +3519,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6182ABEC-DC80-4655-8F77-FAB0303A94D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7E5D4-7DD9-4F16-9E20-8C7B6DEACC62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify indicator_df to add extra information to indicators. (#29)
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\documents\WHO\seth_billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406C9BBF-CC22-4964-B938-974A5795BFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AE1629-F5D2-4D12-84D0-6C2DDBB396F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="558">
   <si>
     <t>dashboard_id</t>
   </si>
@@ -2096,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5172,6 +5172,12 @@
       <c r="N77" t="s">
         <v>550</v>
       </c>
+      <c r="P77">
+        <v>65</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -5915,6 +5921,12 @@
       </c>
       <c r="O92" t="s">
         <v>551</v>
+      </c>
+      <c r="P92">
+        <v>66</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
removing '$' in espar10
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WHO\billionaiRe\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CB91B4-E837-46E5-A296-F5B537338C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6693E9E6-59D4-4F88-8AE0-7E1493FEE32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="518">
   <si>
     <t>dashboard_id</t>
   </si>
@@ -1004,9 +1004,6 @@
   </si>
   <si>
     <t>Risk communication</t>
-  </si>
-  <si>
-    <t>$Risk communication</t>
   </si>
   <si>
     <t>HE_points</t>
@@ -1965,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,7 +2030,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B2" t="s">
         <v>262</v>
@@ -2089,10 +2086,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B3" t="s">
         <v>468</v>
-      </c>
-      <c r="B3" t="s">
-        <v>469</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -2112,7 +2109,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D4" t="s">
         <v>52</v>
@@ -2133,11 +2130,11 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
+        <v>373</v>
+      </c>
+      <c r="K4" t="s">
         <v>374</v>
       </c>
-      <c r="K4" t="s">
-        <v>375</v>
-      </c>
       <c r="L4" t="s">
         <v>24</v>
       </c>
@@ -2145,27 +2142,27 @@
         <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q4">
         <v>58</v>
       </c>
       <c r="R4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B5" t="s">
         <v>470</v>
-      </c>
-      <c r="B5" t="s">
-        <v>471</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -2188,10 +2185,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D6" t="s">
         <v>52</v>
@@ -2214,7 +2211,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -2234,7 +2231,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -2254,7 +2251,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -2274,7 +2271,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -2294,10 +2291,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>378</v>
+      </c>
+      <c r="B11" t="s">
         <v>379</v>
-      </c>
-      <c r="B11" t="s">
-        <v>380</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -2318,39 +2315,39 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
+        <v>380</v>
+      </c>
+      <c r="K11" t="s">
         <v>381</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>382</v>
       </c>
-      <c r="L11" t="s">
-        <v>383</v>
-      </c>
       <c r="M11" t="s">
         <v>24</v>
       </c>
       <c r="N11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="O11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="P11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="Q11">
         <v>60</v>
       </c>
       <c r="R11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -2371,36 +2368,36 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
+        <v>393</v>
+      </c>
+      <c r="K12" t="s">
         <v>394</v>
       </c>
-      <c r="K12" t="s">
-        <v>395</v>
-      </c>
       <c r="L12" t="s">
+        <v>382</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" t="s">
+        <v>394</v>
+      </c>
+      <c r="O12" t="s">
+        <v>394</v>
+      </c>
+      <c r="P12" t="s">
         <v>383</v>
-      </c>
-      <c r="M12" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" t="s">
-        <v>395</v>
-      </c>
-      <c r="O12" t="s">
-        <v>395</v>
-      </c>
-      <c r="P12" t="s">
-        <v>384</v>
       </c>
       <c r="Q12">
         <v>63</v>
       </c>
       <c r="R12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -2420,7 +2417,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -2440,7 +2437,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -2460,7 +2457,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
@@ -2557,27 +2554,27 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
+        <v>400</v>
+      </c>
+      <c r="L18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" t="s">
         <v>401</v>
       </c>
-      <c r="L18" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18" t="s">
-        <v>24</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>402</v>
       </c>
-      <c r="O18" t="s">
-        <v>403</v>
-      </c>
       <c r="P18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -2598,27 +2595,27 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
+        <v>404</v>
+      </c>
+      <c r="L19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" t="s">
         <v>405</v>
       </c>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" t="s">
-        <v>24</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>406</v>
       </c>
-      <c r="O19" t="s">
-        <v>407</v>
-      </c>
       <c r="P19" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -2639,22 +2636,22 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
+        <v>408</v>
+      </c>
+      <c r="L20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" t="s">
         <v>409</v>
       </c>
-      <c r="L20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" t="s">
-        <v>24</v>
-      </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>410</v>
       </c>
-      <c r="O20" t="s">
-        <v>411</v>
-      </c>
       <c r="P20" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -2715,7 +2712,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -2736,27 +2733,27 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
+        <v>412</v>
+      </c>
+      <c r="L22" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" t="s">
         <v>413</v>
       </c>
-      <c r="L22" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" t="s">
-        <v>24</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>414</v>
       </c>
-      <c r="O22" t="s">
-        <v>415</v>
-      </c>
       <c r="P22" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C23" t="s">
         <v>283</v>
@@ -2780,22 +2777,22 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
+        <v>416</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
         <v>417</v>
       </c>
-      <c r="L23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" t="s">
-        <v>24</v>
-      </c>
-      <c r="N23" t="s">
-        <v>418</v>
-      </c>
       <c r="O23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="P23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -2968,7 +2965,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -2989,27 +2986,27 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
+        <v>419</v>
+      </c>
+      <c r="L27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N27" t="s">
         <v>420</v>
       </c>
-      <c r="L27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27" t="s">
-        <v>24</v>
-      </c>
-      <c r="N27" t="s">
-        <v>421</v>
-      </c>
       <c r="O27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
@@ -3030,27 +3027,27 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
+        <v>422</v>
+      </c>
+      <c r="L28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" t="s">
         <v>423</v>
       </c>
-      <c r="L28" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" t="s">
-        <v>24</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>424</v>
       </c>
-      <c r="O28" t="s">
-        <v>425</v>
-      </c>
       <c r="P28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D29" t="s">
         <v>21</v>
@@ -3071,22 +3068,22 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
+        <v>426</v>
+      </c>
+      <c r="L29" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" t="s">
         <v>427</v>
       </c>
-      <c r="L29" t="s">
-        <v>24</v>
-      </c>
-      <c r="M29" t="s">
-        <v>24</v>
-      </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>428</v>
       </c>
-      <c r="O29" t="s">
-        <v>429</v>
-      </c>
       <c r="P29" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -3147,7 +3144,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
@@ -3168,27 +3165,27 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
+        <v>430</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
+        <v>24</v>
+      </c>
+      <c r="N31" t="s">
         <v>431</v>
       </c>
-      <c r="L31" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" t="s">
-        <v>24</v>
-      </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>432</v>
       </c>
-      <c r="O31" t="s">
-        <v>433</v>
-      </c>
       <c r="P31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
@@ -3209,22 +3206,22 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
+        <v>434</v>
+      </c>
+      <c r="L32" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" t="s">
         <v>435</v>
       </c>
-      <c r="L32" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" t="s">
-        <v>24</v>
-      </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>436</v>
       </c>
-      <c r="O32" t="s">
-        <v>437</v>
-      </c>
       <c r="P32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
@@ -3341,7 +3338,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D35" t="s">
         <v>21</v>
@@ -3362,27 +3359,27 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
+        <v>438</v>
+      </c>
+      <c r="L35" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" t="s">
         <v>439</v>
       </c>
-      <c r="L35" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" t="s">
-        <v>24</v>
-      </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>440</v>
       </c>
-      <c r="O35" t="s">
-        <v>441</v>
-      </c>
       <c r="P35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D36" t="s">
         <v>21</v>
@@ -3403,22 +3400,22 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
+        <v>442</v>
+      </c>
+      <c r="L36" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" t="s">
+        <v>24</v>
+      </c>
+      <c r="N36" t="s">
         <v>443</v>
       </c>
-      <c r="L36" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" t="s">
-        <v>24</v>
-      </c>
-      <c r="N36" t="s">
-        <v>444</v>
-      </c>
       <c r="O36" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P36" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
@@ -3426,7 +3423,7 @@
         <v>313</v>
       </c>
       <c r="B37" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D37" t="s">
         <v>21</v>
@@ -3447,22 +3444,22 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
+        <v>445</v>
+      </c>
+      <c r="L37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N37" t="s">
         <v>446</v>
       </c>
-      <c r="L37" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" t="s">
-        <v>24</v>
-      </c>
-      <c r="N37" t="s">
-        <v>447</v>
-      </c>
       <c r="O37" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="P37" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
@@ -3523,7 +3520,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D39" t="s">
         <v>21</v>
@@ -3544,27 +3541,27 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
+        <v>448</v>
+      </c>
+      <c r="L39" t="s">
+        <v>24</v>
+      </c>
+      <c r="M39" t="s">
+        <v>24</v>
+      </c>
+      <c r="N39" t="s">
         <v>449</v>
       </c>
-      <c r="L39" t="s">
-        <v>24</v>
-      </c>
-      <c r="M39" t="s">
-        <v>24</v>
-      </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>450</v>
       </c>
-      <c r="O39" t="s">
-        <v>451</v>
-      </c>
       <c r="P39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D40" t="s">
         <v>21</v>
@@ -3585,27 +3582,27 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
+        <v>452</v>
+      </c>
+      <c r="L40" t="s">
+        <v>24</v>
+      </c>
+      <c r="M40" t="s">
+        <v>24</v>
+      </c>
+      <c r="N40" t="s">
         <v>453</v>
       </c>
-      <c r="L40" t="s">
-        <v>24</v>
-      </c>
-      <c r="M40" t="s">
-        <v>24</v>
-      </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>454</v>
       </c>
-      <c r="O40" t="s">
-        <v>455</v>
-      </c>
       <c r="P40" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D41" t="s">
         <v>21</v>
@@ -3626,22 +3623,22 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
+        <v>456</v>
+      </c>
+      <c r="L41" t="s">
+        <v>24</v>
+      </c>
+      <c r="M41" t="s">
+        <v>24</v>
+      </c>
+      <c r="N41" t="s">
         <v>457</v>
       </c>
-      <c r="L41" t="s">
-        <v>24</v>
-      </c>
-      <c r="M41" t="s">
-        <v>24</v>
-      </c>
-      <c r="N41" t="s">
+      <c r="O41" t="s">
         <v>458</v>
       </c>
-      <c r="O41" t="s">
-        <v>459</v>
-      </c>
       <c r="P41" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
@@ -3685,7 +3682,7 @@
         <v>24</v>
       </c>
       <c r="N42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O42" t="s">
         <v>327</v>
@@ -3702,13 +3699,13 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>328</v>
+      </c>
+      <c r="B43" t="s">
         <v>329</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>330</v>
-      </c>
-      <c r="C43" t="s">
-        <v>331</v>
       </c>
       <c r="D43" t="s">
         <v>21</v>
@@ -3729,11 +3726,11 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
+        <v>331</v>
+      </c>
+      <c r="K43" t="s">
         <v>332</v>
       </c>
-      <c r="K43" t="s">
-        <v>333</v>
-      </c>
       <c r="L43" t="s">
         <v>24</v>
       </c>
@@ -3741,13 +3738,13 @@
         <v>24</v>
       </c>
       <c r="N43" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O43" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P43" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q43">
         <v>49</v>
@@ -3758,7 +3755,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D44" t="s">
         <v>21</v>
@@ -3779,27 +3776,27 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
+        <v>460</v>
+      </c>
+      <c r="L44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M44" t="s">
+        <v>24</v>
+      </c>
+      <c r="N44" t="s">
         <v>461</v>
       </c>
-      <c r="L44" t="s">
-        <v>24</v>
-      </c>
-      <c r="M44" t="s">
-        <v>24</v>
-      </c>
-      <c r="N44" t="s">
+      <c r="O44" t="s">
         <v>462</v>
       </c>
-      <c r="O44" t="s">
-        <v>463</v>
-      </c>
       <c r="P44" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D45" t="s">
         <v>21</v>
@@ -3820,33 +3817,33 @@
         <v>0</v>
       </c>
       <c r="J45" t="s">
+        <v>464</v>
+      </c>
+      <c r="L45" t="s">
+        <v>24</v>
+      </c>
+      <c r="M45" t="s">
+        <v>24</v>
+      </c>
+      <c r="N45" t="s">
         <v>465</v>
       </c>
-      <c r="L45" t="s">
-        <v>24</v>
-      </c>
-      <c r="M45" t="s">
-        <v>24</v>
-      </c>
-      <c r="N45" t="s">
+      <c r="O45" t="s">
         <v>466</v>
       </c>
-      <c r="O45" t="s">
-        <v>467</v>
-      </c>
       <c r="P45" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>333</v>
+      </c>
+      <c r="B46" t="s">
         <v>334</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>335</v>
-      </c>
-      <c r="C46" t="s">
-        <v>336</v>
       </c>
       <c r="D46" t="s">
         <v>21</v>
@@ -3867,11 +3864,11 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
+        <v>336</v>
+      </c>
+      <c r="K46" t="s">
         <v>337</v>
       </c>
-      <c r="K46" t="s">
-        <v>338</v>
-      </c>
       <c r="L46" t="s">
         <v>24</v>
       </c>
@@ -3879,13 +3876,13 @@
         <v>24</v>
       </c>
       <c r="N46" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O46" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P46" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q46">
         <v>50</v>
@@ -3896,13 +3893,13 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>338</v>
+      </c>
+      <c r="B47" t="s">
         <v>339</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>340</v>
-      </c>
-      <c r="C47" t="s">
-        <v>341</v>
       </c>
       <c r="D47" t="s">
         <v>21</v>
@@ -3923,11 +3920,11 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
+        <v>341</v>
+      </c>
+      <c r="K47" t="s">
         <v>342</v>
       </c>
-      <c r="K47" t="s">
-        <v>343</v>
-      </c>
       <c r="L47" t="s">
         <v>24</v>
       </c>
@@ -3935,13 +3932,13 @@
         <v>24</v>
       </c>
       <c r="N47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P47" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q47">
         <v>51</v>
@@ -3952,46 +3949,46 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>395</v>
+      </c>
+      <c r="B48" t="s">
         <v>396</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
         <v>397</v>
       </c>
-      <c r="E48" t="b">
-        <v>0</v>
-      </c>
-      <c r="F48" t="b">
-        <v>0</v>
-      </c>
-      <c r="G48" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" t="b">
-        <v>1</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
+        <v>397</v>
+      </c>
+      <c r="L48" t="s">
+        <v>24</v>
+      </c>
+      <c r="M48" t="s">
+        <v>24</v>
+      </c>
+      <c r="N48" t="s">
         <v>398</v>
       </c>
-      <c r="K48" t="s">
+      <c r="O48" t="s">
         <v>398</v>
       </c>
-      <c r="L48" t="s">
-        <v>24</v>
-      </c>
-      <c r="M48" t="s">
-        <v>24</v>
-      </c>
-      <c r="N48" t="s">
-        <v>399</v>
-      </c>
-      <c r="O48" t="s">
-        <v>399</v>
-      </c>
       <c r="P48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q48">
         <v>64</v>
@@ -4002,10 +3999,10 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>480</v>
+      </c>
+      <c r="B49" t="s">
         <v>481</v>
-      </c>
-      <c r="B49" t="s">
-        <v>482</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -4025,7 +4022,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -4045,7 +4042,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -4065,7 +4062,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -4085,7 +4082,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -4105,13 +4102,13 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>349</v>
+      </c>
+      <c r="B54" t="s">
         <v>350</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>351</v>
-      </c>
-      <c r="C54" t="s">
-        <v>352</v>
       </c>
       <c r="D54" t="s">
         <v>21</v>
@@ -4132,36 +4129,36 @@
         <v>0</v>
       </c>
       <c r="J54" t="s">
+        <v>352</v>
+      </c>
+      <c r="K54" t="s">
         <v>353</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
+        <v>24</v>
+      </c>
+      <c r="M54" t="s">
+        <v>24</v>
+      </c>
+      <c r="N54" t="s">
         <v>354</v>
       </c>
-      <c r="L54" t="s">
-        <v>24</v>
-      </c>
-      <c r="M54" t="s">
-        <v>24</v>
-      </c>
-      <c r="N54" t="s">
-        <v>355</v>
-      </c>
       <c r="O54" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q54">
         <v>53</v>
       </c>
       <c r="R54" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -4181,7 +4178,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -4201,7 +4198,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D57" t="s">
         <v>52</v>
@@ -4222,11 +4219,11 @@
         <v>0</v>
       </c>
       <c r="J57" t="s">
+        <v>369</v>
+      </c>
+      <c r="K57" t="s">
         <v>370</v>
       </c>
-      <c r="K57" t="s">
-        <v>371</v>
-      </c>
       <c r="L57" t="s">
         <v>24</v>
       </c>
@@ -4234,27 +4231,27 @@
         <v>24</v>
       </c>
       <c r="N57" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O57" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="P57" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q57">
         <v>57</v>
       </c>
       <c r="R57" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>488</v>
+      </c>
+      <c r="B58" t="s">
         <v>489</v>
-      </c>
-      <c r="B58" t="s">
-        <v>490</v>
       </c>
       <c r="D58" t="s">
         <v>52</v>
@@ -4277,10 +4274,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D59" t="s">
         <v>52</v>
@@ -4303,10 +4300,10 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>363</v>
+      </c>
+      <c r="B60" t="s">
         <v>364</v>
-      </c>
-      <c r="B60" t="s">
-        <v>365</v>
       </c>
       <c r="D60" t="s">
         <v>21</v>
@@ -4327,11 +4324,11 @@
         <v>0</v>
       </c>
       <c r="J60" t="s">
+        <v>365</v>
+      </c>
+      <c r="K60" t="s">
         <v>366</v>
       </c>
-      <c r="K60" t="s">
-        <v>367</v>
-      </c>
       <c r="L60" t="s">
         <v>24</v>
       </c>
@@ -4339,24 +4336,24 @@
         <v>24</v>
       </c>
       <c r="N60" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O60" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P60" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q60">
         <v>56</v>
       </c>
       <c r="R60" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -4376,10 +4373,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>384</v>
+      </c>
+      <c r="B62" t="s">
         <v>385</v>
-      </c>
-      <c r="B62" t="s">
-        <v>386</v>
       </c>
       <c r="D62" t="s">
         <v>21</v>
@@ -4400,36 +4397,36 @@
         <v>0</v>
       </c>
       <c r="J62" t="s">
+        <v>386</v>
+      </c>
+      <c r="K62" t="s">
         <v>387</v>
       </c>
-      <c r="K62" t="s">
-        <v>388</v>
-      </c>
       <c r="L62" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M62" t="s">
         <v>24</v>
       </c>
       <c r="N62" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O62" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P62" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q62">
         <v>61</v>
       </c>
       <c r="R62" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -4449,13 +4446,13 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>343</v>
+      </c>
+      <c r="B64" t="s">
         <v>344</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>345</v>
-      </c>
-      <c r="C64" t="s">
-        <v>346</v>
       </c>
       <c r="D64" t="s">
         <v>21</v>
@@ -4476,11 +4473,11 @@
         <v>0</v>
       </c>
       <c r="J64" t="s">
+        <v>346</v>
+      </c>
+      <c r="K64" t="s">
         <v>347</v>
       </c>
-      <c r="K64" t="s">
-        <v>348</v>
-      </c>
       <c r="L64" t="s">
         <v>24</v>
       </c>
@@ -4488,24 +4485,24 @@
         <v>24</v>
       </c>
       <c r="N64" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O64" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P64" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q64">
         <v>52</v>
       </c>
       <c r="R64" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -4525,32 +4522,32 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>375</v>
+      </c>
+      <c r="B66" t="s">
+        <v>348</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" t="s">
         <v>376</v>
       </c>
-      <c r="B66" t="s">
-        <v>349</v>
-      </c>
-      <c r="E66" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" t="b">
-        <v>0</v>
-      </c>
-      <c r="G66" t="b">
-        <v>1</v>
-      </c>
-      <c r="H66" t="b">
-        <v>0</v>
-      </c>
-      <c r="I66" t="b">
-        <v>1</v>
-      </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>377</v>
       </c>
-      <c r="K66" t="s">
-        <v>378</v>
-      </c>
       <c r="L66" t="s">
         <v>24</v>
       </c>
@@ -4558,27 +4555,27 @@
         <v>24</v>
       </c>
       <c r="N66" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O66" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P66" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q66">
         <v>59</v>
       </c>
       <c r="R66" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>388</v>
+      </c>
+      <c r="B67" t="s">
         <v>389</v>
-      </c>
-      <c r="B67" t="s">
-        <v>390</v>
       </c>
       <c r="D67" t="s">
         <v>21</v>
@@ -4599,39 +4596,39 @@
         <v>0</v>
       </c>
       <c r="J67" t="s">
+        <v>390</v>
+      </c>
+      <c r="K67" t="s">
         <v>391</v>
       </c>
-      <c r="K67" t="s">
-        <v>392</v>
-      </c>
       <c r="L67" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M67" t="s">
         <v>24</v>
       </c>
       <c r="N67" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O67" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="P67" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q67">
         <v>62</v>
       </c>
       <c r="R67" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>494</v>
+      </c>
+      <c r="B68" t="s">
         <v>495</v>
-      </c>
-      <c r="B68" t="s">
-        <v>496</v>
       </c>
       <c r="D68" t="s">
         <v>52</v>
@@ -4654,7 +4651,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -4674,7 +4671,7 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D70" t="s">
         <v>52</v>
@@ -4695,11 +4692,11 @@
         <v>0</v>
       </c>
       <c r="J70" t="s">
+        <v>361</v>
+      </c>
+      <c r="K70" t="s">
         <v>362</v>
       </c>
-      <c r="K70" t="s">
-        <v>363</v>
-      </c>
       <c r="L70" t="s">
         <v>24</v>
       </c>
@@ -4707,27 +4704,27 @@
         <v>24</v>
       </c>
       <c r="N70" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="O70" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P70" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q70">
         <v>55</v>
       </c>
       <c r="R70" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>497</v>
+      </c>
+      <c r="B71" t="s">
         <v>498</v>
-      </c>
-      <c r="B71" t="s">
-        <v>499</v>
       </c>
       <c r="D71" t="s">
         <v>52</v>
@@ -4750,10 +4747,10 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B72" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D72" t="s">
         <v>52</v>
@@ -4776,10 +4773,10 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>355</v>
+      </c>
+      <c r="B73" t="s">
         <v>356</v>
-      </c>
-      <c r="B73" t="s">
-        <v>357</v>
       </c>
       <c r="D73" t="s">
         <v>21</v>
@@ -4800,11 +4797,11 @@
         <v>0</v>
       </c>
       <c r="J73" t="s">
+        <v>357</v>
+      </c>
+      <c r="K73" t="s">
         <v>358</v>
       </c>
-      <c r="K73" t="s">
-        <v>359</v>
-      </c>
       <c r="L73" t="s">
         <v>24</v>
       </c>
@@ -4812,24 +4809,24 @@
         <v>24</v>
       </c>
       <c r="N73" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="O73" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P73" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q73">
         <v>54</v>
       </c>
       <c r="R73" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
@@ -4961,10 +4958,10 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B77" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E77" t="b">
         <v>1</v>
@@ -5264,7 +5261,7 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B83" t="s">
         <v>158</v>
@@ -5597,7 +5594,7 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D89" t="s">
         <v>21</v>
@@ -5732,10 +5729,10 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B92" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E92" t="b">
         <v>1</v>
@@ -6147,10 +6144,10 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B100" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E100" t="b">
         <v>0</v>
@@ -6170,10 +6167,10 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B101" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E101" t="b">
         <v>0</v>
@@ -6193,10 +6190,10 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B102" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
@@ -6216,7 +6213,7 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E103" t="b">
         <v>0</v>
@@ -6236,10 +6233,10 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B104" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -6259,7 +6256,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
adding missing orders for UHC calculated
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406C9BBF-CC22-4964-B938-974A5795BFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D032DB-C416-4BA8-87CC-E85D50947675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2094,10 +2094,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,7 +2216,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>467</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>372</v>
       </c>
@@ -2285,7 +2286,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>469</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>371</v>
       </c>
@@ -2337,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>472</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>473</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>474</v>
       </c>
@@ -2397,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>475</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>392</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>476</v>
       </c>
@@ -2537,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>477</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>478</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>479</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>274</v>
       </c>
@@ -2650,7 +2651,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>399</v>
       </c>
@@ -2688,7 +2689,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>403</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>407</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>280</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>411</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>415</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>286</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>292</v>
       </c>
@@ -3002,7 +3003,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>297</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>418</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>421</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>425</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>302</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>429</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>433</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>307</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -3404,7 +3405,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>437</v>
       </c>
@@ -3442,7 +3443,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>441</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>312</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>317</v>
       </c>
@@ -3574,7 +3575,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>447</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>451</v>
       </c>
@@ -3650,7 +3651,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>455</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>322</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>328</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>459</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>463</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>333</v>
       </c>
@@ -3923,7 +3924,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>338</v>
       </c>
@@ -3976,7 +3977,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>395</v>
       </c>
@@ -4023,7 +4024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>480</v>
       </c>
@@ -4046,7 +4047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>482</v>
       </c>
@@ -4078,7 +4079,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>483</v>
       </c>
@@ -4110,7 +4111,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>484</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>485</v>
       </c>
@@ -4174,7 +4175,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>349</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>486</v>
       </c>
@@ -4259,7 +4260,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>487</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>368</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>488</v>
       </c>
@@ -4376,7 +4377,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>367</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>363</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>491</v>
       </c>
@@ -4496,7 +4497,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>384</v>
       </c>
@@ -4546,7 +4547,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>492</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>343</v>
       </c>
@@ -4631,7 +4632,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>493</v>
       </c>
@@ -4663,7 +4664,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>375</v>
       </c>
@@ -4710,7 +4711,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>388</v>
       </c>
@@ -4760,7 +4761,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>494</v>
       </c>
@@ -4798,7 +4799,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>496</v>
       </c>
@@ -4830,7 +4831,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>360</v>
       </c>
@@ -4877,7 +4878,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>497</v>
       </c>
@@ -4915,7 +4916,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>359</v>
       </c>
@@ -4953,7 +4954,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>355</v>
       </c>
@@ -5003,7 +5004,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>500</v>
       </c>
@@ -5172,6 +5173,9 @@
       <c r="N77" t="s">
         <v>550</v>
       </c>
+      <c r="P77">
+        <v>65</v>
+      </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -5916,6 +5920,9 @@
       <c r="O92" t="s">
         <v>551</v>
       </c>
+      <c r="P92">
+        <v>66</v>
+      </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
@@ -5970,7 +5977,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>143</v>
       </c>
@@ -6023,7 +6030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>121</v>
       </c>
@@ -6076,7 +6083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -6129,7 +6136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>63</v>
       </c>
@@ -6182,7 +6189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>41</v>
       </c>
@@ -6235,7 +6242,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -6288,7 +6295,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>514</v>
       </c>
@@ -6317,7 +6324,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>515</v>
       </c>
@@ -6346,7 +6353,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>516</v>
       </c>
@@ -6375,7 +6382,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>504</v>
       </c>
@@ -6401,7 +6408,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>517</v>
       </c>
@@ -6430,7 +6437,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>506</v>
       </c>
@@ -6456,7 +6463,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -6509,7 +6516,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>110</v>
       </c>
@@ -6559,7 +6566,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>106</v>
       </c>
@@ -6609,7 +6616,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>137</v>
       </c>
@@ -6662,7 +6669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>56</v>
       </c>
@@ -6715,7 +6722,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>34</v>
       </c>
@@ -6768,7 +6775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>129</v>
       </c>
@@ -6821,7 +6828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -6874,7 +6881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -6927,7 +6934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>70</v>
       </c>
@@ -6980,7 +6987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>150</v>
       </c>
@@ -7033,7 +7040,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -7086,7 +7093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>85</v>
       </c>
@@ -7139,7 +7146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>96</v>
       </c>
@@ -7189,7 +7196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>92</v>
       </c>
@@ -7240,7 +7247,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q120" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q120" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q120">
     <sortCondition descending="1" ref="G2:G120"/>
     <sortCondition descending="1" ref="E2:E120"/>

</xml_diff>

<commit_message>
Fixed to names for campaign indicators.
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\documents\WHO\seth_billionaiRe\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AE1629-F5D2-4D12-84D0-6C2DDBB396F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16D089E-B839-48BE-8959-82C601A9C9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="568">
   <si>
     <t>dashboard_id</t>
   </si>
@@ -1708,6 +1708,36 @@
   </si>
   <si>
     <t>Overall HPOP Population healthier (with double counting)</t>
+  </si>
+  <si>
+    <t>Cholera - Campaign target population (denominator)</t>
+  </si>
+  <si>
+    <t>Cholera - Campaign reached population (numerator)</t>
+  </si>
+  <si>
+    <t>Cholera Campaign denominator</t>
+  </si>
+  <si>
+    <t>Cholera Campaign numerator</t>
+  </si>
+  <si>
+    <t>Measles Campaign denominator</t>
+  </si>
+  <si>
+    <t>Measles Campaign numerator</t>
+  </si>
+  <si>
+    <t>Meningitis Campaign denominator</t>
+  </si>
+  <si>
+    <t>Meningitis Campaign numerator</t>
+  </si>
+  <si>
+    <t>Yellow Fever Campaign denominator</t>
+  </si>
+  <si>
+    <t>Yellow Fever Campaign numerator</t>
   </si>
 </sst>
 </file>
@@ -2094,10 +2124,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2162,7 +2193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>510</v>
       </c>
@@ -2215,7 +2246,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>467</v>
       </c>
@@ -2310,6 +2341,15 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
+      <c r="K5" t="s">
+        <v>560</v>
+      </c>
+      <c r="N5" t="s">
+        <v>558</v>
+      </c>
+      <c r="O5" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2336,8 +2376,17 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>561</v>
+      </c>
+      <c r="N6" t="s">
+        <v>559</v>
+      </c>
+      <c r="O6" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>472</v>
       </c>
@@ -2417,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -2467,7 +2516,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>392</v>
       </c>
@@ -2517,7 +2566,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>476</v>
       </c>
@@ -2597,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>274</v>
       </c>
@@ -2650,7 +2699,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>399</v>
       </c>
@@ -2688,7 +2737,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>403</v>
       </c>
@@ -2726,7 +2775,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>407</v>
       </c>
@@ -2764,7 +2813,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>280</v>
       </c>
@@ -2817,7 +2866,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>411</v>
       </c>
@@ -2855,7 +2904,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>415</v>
       </c>
@@ -2896,7 +2945,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>286</v>
       </c>
@@ -2949,7 +2998,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>292</v>
       </c>
@@ -3002,7 +3051,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>297</v>
       </c>
@@ -3055,7 +3104,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>418</v>
       </c>
@@ -3093,7 +3142,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>421</v>
       </c>
@@ -3131,7 +3180,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>425</v>
       </c>
@@ -3169,7 +3218,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>302</v>
       </c>
@@ -3222,7 +3271,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>429</v>
       </c>
@@ -3260,7 +3309,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>433</v>
       </c>
@@ -3298,7 +3347,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>307</v>
       </c>
@@ -3351,7 +3400,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -3404,7 +3453,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>437</v>
       </c>
@@ -3442,7 +3491,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>441</v>
       </c>
@@ -3480,7 +3529,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>312</v>
       </c>
@@ -3521,7 +3570,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>317</v>
       </c>
@@ -3574,7 +3623,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>447</v>
       </c>
@@ -3612,7 +3661,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>451</v>
       </c>
@@ -3650,7 +3699,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>455</v>
       </c>
@@ -3688,7 +3737,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>322</v>
       </c>
@@ -3741,7 +3790,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>328</v>
       </c>
@@ -3794,7 +3843,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>459</v>
       </c>
@@ -3832,7 +3881,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>463</v>
       </c>
@@ -3870,7 +3919,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>333</v>
       </c>
@@ -3923,7 +3972,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>338</v>
       </c>
@@ -3976,7 +4025,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>395</v>
       </c>
@@ -4023,7 +4072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>480</v>
       </c>
@@ -4046,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>482</v>
       </c>
@@ -4129,6 +4178,9 @@
       <c r="I52" t="b">
         <v>0</v>
       </c>
+      <c r="K52" t="s">
+        <v>562</v>
+      </c>
       <c r="L52" t="s">
         <v>549</v>
       </c>
@@ -4161,6 +4213,9 @@
       <c r="I53" t="b">
         <v>0</v>
       </c>
+      <c r="K53" t="s">
+        <v>563</v>
+      </c>
       <c r="L53" t="s">
         <v>549</v>
       </c>
@@ -4174,7 +4229,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>349</v>
       </c>
@@ -4227,7 +4282,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>486</v>
       </c>
@@ -4259,7 +4314,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>487</v>
       </c>
@@ -4363,6 +4418,9 @@
       <c r="I58" t="b">
         <v>0</v>
       </c>
+      <c r="K58" t="s">
+        <v>564</v>
+      </c>
       <c r="L58" t="s">
         <v>549</v>
       </c>
@@ -4401,6 +4459,9 @@
       <c r="I59" t="b">
         <v>0</v>
       </c>
+      <c r="K59" t="s">
+        <v>565</v>
+      </c>
       <c r="L59" t="s">
         <v>549</v>
       </c>
@@ -4414,7 +4475,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>363</v>
       </c>
@@ -4464,7 +4525,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>491</v>
       </c>
@@ -4496,7 +4557,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>384</v>
       </c>
@@ -4546,7 +4607,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>492</v>
       </c>
@@ -4578,7 +4639,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>343</v>
       </c>
@@ -4631,7 +4692,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>493</v>
       </c>
@@ -4663,7 +4724,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>375</v>
       </c>
@@ -4710,7 +4771,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>388</v>
       </c>
@@ -4760,7 +4821,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>494</v>
       </c>
@@ -4798,7 +4859,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>496</v>
       </c>
@@ -4902,6 +4963,9 @@
       <c r="I71" t="b">
         <v>0</v>
       </c>
+      <c r="K71" t="s">
+        <v>566</v>
+      </c>
       <c r="L71" t="s">
         <v>549</v>
       </c>
@@ -4940,6 +5004,9 @@
       <c r="I72" t="b">
         <v>0</v>
       </c>
+      <c r="K72" t="s">
+        <v>567</v>
+      </c>
       <c r="L72" t="s">
         <v>549</v>
       </c>
@@ -4953,7 +5020,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>355</v>
       </c>
@@ -5003,7 +5070,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>500</v>
       </c>
@@ -5035,7 +5102,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -5088,7 +5155,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>191</v>
       </c>
@@ -5141,7 +5208,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>511</v>
       </c>
@@ -5179,7 +5246,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>232</v>
       </c>
@@ -5232,7 +5299,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>211</v>
       </c>
@@ -5285,7 +5352,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>247</v>
       </c>
@@ -5338,7 +5405,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>170</v>
       </c>
@@ -5391,7 +5458,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>267</v>
       </c>
@@ -5444,7 +5511,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>512</v>
       </c>
@@ -5497,7 +5564,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>219</v>
       </c>
@@ -5550,7 +5617,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>241</v>
       </c>
@@ -5600,7 +5667,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -5653,7 +5720,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>254</v>
       </c>
@@ -5706,7 +5773,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>177</v>
       </c>
@@ -5759,7 +5826,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>508</v>
       </c>
@@ -5782,7 +5849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>184</v>
       </c>
@@ -5835,7 +5902,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>204</v>
       </c>
@@ -5888,7 +5955,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>513</v>
       </c>
@@ -5929,7 +5996,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>227</v>
       </c>
@@ -5982,7 +6049,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>143</v>
       </c>
@@ -6035,7 +6102,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>121</v>
       </c>
@@ -6088,7 +6155,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -6141,7 +6208,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>63</v>
       </c>
@@ -6194,7 +6261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>41</v>
       </c>
@@ -6247,7 +6314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -6300,7 +6367,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>514</v>
       </c>
@@ -6329,7 +6396,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>515</v>
       </c>
@@ -6358,7 +6425,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>516</v>
       </c>
@@ -6387,7 +6454,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>504</v>
       </c>
@@ -6413,7 +6480,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>517</v>
       </c>
@@ -6442,7 +6509,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>506</v>
       </c>
@@ -6468,7 +6535,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -6521,7 +6588,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>110</v>
       </c>
@@ -6571,7 +6638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>106</v>
       </c>
@@ -6621,7 +6688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>137</v>
       </c>
@@ -6674,7 +6741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>56</v>
       </c>
@@ -6727,7 +6794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>34</v>
       </c>
@@ -6780,7 +6847,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>129</v>
       </c>
@@ -6833,7 +6900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -6886,7 +6953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -6939,7 +7006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>70</v>
       </c>
@@ -6992,7 +7059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>150</v>
       </c>
@@ -7045,7 +7112,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -7098,7 +7165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>85</v>
       </c>
@@ -7151,7 +7218,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>96</v>
       </c>
@@ -7201,7 +7268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>92</v>
       </c>
@@ -7252,7 +7319,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q120" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q120" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*campaign*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q120">
     <sortCondition descending="1" ref="G2:G120"/>
     <sortCondition descending="1" ref="E2:E120"/>

</xml_diff>

<commit_message>
Converts xlsx files in data-raw to xslx to allow track change.
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WHO\billionaiRe\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16D089E-B839-48BE-8959-82C601A9C9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF5D77E-1965-4558-AF1D-9C5B37DB941A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="558">
   <si>
     <t>dashboard_id</t>
   </si>
@@ -1708,36 +1708,6 @@
   </si>
   <si>
     <t>Overall HPOP Population healthier (with double counting)</t>
-  </si>
-  <si>
-    <t>Cholera - Campaign target population (denominator)</t>
-  </si>
-  <si>
-    <t>Cholera - Campaign reached population (numerator)</t>
-  </si>
-  <si>
-    <t>Cholera Campaign denominator</t>
-  </si>
-  <si>
-    <t>Cholera Campaign numerator</t>
-  </si>
-  <si>
-    <t>Measles Campaign denominator</t>
-  </si>
-  <si>
-    <t>Measles Campaign numerator</t>
-  </si>
-  <si>
-    <t>Meningitis Campaign denominator</t>
-  </si>
-  <si>
-    <t>Meningitis Campaign numerator</t>
-  </si>
-  <si>
-    <t>Yellow Fever Campaign denominator</t>
-  </si>
-  <si>
-    <t>Yellow Fever Campaign numerator</t>
   </si>
 </sst>
 </file>
@@ -2127,8 +2097,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2193,7 +2163,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>510</v>
       </c>
@@ -2269,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>372</v>
       </c>
@@ -2316,7 +2286,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>469</v>
       </c>
@@ -2341,17 +2311,8 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
-        <v>560</v>
-      </c>
-      <c r="N5" t="s">
-        <v>558</v>
-      </c>
-      <c r="O5" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>371</v>
       </c>
@@ -2375,15 +2336,6 @@
       </c>
       <c r="I6" t="b">
         <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>561</v>
-      </c>
-      <c r="N6" t="s">
-        <v>559</v>
-      </c>
-      <c r="O6" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
@@ -2406,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>473</v>
       </c>
@@ -2426,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>474</v>
       </c>
@@ -2446,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>475</v>
       </c>
@@ -2586,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>477</v>
       </c>
@@ -2606,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>478</v>
       </c>
@@ -2626,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>479</v>
       </c>
@@ -4127,7 +4079,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>483</v>
       </c>
@@ -4159,7 +4111,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>484</v>
       </c>
@@ -4178,9 +4130,6 @@
       <c r="I52" t="b">
         <v>0</v>
       </c>
-      <c r="K52" t="s">
-        <v>562</v>
-      </c>
       <c r="L52" t="s">
         <v>549</v>
       </c>
@@ -4194,7 +4143,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>485</v>
       </c>
@@ -4212,9 +4161,6 @@
       </c>
       <c r="I53" t="b">
         <v>0</v>
-      </c>
-      <c r="K53" t="s">
-        <v>563</v>
       </c>
       <c r="L53" t="s">
         <v>549</v>
@@ -4346,7 +4292,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>368</v>
       </c>
@@ -4393,7 +4339,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>488</v>
       </c>
@@ -4418,9 +4364,6 @@
       <c r="I58" t="b">
         <v>0</v>
       </c>
-      <c r="K58" t="s">
-        <v>564</v>
-      </c>
       <c r="L58" t="s">
         <v>549</v>
       </c>
@@ -4434,7 +4377,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>367</v>
       </c>
@@ -4458,9 +4401,6 @@
       </c>
       <c r="I59" t="b">
         <v>0</v>
-      </c>
-      <c r="K59" t="s">
-        <v>565</v>
       </c>
       <c r="L59" t="s">
         <v>549</v>
@@ -4891,7 +4831,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>360</v>
       </c>
@@ -4938,7 +4878,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>497</v>
       </c>
@@ -4963,9 +4903,6 @@
       <c r="I71" t="b">
         <v>0</v>
       </c>
-      <c r="K71" t="s">
-        <v>566</v>
-      </c>
       <c r="L71" t="s">
         <v>549</v>
       </c>
@@ -4979,7 +4916,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>359</v>
       </c>
@@ -5003,9 +4940,6 @@
       </c>
       <c r="I72" t="b">
         <v>0</v>
-      </c>
-      <c r="K72" t="s">
-        <v>567</v>
       </c>
       <c r="L72" t="s">
         <v>549</v>
@@ -5102,7 +5036,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -5155,7 +5089,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>191</v>
       </c>
@@ -5208,7 +5142,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>511</v>
       </c>
@@ -5246,7 +5180,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>232</v>
       </c>
@@ -5299,7 +5233,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>211</v>
       </c>
@@ -5352,7 +5286,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>247</v>
       </c>
@@ -5405,7 +5339,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>170</v>
       </c>
@@ -5458,7 +5392,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>267</v>
       </c>
@@ -5511,7 +5445,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>512</v>
       </c>
@@ -5564,7 +5498,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>219</v>
       </c>
@@ -5617,7 +5551,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>241</v>
       </c>
@@ -5667,7 +5601,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -5720,7 +5654,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>254</v>
       </c>
@@ -5773,7 +5707,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>177</v>
       </c>
@@ -5826,7 +5760,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>508</v>
       </c>
@@ -5849,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>184</v>
       </c>
@@ -5902,7 +5836,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>204</v>
       </c>
@@ -5955,7 +5889,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>513</v>
       </c>
@@ -5996,7 +5930,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>227</v>
       </c>
@@ -7320,10 +7254,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q120" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter val="*campaign*"/>
-      </customFilters>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q120">

</xml_diff>

<commit_message>
updating indicator_df clean fuels
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/robsona_who_int/Documents/Alice/Rwork/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{6693E9E6-59D4-4F88-8AE0-7E1493FEE32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23CC0029-0578-44B5-9EF6-AA0AC217F08D}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{6693E9E6-59D4-4F88-8AE0-7E1493FEE32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9D95AF4-B5C9-4B36-98CA-0EEF706A9306}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28335" yWindow="690" windowWidth="26085" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="525">
   <si>
     <t>dashboard_id</t>
   </si>
@@ -1589,6 +1589,12 @@
   </si>
   <si>
     <t>data_source</t>
+  </si>
+  <si>
+    <t>Global Health Observatory (GHO), World Health Organisation (WHO).</t>
+  </si>
+  <si>
+    <t>$filter=SpatialDimType eq 'COUNTRY' and  Dim1 eq 'TOTL'</t>
   </si>
 </sst>
 </file>
@@ -1991,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6138,6 +6144,12 @@
       <c r="C99" s="2" t="s">
         <v>518</v>
       </c>
+      <c r="D99" t="s">
+        <v>524</v>
+      </c>
+      <c r="E99" t="s">
+        <v>523</v>
+      </c>
       <c r="F99" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
updating indicator_df for source and gho_query
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/robsona_who_int/Documents/Alice/Rwork/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{6693E9E6-59D4-4F88-8AE0-7E1493FEE32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9D95AF4-B5C9-4B36-98CA-0EEF706A9306}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{6693E9E6-59D4-4F88-8AE0-7E1493FEE32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D04EA952-50D1-4A11-AF84-8E3141C95738}"/>
   <bookViews>
-    <workbookView xWindow="-28335" yWindow="690" windowWidth="26085" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27645" yWindow="1380" windowWidth="26085" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="538">
   <si>
     <t>dashboard_id</t>
   </si>
@@ -1561,9 +1561,6 @@
     <t>NHL</t>
   </si>
   <si>
-    <t>SDGIPV12M</t>
-  </si>
-  <si>
     <t>NUTSTUNTINGPREV</t>
   </si>
   <si>
@@ -1595,6 +1592,48 @@
   </si>
   <si>
     <t>$filter=SpatialDimType eq 'COUNTRY' and  Dim1 eq 'TOTL'</t>
+  </si>
+  <si>
+    <t>$filter=SpatialDimType eq 'COUNTRY' and  Dim1 eq 'BTSX'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Global Status Report on Road Safety, WHO (2018)</t>
+  </si>
+  <si>
+    <t>WHO estimates, 2016</t>
+  </si>
+  <si>
+    <t>$filter=SpatialDimType eq 'COUNTRY' and  Dim1 eq 'BTSX' and Dim2 eq 'YEARS05-19'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Multiple survey data</t>
+  </si>
+  <si>
+    <t>WHO Global Information System on Alcohol and Health (GISAH)</t>
+  </si>
+  <si>
+    <t>WHO/UNICEF Joint Monitoring Programme for Water Supply, Sanitation and Hygiene (2021)</t>
+  </si>
+  <si>
+    <t>WHO global report on trends in prevalence of tobacco use 2000-2025, 4th edition, 2021</t>
+  </si>
+  <si>
+    <t>WHO GHO</t>
+  </si>
+  <si>
+    <t>Joint Child Malnutrition Estimates (2021 Edition), United Nations Children's Fund (UNICEF), World Health Organisation (WHO) and the World Bank Group.</t>
+  </si>
+  <si>
+    <t>Half the world's population are exposed to increasing air pollution. Clim Atmos Sci (2020)</t>
+  </si>
+  <si>
+    <t>Multiple survey data. UNICEF/WHO/World Bank.</t>
+  </si>
+  <si>
+    <t>SDGIPVLT</t>
+  </si>
+  <si>
+    <t>GINA - TFA Country Score Card</t>
   </si>
 </sst>
 </file>
@@ -1998,14 +2037,16 @@
   <dimension ref="A1:T120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2019,10 +2060,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -5723,6 +5764,9 @@
       <c r="C91" t="s">
         <v>203</v>
       </c>
+      <c r="E91" t="s">
+        <v>530</v>
+      </c>
       <c r="F91" t="s">
         <v>20</v>
       </c>
@@ -5800,10 +5844,13 @@
         <v>224</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D93" t="s">
-        <v>519</v>
+        <v>518</v>
+      </c>
+      <c r="E93" t="s">
+        <v>531</v>
       </c>
       <c r="F93" t="s">
         <v>50</v>
@@ -5862,7 +5909,10 @@
         <v>142</v>
       </c>
       <c r="D94" t="s">
-        <v>519</v>
+        <v>524</v>
+      </c>
+      <c r="E94" t="s">
+        <v>526</v>
       </c>
       <c r="F94" t="s">
         <v>50</v>
@@ -5920,6 +5970,12 @@
       <c r="C95" t="s">
         <v>120</v>
       </c>
+      <c r="D95" t="s">
+        <v>527</v>
+      </c>
+      <c r="E95" t="s">
+        <v>529</v>
+      </c>
       <c r="F95" t="s">
         <v>20</v>
       </c>
@@ -5976,6 +6032,9 @@
       <c r="C96" t="s">
         <v>49</v>
       </c>
+      <c r="E96" t="s">
+        <v>526</v>
+      </c>
       <c r="F96" t="s">
         <v>50</v>
       </c>
@@ -6032,6 +6091,9 @@
       <c r="C97" t="s">
         <v>63</v>
       </c>
+      <c r="E97" t="s">
+        <v>528</v>
+      </c>
       <c r="F97" t="s">
         <v>20</v>
       </c>
@@ -6088,6 +6150,9 @@
       <c r="C98" t="s">
         <v>42</v>
       </c>
+      <c r="E98" t="s">
+        <v>528</v>
+      </c>
       <c r="F98" t="s">
         <v>20</v>
       </c>
@@ -6142,13 +6207,13 @@
         <v>113</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D99" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E99" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F99" t="s">
         <v>50</v>
@@ -6339,7 +6404,10 @@
         <v>99</v>
       </c>
       <c r="D106" t="s">
-        <v>520</v>
+        <v>519</v>
+      </c>
+      <c r="E106" t="s">
+        <v>530</v>
       </c>
       <c r="F106" t="s">
         <v>20</v>
@@ -6503,6 +6571,12 @@
       <c r="C109" t="s">
         <v>135</v>
       </c>
+      <c r="D109" t="s">
+        <v>518</v>
+      </c>
+      <c r="E109" t="s">
+        <v>531</v>
+      </c>
       <c r="F109" t="s">
         <v>50</v>
       </c>
@@ -6557,7 +6631,10 @@
         <v>56</v>
       </c>
       <c r="C110" t="s">
-        <v>513</v>
+        <v>536</v>
+      </c>
+      <c r="E110" t="s">
+        <v>532</v>
       </c>
       <c r="F110" t="s">
         <v>20</v>
@@ -6613,10 +6690,12 @@
         <v>35</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
+      <c r="E111" s="2" t="s">
+        <v>533</v>
+      </c>
       <c r="F111" t="s">
         <v>20</v>
       </c>
@@ -6673,6 +6752,12 @@
       <c r="C112" t="s">
         <v>128</v>
       </c>
+      <c r="D112" t="s">
+        <v>523</v>
+      </c>
+      <c r="E112" t="s">
+        <v>534</v>
+      </c>
       <c r="F112" t="s">
         <v>50</v>
       </c>
@@ -6729,6 +6814,12 @@
       <c r="C113" t="s">
         <v>77</v>
       </c>
+      <c r="D113" t="s">
+        <v>524</v>
+      </c>
+      <c r="E113" t="s">
+        <v>525</v>
+      </c>
       <c r="F113" t="s">
         <v>20</v>
       </c>
@@ -6783,10 +6874,12 @@
         <v>19</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
+      <c r="E114" s="2" t="s">
+        <v>533</v>
+      </c>
       <c r="F114" t="s">
         <v>20</v>
       </c>
@@ -6844,10 +6937,10 @@
         <v>70</v>
       </c>
       <c r="D115" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E115" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F115" t="s">
         <v>20</v>
@@ -6905,6 +6998,9 @@
       <c r="C116" t="s">
         <v>149</v>
       </c>
+      <c r="E116" t="s">
+        <v>537</v>
+      </c>
       <c r="F116" t="s">
         <v>50</v>
       </c>
@@ -6961,6 +7057,9 @@
       <c r="C117" t="s">
         <v>29</v>
       </c>
+      <c r="E117" t="s">
+        <v>535</v>
+      </c>
       <c r="F117" t="s">
         <v>20</v>
       </c>
@@ -7018,7 +7117,10 @@
         <v>85</v>
       </c>
       <c r="D118" t="s">
-        <v>520</v>
+        <v>519</v>
+      </c>
+      <c r="E118" t="s">
+        <v>530</v>
       </c>
       <c r="F118" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Changed GHO code for blood pressure to "Prevalence of hypertension (defined as having systolic blood pressure ≥140 mmHg, diastolic blood pressure ≥90 mmHg, or taking medication for hypertension) among adults aged 30-79."
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/robsona_who_int/Documents/Alice/Rwork/billionaiRe/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vasa/who/3b/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{6693E9E6-59D4-4F88-8AE0-7E1493FEE32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{449B8437-A255-483D-BF8C-5C210A66CE0E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BBEAAE-6B10-C441-85A1-E977C41429A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27645" yWindow="1380" windowWidth="26085" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,18 +652,12 @@
     <t>bp</t>
   </si>
   <si>
-    <t>BP_04</t>
-  </si>
-  <si>
     <t>SDG 3.8.1.9</t>
   </si>
   <si>
     <t>Prevention of cardiovascular disease</t>
   </si>
   <si>
-    <t>Prevalence of raised blood pressure*</t>
-  </si>
-  <si>
     <t>Non-elevated blood pressure</t>
   </si>
   <si>
@@ -1634,6 +1628,12 @@
   </si>
   <si>
     <t>GINA - TFA Country Score Card</t>
+  </si>
+  <si>
+    <t>NCD_HYP_TREATMENT_A</t>
+  </si>
+  <si>
+    <t>Prevalence of hypertension (defined as having systolic blood pressure ≥140 mmHg, diastolic blood pressure ≥90 mmHg, or taking medication for hypertension) among adults aged 30-79.</t>
   </si>
 </sst>
 </file>
@@ -2036,18 +2036,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="C72" workbookViewId="0">
+      <selection activeCell="Q79" sqref="Q79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="27.5" customWidth="1"/>
+    <col min="16" max="16" width="34.33203125" customWidth="1"/>
+    <col min="17" max="17" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2058,10 +2060,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2109,15 +2111,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -2138,39 +2140,39 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M2" t="s">
+        <v>258</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
         <v>259</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>260</v>
       </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>262</v>
-      </c>
       <c r="R2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="S2">
         <v>37</v>
       </c>
       <c r="T2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2188,9 +2190,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F4" t="s">
         <v>50</v>
@@ -2211,10 +2213,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="M4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="N4" t="s">
         <v>23</v>
@@ -2223,27 +2225,27 @@
         <v>23</v>
       </c>
       <c r="P4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="Q4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="R4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="S4">
         <v>58</v>
       </c>
       <c r="T4" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -2264,12 +2266,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F6" t="s">
         <v>50</v>
@@ -2290,70 +2292,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>465</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>466</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>467</v>
       </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>468</v>
       </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>469</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>470</v>
-      </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
@@ -2370,12 +2372,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -2396,39 +2398,39 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
+        <v>373</v>
+      </c>
+      <c r="M11" t="s">
+        <v>374</v>
+      </c>
+      <c r="N11" t="s">
         <v>375</v>
       </c>
-      <c r="M11" t="s">
-        <v>376</v>
-      </c>
-      <c r="N11" t="s">
-        <v>377</v>
-      </c>
       <c r="O11" t="s">
         <v>23</v>
       </c>
       <c r="P11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="Q11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="R11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="S11">
         <v>60</v>
       </c>
       <c r="T11" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -2449,97 +2451,97 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="N12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="O12" t="s">
         <v>23</v>
       </c>
       <c r="P12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="Q12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="R12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S12">
         <v>63</v>
       </c>
       <c r="T12" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>469</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>470</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>471</v>
       </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>472</v>
       </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>473</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>474</v>
-      </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
@@ -2556,15 +2558,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" t="s">
+        <v>269</v>
+      </c>
+      <c r="C17" t="s">
         <v>270</v>
-      </c>
-      <c r="B17" t="s">
-        <v>271</v>
-      </c>
-      <c r="C17" t="s">
-        <v>272</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -2585,10 +2587,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="N17" t="s">
         <v>23</v>
@@ -2597,24 +2599,24 @@
         <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="R17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="S17">
         <v>39</v>
       </c>
       <c r="T17" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
@@ -2635,27 +2637,27 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
+        <v>393</v>
+      </c>
+      <c r="N18" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P18" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q18" t="s">
         <v>395</v>
       </c>
-      <c r="N18" t="s">
-        <v>23</v>
-      </c>
-      <c r="O18" t="s">
-        <v>23</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>396</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>397</v>
-      </c>
-      <c r="R18" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>398</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
@@ -2676,27 +2678,27 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
+        <v>397</v>
+      </c>
+      <c r="N19" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q19" t="s">
         <v>399</v>
       </c>
-      <c r="N19" t="s">
-        <v>23</v>
-      </c>
-      <c r="O19" t="s">
-        <v>23</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>400</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>401</v>
-      </c>
-      <c r="R19" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>402</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
@@ -2717,33 +2719,33 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
+        <v>401</v>
+      </c>
+      <c r="N20" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" t="s">
+        <v>23</v>
+      </c>
+      <c r="P20" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q20" t="s">
         <v>403</v>
       </c>
-      <c r="N20" t="s">
-        <v>23</v>
-      </c>
-      <c r="O20" t="s">
-        <v>23</v>
-      </c>
-      <c r="P20" t="s">
-        <v>404</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>405</v>
-      </c>
       <c r="R20" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>274</v>
+      </c>
+      <c r="B21" t="s">
+        <v>275</v>
+      </c>
+      <c r="C21" t="s">
         <v>276</v>
-      </c>
-      <c r="B21" t="s">
-        <v>277</v>
-      </c>
-      <c r="C21" t="s">
-        <v>278</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
@@ -2764,36 +2766,36 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M21" t="s">
+        <v>278</v>
+      </c>
+      <c r="N21" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" t="s">
         <v>279</v>
       </c>
-      <c r="M21" t="s">
-        <v>280</v>
-      </c>
-      <c r="N21" t="s">
-        <v>23</v>
-      </c>
-      <c r="O21" t="s">
-        <v>23</v>
-      </c>
-      <c r="P21" t="s">
-        <v>281</v>
-      </c>
       <c r="Q21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="R21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="S21">
         <v>40</v>
       </c>
       <c r="T21" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -2814,30 +2816,30 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
+        <v>405</v>
+      </c>
+      <c r="N22" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q22" t="s">
         <v>407</v>
       </c>
-      <c r="N22" t="s">
-        <v>23</v>
-      </c>
-      <c r="O22" t="s">
-        <v>23</v>
-      </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>408</v>
       </c>
-      <c r="Q22" t="s">
-        <v>409</v>
-      </c>
-      <c r="R22" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>410</v>
-      </c>
       <c r="C23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
@@ -2858,7 +2860,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="N23" t="s">
         <v>23</v>
@@ -2867,24 +2869,24 @@
         <v>23</v>
       </c>
       <c r="P23" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="Q23" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="R23" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>280</v>
+      </c>
+      <c r="B24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C24" t="s">
         <v>282</v>
-      </c>
-      <c r="B24" t="s">
-        <v>283</v>
-      </c>
-      <c r="C24" t="s">
-        <v>284</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
@@ -2905,42 +2907,42 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
+        <v>283</v>
+      </c>
+      <c r="M24" t="s">
+        <v>284</v>
+      </c>
+      <c r="N24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" t="s">
         <v>285</v>
       </c>
-      <c r="M24" t="s">
-        <v>286</v>
-      </c>
-      <c r="N24" t="s">
-        <v>23</v>
-      </c>
-      <c r="O24" t="s">
-        <v>23</v>
-      </c>
-      <c r="P24" t="s">
-        <v>287</v>
-      </c>
       <c r="Q24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="R24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="S24">
         <v>41</v>
       </c>
       <c r="T24" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>286</v>
+      </c>
+      <c r="B25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C25" t="s">
         <v>288</v>
-      </c>
-      <c r="B25" t="s">
-        <v>289</v>
-      </c>
-      <c r="C25" t="s">
-        <v>290</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
@@ -2961,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N25" t="s">
         <v>23</v>
@@ -2973,30 +2975,30 @@
         <v>23</v>
       </c>
       <c r="P25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="R25" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="S25">
         <v>42</v>
       </c>
       <c r="T25" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C26" t="s">
         <v>293</v>
-      </c>
-      <c r="B26" t="s">
-        <v>294</v>
-      </c>
-      <c r="C26" t="s">
-        <v>295</v>
       </c>
       <c r="F26" t="s">
         <v>20</v>
@@ -3017,10 +3019,10 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="N26" t="s">
         <v>23</v>
@@ -3029,24 +3031,24 @@
         <v>23</v>
       </c>
       <c r="P26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Q26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="R26" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="S26">
         <v>43</v>
       </c>
       <c r="T26" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
@@ -3067,27 +3069,27 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
+        <v>412</v>
+      </c>
+      <c r="N27" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" t="s">
+        <v>23</v>
+      </c>
+      <c r="P27" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>413</v>
+      </c>
+      <c r="R27" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>414</v>
-      </c>
-      <c r="N27" t="s">
-        <v>23</v>
-      </c>
-      <c r="O27" t="s">
-        <v>23</v>
-      </c>
-      <c r="P27" t="s">
-        <v>415</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>415</v>
-      </c>
-      <c r="R27" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>416</v>
       </c>
       <c r="F28" t="s">
         <v>20</v>
@@ -3108,27 +3110,27 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
+        <v>415</v>
+      </c>
+      <c r="N28" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P28" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q28" t="s">
         <v>417</v>
       </c>
-      <c r="N28" t="s">
-        <v>23</v>
-      </c>
-      <c r="O28" t="s">
-        <v>23</v>
-      </c>
-      <c r="P28" t="s">
+      <c r="R28" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>418</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>419</v>
-      </c>
-      <c r="R28" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>420</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
@@ -3149,33 +3151,33 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
+        <v>419</v>
+      </c>
+      <c r="N29" t="s">
+        <v>23</v>
+      </c>
+      <c r="O29" t="s">
+        <v>23</v>
+      </c>
+      <c r="P29" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q29" t="s">
         <v>421</v>
       </c>
-      <c r="N29" t="s">
-        <v>23</v>
-      </c>
-      <c r="O29" t="s">
-        <v>23</v>
-      </c>
-      <c r="P29" t="s">
-        <v>422</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>423</v>
-      </c>
       <c r="R29" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" t="s">
+        <v>297</v>
+      </c>
+      <c r="C30" t="s">
         <v>298</v>
-      </c>
-      <c r="B30" t="s">
-        <v>299</v>
-      </c>
-      <c r="C30" t="s">
-        <v>300</v>
       </c>
       <c r="F30" t="s">
         <v>20</v>
@@ -3196,10 +3198,10 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N30" t="s">
         <v>23</v>
@@ -3208,24 +3210,24 @@
         <v>23</v>
       </c>
       <c r="P30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Q30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="R30" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="S30">
         <v>44</v>
       </c>
       <c r="T30" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
@@ -3246,27 +3248,27 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
+        <v>423</v>
+      </c>
+      <c r="N31" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" t="s">
+        <v>23</v>
+      </c>
+      <c r="P31" t="s">
+        <v>424</v>
+      </c>
+      <c r="Q31" t="s">
         <v>425</v>
       </c>
-      <c r="N31" t="s">
-        <v>23</v>
-      </c>
-      <c r="O31" t="s">
-        <v>23</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="R31" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>426</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>427</v>
-      </c>
-      <c r="R31" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>428</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
@@ -3287,33 +3289,33 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
+        <v>427</v>
+      </c>
+      <c r="N32" t="s">
+        <v>23</v>
+      </c>
+      <c r="O32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P32" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q32" t="s">
         <v>429</v>
       </c>
-      <c r="N32" t="s">
-        <v>23</v>
-      </c>
-      <c r="O32" t="s">
-        <v>23</v>
-      </c>
-      <c r="P32" t="s">
-        <v>430</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>431</v>
-      </c>
       <c r="R32" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>301</v>
+      </c>
+      <c r="B33" t="s">
+        <v>302</v>
+      </c>
+      <c r="C33" t="s">
         <v>303</v>
-      </c>
-      <c r="B33" t="s">
-        <v>304</v>
-      </c>
-      <c r="C33" t="s">
-        <v>305</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
@@ -3334,10 +3336,10 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M33" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="N33" t="s">
         <v>23</v>
@@ -3346,30 +3348,30 @@
         <v>23</v>
       </c>
       <c r="P33" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Q33" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="R33" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="S33">
         <v>45</v>
       </c>
       <c r="T33" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>306</v>
+      </c>
+      <c r="B34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C34" t="s">
         <v>308</v>
-      </c>
-      <c r="B34" t="s">
-        <v>309</v>
-      </c>
-      <c r="C34" t="s">
-        <v>310</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
@@ -3390,10 +3392,10 @@
         <v>0</v>
       </c>
       <c r="L34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="M34" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="N34" t="s">
         <v>23</v>
@@ -3402,24 +3404,24 @@
         <v>23</v>
       </c>
       <c r="P34" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="Q34" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="R34" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="S34">
         <v>46</v>
       </c>
       <c r="T34" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F35" t="s">
         <v>20</v>
@@ -3440,27 +3442,27 @@
         <v>0</v>
       </c>
       <c r="L35" t="s">
+        <v>431</v>
+      </c>
+      <c r="N35" t="s">
+        <v>23</v>
+      </c>
+      <c r="O35" t="s">
+        <v>23</v>
+      </c>
+      <c r="P35" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q35" t="s">
         <v>433</v>
       </c>
-      <c r="N35" t="s">
-        <v>23</v>
-      </c>
-      <c r="O35" t="s">
-        <v>23</v>
-      </c>
-      <c r="P35" t="s">
+      <c r="R35" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>434</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>435</v>
-      </c>
-      <c r="R35" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>436</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
@@ -3481,30 +3483,30 @@
         <v>0</v>
       </c>
       <c r="L36" t="s">
+        <v>435</v>
+      </c>
+      <c r="N36" t="s">
+        <v>23</v>
+      </c>
+      <c r="O36" t="s">
+        <v>23</v>
+      </c>
+      <c r="P36" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>436</v>
+      </c>
+      <c r="R36" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>306</v>
+      </c>
+      <c r="B37" t="s">
         <v>437</v>
-      </c>
-      <c r="N36" t="s">
-        <v>23</v>
-      </c>
-      <c r="O36" t="s">
-        <v>23</v>
-      </c>
-      <c r="P36" t="s">
-        <v>438</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>438</v>
-      </c>
-      <c r="R36" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>308</v>
-      </c>
-      <c r="B37" t="s">
-        <v>439</v>
       </c>
       <c r="F37" t="s">
         <v>20</v>
@@ -3525,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="L37" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="N37" t="s">
         <v>23</v>
@@ -3534,24 +3536,24 @@
         <v>23</v>
       </c>
       <c r="P37" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q37" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="R37" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>311</v>
+      </c>
+      <c r="B38" t="s">
+        <v>312</v>
+      </c>
+      <c r="C38" t="s">
         <v>313</v>
-      </c>
-      <c r="B38" t="s">
-        <v>314</v>
-      </c>
-      <c r="C38" t="s">
-        <v>315</v>
       </c>
       <c r="F38" t="s">
         <v>20</v>
@@ -3572,10 +3574,10 @@
         <v>0</v>
       </c>
       <c r="L38" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M38" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N38" t="s">
         <v>23</v>
@@ -3584,24 +3586,24 @@
         <v>23</v>
       </c>
       <c r="P38" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q38" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="S38">
         <v>47</v>
       </c>
       <c r="T38" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
@@ -3622,27 +3624,27 @@
         <v>0</v>
       </c>
       <c r="L39" t="s">
+        <v>441</v>
+      </c>
+      <c r="N39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P39" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q39" t="s">
         <v>443</v>
       </c>
-      <c r="N39" t="s">
-        <v>23</v>
-      </c>
-      <c r="O39" t="s">
-        <v>23</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="R39" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>444</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>445</v>
-      </c>
-      <c r="R39" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>446</v>
       </c>
       <c r="F40" t="s">
         <v>20</v>
@@ -3663,27 +3665,27 @@
         <v>0</v>
       </c>
       <c r="L40" t="s">
+        <v>445</v>
+      </c>
+      <c r="N40" t="s">
+        <v>23</v>
+      </c>
+      <c r="O40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P40" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q40" t="s">
         <v>447</v>
       </c>
-      <c r="N40" t="s">
-        <v>23</v>
-      </c>
-      <c r="O40" t="s">
-        <v>23</v>
-      </c>
-      <c r="P40" t="s">
+      <c r="R40" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>448</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>449</v>
-      </c>
-      <c r="R40" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>450</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
@@ -3704,33 +3706,33 @@
         <v>0</v>
       </c>
       <c r="L41" t="s">
+        <v>449</v>
+      </c>
+      <c r="N41" t="s">
+        <v>23</v>
+      </c>
+      <c r="O41" t="s">
+        <v>23</v>
+      </c>
+      <c r="P41" t="s">
+        <v>450</v>
+      </c>
+      <c r="Q41" t="s">
         <v>451</v>
       </c>
-      <c r="N41" t="s">
-        <v>23</v>
-      </c>
-      <c r="O41" t="s">
-        <v>23</v>
-      </c>
-      <c r="P41" t="s">
-        <v>452</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>453</v>
-      </c>
       <c r="R41" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>316</v>
+      </c>
+      <c r="B42" t="s">
+        <v>317</v>
+      </c>
+      <c r="C42" t="s">
         <v>318</v>
-      </c>
-      <c r="B42" t="s">
-        <v>319</v>
-      </c>
-      <c r="C42" t="s">
-        <v>320</v>
       </c>
       <c r="F42" t="s">
         <v>20</v>
@@ -3751,10 +3753,10 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="M42" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N42" t="s">
         <v>23</v>
@@ -3763,30 +3765,30 @@
         <v>23</v>
       </c>
       <c r="P42" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="Q42" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="R42" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S42">
         <v>48</v>
       </c>
       <c r="T42" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>321</v>
+      </c>
+      <c r="B43" t="s">
+        <v>322</v>
+      </c>
+      <c r="C43" t="s">
         <v>323</v>
-      </c>
-      <c r="B43" t="s">
-        <v>324</v>
-      </c>
-      <c r="C43" t="s">
-        <v>325</v>
       </c>
       <c r="F43" t="s">
         <v>20</v>
@@ -3807,10 +3809,10 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="N43" t="s">
         <v>23</v>
@@ -3819,24 +3821,24 @@
         <v>23</v>
       </c>
       <c r="P43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="R43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="S43">
         <v>49</v>
       </c>
       <c r="T43" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
@@ -3857,27 +3859,27 @@
         <v>0</v>
       </c>
       <c r="L44" t="s">
+        <v>453</v>
+      </c>
+      <c r="N44" t="s">
+        <v>23</v>
+      </c>
+      <c r="O44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P44" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q44" t="s">
         <v>455</v>
       </c>
-      <c r="N44" t="s">
-        <v>23</v>
-      </c>
-      <c r="O44" t="s">
-        <v>23</v>
-      </c>
-      <c r="P44" t="s">
+      <c r="R44" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>456</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>457</v>
-      </c>
-      <c r="R44" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>458</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
@@ -3898,33 +3900,33 @@
         <v>0</v>
       </c>
       <c r="L45" t="s">
+        <v>457</v>
+      </c>
+      <c r="N45" t="s">
+        <v>23</v>
+      </c>
+      <c r="O45" t="s">
+        <v>23</v>
+      </c>
+      <c r="P45" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q45" t="s">
         <v>459</v>
       </c>
-      <c r="N45" t="s">
-        <v>23</v>
-      </c>
-      <c r="O45" t="s">
-        <v>23</v>
-      </c>
-      <c r="P45" t="s">
-        <v>460</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>461</v>
-      </c>
       <c r="R45" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>326</v>
+      </c>
+      <c r="B46" t="s">
+        <v>327</v>
+      </c>
+      <c r="C46" t="s">
         <v>328</v>
-      </c>
-      <c r="B46" t="s">
-        <v>329</v>
-      </c>
-      <c r="C46" t="s">
-        <v>330</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
@@ -3945,10 +3947,10 @@
         <v>0</v>
       </c>
       <c r="L46" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M46" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N46" t="s">
         <v>23</v>
@@ -3957,30 +3959,30 @@
         <v>23</v>
       </c>
       <c r="P46" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="Q46" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="R46" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="S46">
         <v>50</v>
       </c>
       <c r="T46" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>331</v>
+      </c>
+      <c r="B47" t="s">
+        <v>332</v>
+      </c>
+      <c r="C47" t="s">
         <v>333</v>
-      </c>
-      <c r="B47" t="s">
-        <v>334</v>
-      </c>
-      <c r="C47" t="s">
-        <v>335</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
@@ -4001,10 +4003,10 @@
         <v>0</v>
       </c>
       <c r="L47" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M47" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="N47" t="s">
         <v>23</v>
@@ -4013,63 +4015,63 @@
         <v>23</v>
       </c>
       <c r="P47" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="Q47" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="R47" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="S47">
         <v>51</v>
       </c>
       <c r="T47" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>388</v>
+      </c>
+      <c r="B48" t="s">
+        <v>389</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L48" t="s">
         <v>390</v>
       </c>
-      <c r="B48" t="s">
+      <c r="M48" t="s">
+        <v>390</v>
+      </c>
+      <c r="N48" t="s">
+        <v>23</v>
+      </c>
+      <c r="O48" t="s">
+        <v>23</v>
+      </c>
+      <c r="P48" t="s">
         <v>391</v>
       </c>
-      <c r="G48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" t="b">
-        <v>1</v>
-      </c>
-      <c r="J48" t="b">
-        <v>0</v>
-      </c>
-      <c r="K48" t="b">
-        <v>1</v>
-      </c>
-      <c r="L48" t="s">
-        <v>392</v>
-      </c>
-      <c r="M48" t="s">
-        <v>392</v>
-      </c>
-      <c r="N48" t="s">
-        <v>23</v>
-      </c>
-      <c r="O48" t="s">
-        <v>23</v>
-      </c>
-      <c r="P48" t="s">
-        <v>393</v>
-      </c>
       <c r="Q48" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="R48" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="S48">
         <v>64</v>
@@ -4078,93 +4080,93 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>473</v>
+      </c>
+      <c r="B49" t="s">
+        <v>474</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
         <v>475</v>
       </c>
-      <c r="B49" t="s">
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
         <v>476</v>
       </c>
-      <c r="G49" t="b">
-        <v>0</v>
-      </c>
-      <c r="H49" t="b">
-        <v>0</v>
-      </c>
-      <c r="I49" t="b">
-        <v>1</v>
-      </c>
-      <c r="J49" t="b">
-        <v>0</v>
-      </c>
-      <c r="K49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>477</v>
       </c>
-      <c r="G50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" t="b">
-        <v>1</v>
-      </c>
-      <c r="J50" t="b">
-        <v>0</v>
-      </c>
-      <c r="K50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>478</v>
       </c>
-      <c r="G51" t="b">
-        <v>0</v>
-      </c>
-      <c r="H51" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" t="b">
-        <v>1</v>
-      </c>
-      <c r="J51" t="b">
-        <v>0</v>
-      </c>
-      <c r="K51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>479</v>
-      </c>
-      <c r="G52" t="b">
-        <v>0</v>
-      </c>
-      <c r="H52" t="b">
-        <v>0</v>
-      </c>
-      <c r="I52" t="b">
-        <v>1</v>
-      </c>
-      <c r="J52" t="b">
-        <v>0</v>
-      </c>
-      <c r="K52" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>480</v>
-      </c>
       <c r="G53" t="b">
         <v>0</v>
       </c>
@@ -4181,15 +4183,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>342</v>
+      </c>
+      <c r="B54" t="s">
+        <v>343</v>
+      </c>
+      <c r="C54" t="s">
         <v>344</v>
-      </c>
-      <c r="B54" t="s">
-        <v>345</v>
-      </c>
-      <c r="C54" t="s">
-        <v>346</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
@@ -4210,36 +4212,36 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
+        <v>345</v>
+      </c>
+      <c r="M54" t="s">
+        <v>346</v>
+      </c>
+      <c r="N54" t="s">
+        <v>23</v>
+      </c>
+      <c r="O54" t="s">
+        <v>23</v>
+      </c>
+      <c r="P54" t="s">
         <v>347</v>
       </c>
-      <c r="M54" t="s">
-        <v>348</v>
-      </c>
-      <c r="N54" t="s">
-        <v>23</v>
-      </c>
-      <c r="O54" t="s">
-        <v>23</v>
-      </c>
-      <c r="P54" t="s">
-        <v>349</v>
-      </c>
       <c r="Q54" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="R54" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="S54">
         <v>53</v>
       </c>
       <c r="T54" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -4257,9 +4259,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G56" t="b">
         <v>0</v>
@@ -4277,9 +4279,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F57" t="s">
         <v>50</v>
@@ -4300,10 +4302,10 @@
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="M57" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="N57" t="s">
         <v>23</v>
@@ -4312,27 +4314,27 @@
         <v>23</v>
       </c>
       <c r="P57" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="Q57" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="R57" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="S57">
         <v>57</v>
       </c>
       <c r="T57" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B58" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F58" t="s">
         <v>50</v>
@@ -4353,12 +4355,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B59" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F59" t="s">
         <v>50</v>
@@ -4379,12 +4381,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B60" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F60" t="s">
         <v>20</v>
@@ -4405,10 +4407,10 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="M60" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="N60" t="s">
         <v>23</v>
@@ -4417,24 +4419,24 @@
         <v>23</v>
       </c>
       <c r="P60" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="Q60" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R60" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="S60">
         <v>56</v>
       </c>
       <c r="T60" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G61" t="b">
         <v>0</v>
@@ -4452,12 +4454,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B62" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F62" t="s">
         <v>20</v>
@@ -4478,36 +4480,36 @@
         <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="M62" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="N62" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="O62" t="s">
         <v>23</v>
       </c>
       <c r="P62" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="Q62" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="R62" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S62">
         <v>61</v>
       </c>
       <c r="T62" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -4525,15 +4527,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>336</v>
+      </c>
+      <c r="B64" t="s">
+        <v>337</v>
+      </c>
+      <c r="C64" t="s">
         <v>338</v>
-      </c>
-      <c r="B64" t="s">
-        <v>339</v>
-      </c>
-      <c r="C64" t="s">
-        <v>340</v>
       </c>
       <c r="F64" t="s">
         <v>20</v>
@@ -4554,10 +4556,10 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M64" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="N64" t="s">
         <v>23</v>
@@ -4566,24 +4568,24 @@
         <v>23</v>
       </c>
       <c r="P64" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Q64" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="R64" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S64">
         <v>52</v>
       </c>
       <c r="T64" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -4601,34 +4603,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>368</v>
+      </c>
+      <c r="B66" t="s">
+        <v>341</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="b">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>369</v>
+      </c>
+      <c r="M66" t="s">
         <v>370</v>
       </c>
-      <c r="B66" t="s">
-        <v>343</v>
-      </c>
-      <c r="G66" t="b">
-        <v>0</v>
-      </c>
-      <c r="H66" t="b">
-        <v>0</v>
-      </c>
-      <c r="I66" t="b">
-        <v>1</v>
-      </c>
-      <c r="J66" t="b">
-        <v>0</v>
-      </c>
-      <c r="K66" t="b">
-        <v>1</v>
-      </c>
-      <c r="L66" t="s">
-        <v>371</v>
-      </c>
-      <c r="M66" t="s">
-        <v>372</v>
-      </c>
       <c r="N66" t="s">
         <v>23</v>
       </c>
@@ -4636,27 +4638,27 @@
         <v>23</v>
       </c>
       <c r="P66" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="Q66" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R66" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="S66">
         <v>59</v>
       </c>
       <c r="T66" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B67" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F67" t="s">
         <v>20</v>
@@ -4677,39 +4679,39 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M67" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="N67" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="O67" t="s">
         <v>23</v>
       </c>
       <c r="P67" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="Q67" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="R67" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S67">
         <v>62</v>
       </c>
       <c r="T67" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B68" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F68" t="s">
         <v>50</v>
@@ -4730,9 +4732,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
@@ -4750,9 +4752,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F70" t="s">
         <v>50</v>
@@ -4773,10 +4775,10 @@
         <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="M70" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N70" t="s">
         <v>23</v>
@@ -4785,27 +4787,27 @@
         <v>23</v>
       </c>
       <c r="P70" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="Q70" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="R70" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="S70">
         <v>55</v>
       </c>
       <c r="T70" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B71" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F71" t="s">
         <v>50</v>
@@ -4826,12 +4828,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B72" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F72" t="s">
         <v>50</v>
@@ -4852,12 +4854,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F73" t="s">
         <v>20</v>
@@ -4878,10 +4880,10 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M73" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N73" t="s">
         <v>23</v>
@@ -4890,24 +4892,24 @@
         <v>23</v>
       </c>
       <c r="P73" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="Q73" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="R73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="S73">
         <v>54</v>
       </c>
       <c r="T73" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
@@ -4925,7 +4927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>160</v>
       </c>
@@ -4981,7 +4983,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>188</v>
       </c>
@@ -5037,12 +5039,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B77" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
@@ -5060,15 +5062,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" t="s">
         <v>228</v>
-      </c>
-      <c r="B78" t="s">
-        <v>229</v>
-      </c>
-      <c r="C78" t="s">
-        <v>230</v>
       </c>
       <c r="F78" t="s">
         <v>20</v>
@@ -5089,34 +5091,34 @@
         <v>0</v>
       </c>
       <c r="L78" t="s">
+        <v>229</v>
+      </c>
+      <c r="M78" t="s">
+        <v>230</v>
+      </c>
+      <c r="N78" t="s">
         <v>231</v>
       </c>
-      <c r="M78" t="s">
+      <c r="O78" t="s">
+        <v>23</v>
+      </c>
+      <c r="P78" t="s">
         <v>232</v>
       </c>
-      <c r="N78" t="s">
+      <c r="Q78" t="s">
         <v>233</v>
       </c>
-      <c r="O78" t="s">
-        <v>23</v>
-      </c>
-      <c r="P78" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>235</v>
-      </c>
       <c r="R78" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="S78">
         <v>33</v>
       </c>
       <c r="T78" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>208</v>
       </c>
@@ -5124,7 +5126,7 @@
         <v>209</v>
       </c>
       <c r="C79" t="s">
-        <v>210</v>
+        <v>536</v>
       </c>
       <c r="F79" t="s">
         <v>20</v>
@@ -5145,22 +5147,22 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
+        <v>210</v>
+      </c>
+      <c r="M79" t="s">
         <v>211</v>
       </c>
-      <c r="M79" t="s">
+      <c r="N79" t="s">
+        <v>23</v>
+      </c>
+      <c r="O79" t="s">
+        <v>23</v>
+      </c>
+      <c r="P79" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q79" t="s">
         <v>212</v>
-      </c>
-      <c r="N79" t="s">
-        <v>23</v>
-      </c>
-      <c r="O79" t="s">
-        <v>23</v>
-      </c>
-      <c r="P79" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>214</v>
       </c>
       <c r="R79" t="s">
         <v>209</v>
@@ -5169,18 +5171,18 @@
         <v>30</v>
       </c>
       <c r="T79" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>241</v>
+      </c>
+      <c r="B80" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" t="s">
         <v>243</v>
-      </c>
-      <c r="B80" t="s">
-        <v>244</v>
-      </c>
-      <c r="C80" t="s">
-        <v>245</v>
       </c>
       <c r="F80" t="s">
         <v>50</v>
@@ -5201,34 +5203,34 @@
         <v>0</v>
       </c>
       <c r="L80" t="s">
+        <v>244</v>
+      </c>
+      <c r="M80" t="s">
+        <v>245</v>
+      </c>
+      <c r="N80" t="s">
+        <v>231</v>
+      </c>
+      <c r="O80" t="s">
+        <v>23</v>
+      </c>
+      <c r="P80" t="s">
         <v>246</v>
       </c>
-      <c r="M80" t="s">
+      <c r="Q80" t="s">
         <v>247</v>
       </c>
-      <c r="N80" t="s">
-        <v>233</v>
-      </c>
-      <c r="O80" t="s">
-        <v>23</v>
-      </c>
-      <c r="P80" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>249</v>
-      </c>
       <c r="R80" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S80">
         <v>35</v>
       </c>
       <c r="T80" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>167</v>
       </c>
@@ -5284,15 +5286,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>261</v>
+      </c>
+      <c r="B82" t="s">
+        <v>262</v>
+      </c>
+      <c r="C82" t="s">
         <v>263</v>
-      </c>
-      <c r="B82" t="s">
-        <v>264</v>
-      </c>
-      <c r="C82" t="s">
-        <v>265</v>
       </c>
       <c r="F82" t="s">
         <v>50</v>
@@ -5313,36 +5315,36 @@
         <v>0</v>
       </c>
       <c r="L82" t="s">
+        <v>264</v>
+      </c>
+      <c r="M82" t="s">
+        <v>265</v>
+      </c>
+      <c r="N82" t="s">
+        <v>23</v>
+      </c>
+      <c r="O82" t="s">
+        <v>23</v>
+      </c>
+      <c r="P82" t="s">
         <v>266</v>
       </c>
-      <c r="M82" t="s">
-        <v>267</v>
-      </c>
-      <c r="N82" t="s">
-        <v>23</v>
-      </c>
-      <c r="O82" t="s">
-        <v>23</v>
-      </c>
-      <c r="P82" t="s">
-        <v>268</v>
-      </c>
       <c r="Q82" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="R82" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="S82">
         <v>38</v>
       </c>
       <c r="T82" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B83" t="s">
         <v>154</v>
@@ -5396,15 +5398,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>214</v>
+      </c>
+      <c r="B84" t="s">
+        <v>215</v>
+      </c>
+      <c r="C84" t="s">
         <v>216</v>
-      </c>
-      <c r="B84" t="s">
-        <v>217</v>
-      </c>
-      <c r="C84" t="s">
-        <v>218</v>
       </c>
       <c r="F84" t="s">
         <v>20</v>
@@ -5425,39 +5427,39 @@
         <v>0</v>
       </c>
       <c r="L84" t="s">
+        <v>217</v>
+      </c>
+      <c r="M84" t="s">
+        <v>218</v>
+      </c>
+      <c r="N84" t="s">
         <v>219</v>
       </c>
-      <c r="M84" t="s">
+      <c r="O84" t="s">
+        <v>23</v>
+      </c>
+      <c r="P84" t="s">
         <v>220</v>
       </c>
-      <c r="N84" t="s">
+      <c r="Q84" t="s">
         <v>221</v>
       </c>
-      <c r="O84" t="s">
-        <v>23</v>
-      </c>
-      <c r="P84" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>223</v>
-      </c>
       <c r="R84" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S84">
         <v>31</v>
       </c>
       <c r="T84" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F85" t="s">
         <v>50</v>
@@ -5478,34 +5480,34 @@
         <v>0</v>
       </c>
       <c r="L85" t="s">
+        <v>237</v>
+      </c>
+      <c r="M85" t="s">
+        <v>238</v>
+      </c>
+      <c r="N85" t="s">
+        <v>231</v>
+      </c>
+      <c r="O85" t="s">
+        <v>23</v>
+      </c>
+      <c r="P85" t="s">
         <v>239</v>
       </c>
-      <c r="M85" t="s">
+      <c r="Q85" t="s">
         <v>240</v>
       </c>
-      <c r="N85" t="s">
-        <v>233</v>
-      </c>
-      <c r="O85" t="s">
-        <v>23</v>
-      </c>
-      <c r="P85" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>242</v>
-      </c>
       <c r="R85" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="S85">
         <v>34</v>
       </c>
       <c r="T85" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>194</v>
       </c>
@@ -5561,15 +5563,15 @@
         <v>187</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>248</v>
+      </c>
+      <c r="B87" t="s">
+        <v>249</v>
+      </c>
+      <c r="C87" t="s">
         <v>250</v>
-      </c>
-      <c r="B87" t="s">
-        <v>251</v>
-      </c>
-      <c r="C87" t="s">
-        <v>252</v>
       </c>
       <c r="F87" t="s">
         <v>50</v>
@@ -5590,34 +5592,34 @@
         <v>0</v>
       </c>
       <c r="L87" t="s">
+        <v>251</v>
+      </c>
+      <c r="M87" t="s">
+        <v>252</v>
+      </c>
+      <c r="N87" t="s">
+        <v>231</v>
+      </c>
+      <c r="O87" t="s">
+        <v>23</v>
+      </c>
+      <c r="P87" t="s">
         <v>253</v>
       </c>
-      <c r="M87" t="s">
+      <c r="Q87" t="s">
         <v>254</v>
       </c>
-      <c r="N87" t="s">
-        <v>233</v>
-      </c>
-      <c r="O87" t="s">
-        <v>23</v>
-      </c>
-      <c r="P87" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q87" t="s">
-        <v>256</v>
-      </c>
       <c r="R87" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="S87">
         <v>36</v>
       </c>
       <c r="T87" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -5673,9 +5675,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F89" t="s">
         <v>20</v>
@@ -5696,7 +5698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>181</v>
       </c>
@@ -5752,7 +5754,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>201</v>
       </c>
@@ -5763,7 +5765,7 @@
         <v>203</v>
       </c>
       <c r="E91" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F91" t="s">
         <v>20</v>
@@ -5811,12 +5813,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B92" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G92" t="b">
         <v>1</v>
@@ -5834,21 +5836,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B93" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D93" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E93" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F93" t="s">
         <v>50</v>
@@ -5869,34 +5871,34 @@
         <v>0</v>
       </c>
       <c r="L93" t="s">
+        <v>223</v>
+      </c>
+      <c r="M93" t="s">
+        <v>224</v>
+      </c>
+      <c r="N93" t="s">
+        <v>23</v>
+      </c>
+      <c r="O93" t="s">
+        <v>23</v>
+      </c>
+      <c r="P93" t="s">
         <v>225</v>
-      </c>
-      <c r="M93" t="s">
-        <v>226</v>
-      </c>
-      <c r="N93" t="s">
-        <v>23</v>
-      </c>
-      <c r="O93" t="s">
-        <v>23</v>
-      </c>
-      <c r="P93" t="s">
-        <v>227</v>
       </c>
       <c r="Q93" t="s">
         <v>139</v>
       </c>
       <c r="R93" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="S93">
         <v>32</v>
       </c>
       <c r="T93" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>140</v>
       </c>
@@ -5907,10 +5909,10 @@
         <v>142</v>
       </c>
       <c r="D94" t="s">
+        <v>522</v>
+      </c>
+      <c r="E94" t="s">
         <v>524</v>
-      </c>
-      <c r="E94" t="s">
-        <v>526</v>
       </c>
       <c r="F94" t="s">
         <v>50</v>
@@ -5958,7 +5960,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>118</v>
       </c>
@@ -5969,10 +5971,10 @@
         <v>120</v>
       </c>
       <c r="D95" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E95" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
@@ -6020,7 +6022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -6031,10 +6033,10 @@
         <v>49</v>
       </c>
       <c r="D96" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E96" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F96" t="s">
         <v>50</v>
@@ -6082,7 +6084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>61</v>
       </c>
@@ -6093,7 +6095,7 @@
         <v>63</v>
       </c>
       <c r="E97" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F97" t="s">
         <v>20</v>
@@ -6141,7 +6143,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>40</v>
       </c>
@@ -6152,7 +6154,7 @@
         <v>42</v>
       </c>
       <c r="E98" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F98" t="s">
         <v>20</v>
@@ -6200,7 +6202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -6208,13 +6210,13 @@
         <v>113</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D99" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E99" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F99" t="s">
         <v>50</v>
@@ -6262,122 +6264,122 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>507</v>
+      </c>
+      <c r="B100" t="s">
+        <v>494</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>1</v>
+      </c>
+      <c r="I100" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>508</v>
+      </c>
+      <c r="B101" t="s">
+        <v>495</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" t="b">
+        <v>1</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>509</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B102" t="s">
         <v>496</v>
       </c>
-      <c r="G100" t="b">
-        <v>0</v>
-      </c>
-      <c r="H100" t="b">
-        <v>1</v>
-      </c>
-      <c r="I100" t="b">
-        <v>0</v>
-      </c>
-      <c r="J100" t="b">
-        <v>0</v>
-      </c>
-      <c r="K100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" t="b">
+        <v>0</v>
+      </c>
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>497</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <v>1</v>
+      </c>
+      <c r="I103" t="b">
+        <v>0</v>
+      </c>
+      <c r="J103" t="b">
+        <v>0</v>
+      </c>
+      <c r="K103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>510</v>
       </c>
-      <c r="B101" t="s">
-        <v>497</v>
-      </c>
-      <c r="G101" t="b">
-        <v>0</v>
-      </c>
-      <c r="H101" t="b">
-        <v>1</v>
-      </c>
-      <c r="I101" t="b">
-        <v>0</v>
-      </c>
-      <c r="J101" t="b">
-        <v>0</v>
-      </c>
-      <c r="K101" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>511</v>
-      </c>
-      <c r="B102" t="s">
+      <c r="B104" t="s">
         <v>498</v>
       </c>
-      <c r="G102" t="b">
-        <v>0</v>
-      </c>
-      <c r="H102" t="b">
-        <v>1</v>
-      </c>
-      <c r="I102" t="b">
-        <v>0</v>
-      </c>
-      <c r="J102" t="b">
-        <v>0</v>
-      </c>
-      <c r="K102" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <v>1</v>
+      </c>
+      <c r="I104" t="b">
+        <v>0</v>
+      </c>
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
         <v>499</v>
       </c>
-      <c r="G103" t="b">
-        <v>0</v>
-      </c>
-      <c r="H103" t="b">
-        <v>1</v>
-      </c>
-      <c r="I103" t="b">
-        <v>0</v>
-      </c>
-      <c r="J103" t="b">
-        <v>0</v>
-      </c>
-      <c r="K103" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>512</v>
-      </c>
-      <c r="B104" t="s">
-        <v>500</v>
-      </c>
-      <c r="G104" t="b">
-        <v>0</v>
-      </c>
-      <c r="H104" t="b">
-        <v>1</v>
-      </c>
-      <c r="I104" t="b">
-        <v>0</v>
-      </c>
-      <c r="J104" t="b">
-        <v>0</v>
-      </c>
-      <c r="K104" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>501</v>
-      </c>
       <c r="G105" t="b">
         <v>0</v>
       </c>
@@ -6394,7 +6396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -6405,10 +6407,10 @@
         <v>99</v>
       </c>
       <c r="D106" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E106" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F106" t="s">
         <v>20</v>
@@ -6456,7 +6458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>108</v>
       </c>
@@ -6509,7 +6511,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>104</v>
       </c>
@@ -6562,7 +6564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>134</v>
       </c>
@@ -6573,10 +6575,10 @@
         <v>135</v>
       </c>
       <c r="D109" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E109" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F109" t="s">
         <v>50</v>
@@ -6624,7 +6626,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>55</v>
       </c>
@@ -6632,10 +6634,10 @@
         <v>56</v>
       </c>
       <c r="C110" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E110" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F110" t="s">
         <v>20</v>
@@ -6683,7 +6685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>34</v>
       </c>
@@ -6691,11 +6693,11 @@
         <v>35</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F111" t="s">
         <v>20</v>
@@ -6743,7 +6745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -6754,10 +6756,10 @@
         <v>128</v>
       </c>
       <c r="D112" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E112" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F112" t="s">
         <v>50</v>
@@ -6805,7 +6807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>75</v>
       </c>
@@ -6816,10 +6818,10 @@
         <v>77</v>
       </c>
       <c r="D113" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E113" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F113" t="s">
         <v>20</v>
@@ -6867,7 +6869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -6875,11 +6877,11 @@
         <v>19</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F114" t="s">
         <v>20</v>
@@ -6927,7 +6929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>68</v>
       </c>
@@ -6938,10 +6940,10 @@
         <v>70</v>
       </c>
       <c r="D115" t="s">
+        <v>516</v>
+      </c>
+      <c r="E115" t="s">
         <v>518</v>
-      </c>
-      <c r="E115" t="s">
-        <v>520</v>
       </c>
       <c r="F115" t="s">
         <v>20</v>
@@ -6989,7 +6991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>147</v>
       </c>
@@ -7000,7 +7002,7 @@
         <v>149</v>
       </c>
       <c r="E116" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F116" t="s">
         <v>50</v>
@@ -7048,7 +7050,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -7059,7 +7061,7 @@
         <v>29</v>
       </c>
       <c r="E117" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F117" t="s">
         <v>20</v>
@@ -7107,7 +7109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -7118,10 +7120,10 @@
         <v>85</v>
       </c>
       <c r="D118" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E118" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F118" t="s">
         <v>20</v>
@@ -7169,7 +7171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>94</v>
       </c>
@@ -7222,7 +7224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Revert "Changed GHO code for blood pressure to "Prevalence of hypertension (defined as having systolic blood pressure ≥140 mmHg, diastolic blood pressure ≥90 mmHg, or taking medication for hypertension) among adults aged 30-79.""
This reverts commit ec1a876732ae6d4db528d4c90e8b307469c22d61.

The change to `indicator_df` was made via the excel file, and exported to the .csv. This is the incorrect workflow, as it introduced additional changes. The .csv files should be edited directly.
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vasa/who/3b/billionaiRe/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/robsona_who_int/Documents/Alice/Rwork/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BBEAAE-6B10-C441-85A1-E977C41429A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{6693E9E6-59D4-4F88-8AE0-7E1493FEE32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{449B8437-A255-483D-BF8C-5C210A66CE0E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27645" yWindow="1380" windowWidth="26085" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,12 +652,18 @@
     <t>bp</t>
   </si>
   <si>
+    <t>BP_04</t>
+  </si>
+  <si>
     <t>SDG 3.8.1.9</t>
   </si>
   <si>
     <t>Prevention of cardiovascular disease</t>
   </si>
   <si>
+    <t>Prevalence of raised blood pressure*</t>
+  </si>
+  <si>
     <t>Non-elevated blood pressure</t>
   </si>
   <si>
@@ -1628,12 +1634,6 @@
   </si>
   <si>
     <t>GINA - TFA Country Score Card</t>
-  </si>
-  <si>
-    <t>NCD_HYP_TREATMENT_A</t>
-  </si>
-  <si>
-    <t>Prevalence of hypertension (defined as having systolic blood pressure ≥140 mmHg, diastolic blood pressure ≥90 mmHg, or taking medication for hypertension) among adults aged 30-79.</t>
   </si>
 </sst>
 </file>
@@ -2036,20 +2036,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C72" workbookViewId="0">
-      <selection activeCell="Q79" sqref="Q79"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="27.5" customWidth="1"/>
-    <col min="16" max="16" width="34.33203125" customWidth="1"/>
-    <col min="17" max="17" width="42.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2060,10 +2058,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2111,15 +2109,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -2140,39 +2138,39 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M2" t="s">
+        <v>260</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>262</v>
+      </c>
+      <c r="R2" t="s">
         <v>257</v>
-      </c>
-      <c r="M2" t="s">
-        <v>258</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>260</v>
-      </c>
-      <c r="R2" t="s">
-        <v>255</v>
       </c>
       <c r="S2">
         <v>37</v>
       </c>
       <c r="T2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B3" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2190,9 +2188,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F4" t="s">
         <v>50</v>
@@ -2213,39 +2211,39 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="M4" t="s">
+        <v>369</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>369</v>
+      </c>
+      <c r="R4" t="s">
         <v>367</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>367</v>
-      </c>
-      <c r="R4" t="s">
-        <v>365</v>
       </c>
       <c r="S4">
         <v>58</v>
       </c>
       <c r="T4" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B5" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -2266,12 +2264,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B6" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F6" t="s">
         <v>50</v>
@@ -2292,9 +2290,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -2312,9 +2310,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -2332,9 +2330,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -2352,9 +2350,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -2372,12 +2370,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B11" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -2398,39 +2396,39 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="M11" t="s">
+        <v>376</v>
+      </c>
+      <c r="N11" t="s">
+        <v>377</v>
+      </c>
+      <c r="O11" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>376</v>
+      </c>
+      <c r="R11" t="s">
         <v>374</v>
-      </c>
-      <c r="N11" t="s">
-        <v>375</v>
-      </c>
-      <c r="O11" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>374</v>
-      </c>
-      <c r="R11" t="s">
-        <v>372</v>
       </c>
       <c r="S11">
         <v>60</v>
       </c>
       <c r="T11" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B12" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -2451,36 +2449,36 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="M12" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="N12" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="O12" t="s">
         <v>23</v>
       </c>
       <c r="P12" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="Q12" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="R12" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="S12">
         <v>63</v>
       </c>
       <c r="T12" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -2498,9 +2496,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -2518,9 +2516,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -2538,9 +2536,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -2558,15 +2556,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B17" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C17" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -2587,36 +2585,36 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
+        <v>273</v>
+      </c>
+      <c r="M17" t="s">
+        <v>274</v>
+      </c>
+      <c r="N17" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>274</v>
+      </c>
+      <c r="R17" t="s">
         <v>271</v>
-      </c>
-      <c r="M17" t="s">
-        <v>272</v>
-      </c>
-      <c r="N17" t="s">
-        <v>23</v>
-      </c>
-      <c r="O17" t="s">
-        <v>23</v>
-      </c>
-      <c r="P17" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>272</v>
-      </c>
-      <c r="R17" t="s">
-        <v>269</v>
       </c>
       <c r="S17">
         <v>39</v>
       </c>
       <c r="T17" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
@@ -2637,7 +2635,7 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="N18" t="s">
         <v>23</v>
@@ -2646,18 +2644,18 @@
         <v>23</v>
       </c>
       <c r="P18" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>397</v>
+      </c>
+      <c r="R18" t="s">
         <v>394</v>
       </c>
-      <c r="Q18" t="s">
-        <v>395</v>
-      </c>
-      <c r="R18" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
@@ -2678,7 +2676,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="N19" t="s">
         <v>23</v>
@@ -2687,18 +2685,18 @@
         <v>23</v>
       </c>
       <c r="P19" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>401</v>
+      </c>
+      <c r="R19" t="s">
         <v>398</v>
       </c>
-      <c r="Q19" t="s">
-        <v>399</v>
-      </c>
-      <c r="R19" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
@@ -2719,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="N20" t="s">
         <v>23</v>
@@ -2728,24 +2726,24 @@
         <v>23</v>
       </c>
       <c r="P20" t="s">
+        <v>404</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>405</v>
+      </c>
+      <c r="R20" t="s">
         <v>402</v>
       </c>
-      <c r="Q20" t="s">
-        <v>403</v>
-      </c>
-      <c r="R20" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B21" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C21" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
@@ -2766,36 +2764,36 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
+        <v>279</v>
+      </c>
+      <c r="M21" t="s">
+        <v>280</v>
+      </c>
+      <c r="N21" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>280</v>
+      </c>
+      <c r="R21" t="s">
         <v>277</v>
-      </c>
-      <c r="M21" t="s">
-        <v>278</v>
-      </c>
-      <c r="N21" t="s">
-        <v>23</v>
-      </c>
-      <c r="O21" t="s">
-        <v>23</v>
-      </c>
-      <c r="P21" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>278</v>
-      </c>
-      <c r="R21" t="s">
-        <v>275</v>
       </c>
       <c r="S21">
         <v>40</v>
       </c>
       <c r="T21" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -2816,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="N22" t="s">
         <v>23</v>
@@ -2825,21 +2823,21 @@
         <v>23</v>
       </c>
       <c r="P22" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>409</v>
+      </c>
+      <c r="R22" t="s">
         <v>406</v>
       </c>
-      <c r="Q22" t="s">
-        <v>407</v>
-      </c>
-      <c r="R22" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C23" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
@@ -2860,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="N23" t="s">
         <v>23</v>
@@ -2869,24 +2867,24 @@
         <v>23</v>
       </c>
       <c r="P23" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>412</v>
+      </c>
+      <c r="R23" t="s">
         <v>410</v>
       </c>
-      <c r="Q23" t="s">
-        <v>410</v>
-      </c>
-      <c r="R23" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B24" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C24" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
@@ -2907,42 +2905,42 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
+        <v>285</v>
+      </c>
+      <c r="M24" t="s">
+        <v>286</v>
+      </c>
+      <c r="N24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>286</v>
+      </c>
+      <c r="R24" t="s">
         <v>283</v>
-      </c>
-      <c r="M24" t="s">
-        <v>284</v>
-      </c>
-      <c r="N24" t="s">
-        <v>23</v>
-      </c>
-      <c r="O24" t="s">
-        <v>23</v>
-      </c>
-      <c r="P24" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>284</v>
-      </c>
-      <c r="R24" t="s">
-        <v>281</v>
       </c>
       <c r="S24">
         <v>41</v>
       </c>
       <c r="T24" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B25" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C25" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
@@ -2963,42 +2961,42 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
+        <v>291</v>
+      </c>
+      <c r="M25" t="s">
+        <v>292</v>
+      </c>
+      <c r="N25" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>292</v>
+      </c>
+      <c r="R25" t="s">
         <v>289</v>
-      </c>
-      <c r="M25" t="s">
-        <v>290</v>
-      </c>
-      <c r="N25" t="s">
-        <v>23</v>
-      </c>
-      <c r="O25" t="s">
-        <v>23</v>
-      </c>
-      <c r="P25" t="s">
-        <v>290</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>290</v>
-      </c>
-      <c r="R25" t="s">
-        <v>287</v>
       </c>
       <c r="S25">
         <v>42</v>
       </c>
       <c r="T25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B26" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C26" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F26" t="s">
         <v>20</v>
@@ -3019,36 +3017,36 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
+        <v>296</v>
+      </c>
+      <c r="M26" t="s">
+        <v>297</v>
+      </c>
+      <c r="N26" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>297</v>
+      </c>
+      <c r="R26" t="s">
         <v>294</v>
-      </c>
-      <c r="M26" t="s">
-        <v>295</v>
-      </c>
-      <c r="N26" t="s">
-        <v>23</v>
-      </c>
-      <c r="O26" t="s">
-        <v>23</v>
-      </c>
-      <c r="P26" t="s">
-        <v>295</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>295</v>
-      </c>
-      <c r="R26" t="s">
-        <v>292</v>
       </c>
       <c r="S26">
         <v>43</v>
       </c>
       <c r="T26" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
@@ -3069,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="N27" t="s">
         <v>23</v>
@@ -3078,18 +3076,18 @@
         <v>23</v>
       </c>
       <c r="P27" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>415</v>
+      </c>
+      <c r="R27" t="s">
         <v>413</v>
       </c>
-      <c r="Q27" t="s">
-        <v>413</v>
-      </c>
-      <c r="R27" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="F28" t="s">
         <v>20</v>
@@ -3110,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="N28" t="s">
         <v>23</v>
@@ -3119,18 +3117,18 @@
         <v>23</v>
       </c>
       <c r="P28" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>419</v>
+      </c>
+      <c r="R28" t="s">
         <v>416</v>
       </c>
-      <c r="Q28" t="s">
-        <v>417</v>
-      </c>
-      <c r="R28" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
@@ -3151,7 +3149,7 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="N29" t="s">
         <v>23</v>
@@ -3160,24 +3158,24 @@
         <v>23</v>
       </c>
       <c r="P29" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>423</v>
+      </c>
+      <c r="R29" t="s">
         <v>420</v>
       </c>
-      <c r="Q29" t="s">
-        <v>421</v>
-      </c>
-      <c r="R29" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B30" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C30" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F30" t="s">
         <v>20</v>
@@ -3198,36 +3196,36 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
+        <v>301</v>
+      </c>
+      <c r="M30" t="s">
+        <v>302</v>
+      </c>
+      <c r="N30" t="s">
+        <v>23</v>
+      </c>
+      <c r="O30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P30" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>302</v>
+      </c>
+      <c r="R30" t="s">
         <v>299</v>
-      </c>
-      <c r="M30" t="s">
-        <v>300</v>
-      </c>
-      <c r="N30" t="s">
-        <v>23</v>
-      </c>
-      <c r="O30" t="s">
-        <v>23</v>
-      </c>
-      <c r="P30" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>300</v>
-      </c>
-      <c r="R30" t="s">
-        <v>297</v>
       </c>
       <c r="S30">
         <v>44</v>
       </c>
       <c r="T30" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
@@ -3248,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="N31" t="s">
         <v>23</v>
@@ -3257,18 +3255,18 @@
         <v>23</v>
       </c>
       <c r="P31" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>427</v>
+      </c>
+      <c r="R31" t="s">
         <v>424</v>
       </c>
-      <c r="Q31" t="s">
-        <v>425</v>
-      </c>
-      <c r="R31" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
@@ -3289,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="N32" t="s">
         <v>23</v>
@@ -3298,24 +3296,24 @@
         <v>23</v>
       </c>
       <c r="P32" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>431</v>
+      </c>
+      <c r="R32" t="s">
         <v>428</v>
       </c>
-      <c r="Q32" t="s">
-        <v>429</v>
-      </c>
-      <c r="R32" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B33" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C33" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
@@ -3336,42 +3334,42 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
+        <v>306</v>
+      </c>
+      <c r="M33" t="s">
+        <v>307</v>
+      </c>
+      <c r="N33" t="s">
+        <v>23</v>
+      </c>
+      <c r="O33" t="s">
+        <v>23</v>
+      </c>
+      <c r="P33" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>307</v>
+      </c>
+      <c r="R33" t="s">
         <v>304</v>
-      </c>
-      <c r="M33" t="s">
-        <v>305</v>
-      </c>
-      <c r="N33" t="s">
-        <v>23</v>
-      </c>
-      <c r="O33" t="s">
-        <v>23</v>
-      </c>
-      <c r="P33" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>305</v>
-      </c>
-      <c r="R33" t="s">
-        <v>302</v>
       </c>
       <c r="S33">
         <v>45</v>
       </c>
       <c r="T33" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B34" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C34" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
@@ -3392,36 +3390,36 @@
         <v>0</v>
       </c>
       <c r="L34" t="s">
+        <v>311</v>
+      </c>
+      <c r="M34" t="s">
+        <v>312</v>
+      </c>
+      <c r="N34" t="s">
+        <v>23</v>
+      </c>
+      <c r="O34" t="s">
+        <v>23</v>
+      </c>
+      <c r="P34" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>312</v>
+      </c>
+      <c r="R34" t="s">
         <v>309</v>
-      </c>
-      <c r="M34" t="s">
-        <v>310</v>
-      </c>
-      <c r="N34" t="s">
-        <v>23</v>
-      </c>
-      <c r="O34" t="s">
-        <v>23</v>
-      </c>
-      <c r="P34" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>310</v>
-      </c>
-      <c r="R34" t="s">
-        <v>307</v>
       </c>
       <c r="S34">
         <v>46</v>
       </c>
       <c r="T34" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="F35" t="s">
         <v>20</v>
@@ -3442,7 +3440,7 @@
         <v>0</v>
       </c>
       <c r="L35" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="N35" t="s">
         <v>23</v>
@@ -3451,18 +3449,18 @@
         <v>23</v>
       </c>
       <c r="P35" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>435</v>
+      </c>
+      <c r="R35" t="s">
         <v>432</v>
       </c>
-      <c r="Q35" t="s">
-        <v>433</v>
-      </c>
-      <c r="R35" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
@@ -3483,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="L36" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="N36" t="s">
         <v>23</v>
@@ -3492,21 +3490,21 @@
         <v>23</v>
       </c>
       <c r="P36" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>438</v>
+      </c>
+      <c r="R36" t="s">
         <v>436</v>
       </c>
-      <c r="Q36" t="s">
-        <v>436</v>
-      </c>
-      <c r="R36" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B37" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F37" t="s">
         <v>20</v>
@@ -3527,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="L37" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N37" t="s">
         <v>23</v>
@@ -3536,24 +3534,24 @@
         <v>23</v>
       </c>
       <c r="P37" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>441</v>
+      </c>
+      <c r="R37" t="s">
         <v>439</v>
       </c>
-      <c r="Q37" t="s">
-        <v>439</v>
-      </c>
-      <c r="R37" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B38" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C38" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F38" t="s">
         <v>20</v>
@@ -3574,36 +3572,36 @@
         <v>0</v>
       </c>
       <c r="L38" t="s">
+        <v>316</v>
+      </c>
+      <c r="M38" t="s">
+        <v>317</v>
+      </c>
+      <c r="N38" t="s">
+        <v>23</v>
+      </c>
+      <c r="O38" t="s">
+        <v>23</v>
+      </c>
+      <c r="P38" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>317</v>
+      </c>
+      <c r="R38" t="s">
         <v>314</v>
-      </c>
-      <c r="M38" t="s">
-        <v>315</v>
-      </c>
-      <c r="N38" t="s">
-        <v>23</v>
-      </c>
-      <c r="O38" t="s">
-        <v>23</v>
-      </c>
-      <c r="P38" t="s">
-        <v>315</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>315</v>
-      </c>
-      <c r="R38" t="s">
-        <v>312</v>
       </c>
       <c r="S38">
         <v>47</v>
       </c>
       <c r="T38" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
@@ -3624,7 +3622,7 @@
         <v>0</v>
       </c>
       <c r="L39" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N39" t="s">
         <v>23</v>
@@ -3633,18 +3631,18 @@
         <v>23</v>
       </c>
       <c r="P39" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>445</v>
+      </c>
+      <c r="R39" t="s">
         <v>442</v>
       </c>
-      <c r="Q39" t="s">
-        <v>443</v>
-      </c>
-      <c r="R39" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="F40" t="s">
         <v>20</v>
@@ -3665,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="L40" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="N40" t="s">
         <v>23</v>
@@ -3674,18 +3672,18 @@
         <v>23</v>
       </c>
       <c r="P40" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>449</v>
+      </c>
+      <c r="R40" t="s">
         <v>446</v>
       </c>
-      <c r="Q40" t="s">
-        <v>447</v>
-      </c>
-      <c r="R40" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
@@ -3706,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="L41" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="N41" t="s">
         <v>23</v>
@@ -3715,24 +3713,24 @@
         <v>23</v>
       </c>
       <c r="P41" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>453</v>
+      </c>
+      <c r="R41" t="s">
         <v>450</v>
       </c>
-      <c r="Q41" t="s">
-        <v>451</v>
-      </c>
-      <c r="R41" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B42" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C42" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F42" t="s">
         <v>20</v>
@@ -3753,42 +3751,42 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
+        <v>321</v>
+      </c>
+      <c r="M42" t="s">
+        <v>322</v>
+      </c>
+      <c r="N42" t="s">
+        <v>23</v>
+      </c>
+      <c r="O42" t="s">
+        <v>23</v>
+      </c>
+      <c r="P42" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>322</v>
+      </c>
+      <c r="R42" t="s">
         <v>319</v>
-      </c>
-      <c r="M42" t="s">
-        <v>320</v>
-      </c>
-      <c r="N42" t="s">
-        <v>23</v>
-      </c>
-      <c r="O42" t="s">
-        <v>23</v>
-      </c>
-      <c r="P42" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>320</v>
-      </c>
-      <c r="R42" t="s">
-        <v>317</v>
       </c>
       <c r="S42">
         <v>48</v>
       </c>
       <c r="T42" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B43" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C43" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F43" t="s">
         <v>20</v>
@@ -3809,36 +3807,36 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
+        <v>326</v>
+      </c>
+      <c r="M43" t="s">
+        <v>327</v>
+      </c>
+      <c r="N43" t="s">
+        <v>23</v>
+      </c>
+      <c r="O43" t="s">
+        <v>23</v>
+      </c>
+      <c r="P43" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>327</v>
+      </c>
+      <c r="R43" t="s">
         <v>324</v>
-      </c>
-      <c r="M43" t="s">
-        <v>325</v>
-      </c>
-      <c r="N43" t="s">
-        <v>23</v>
-      </c>
-      <c r="O43" t="s">
-        <v>23</v>
-      </c>
-      <c r="P43" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>325</v>
-      </c>
-      <c r="R43" t="s">
-        <v>322</v>
       </c>
       <c r="S43">
         <v>49</v>
       </c>
       <c r="T43" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
@@ -3859,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="L44" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="N44" t="s">
         <v>23</v>
@@ -3868,18 +3866,18 @@
         <v>23</v>
       </c>
       <c r="P44" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>457</v>
+      </c>
+      <c r="R44" t="s">
         <v>454</v>
       </c>
-      <c r="Q44" t="s">
-        <v>455</v>
-      </c>
-      <c r="R44" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
@@ -3900,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="L45" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="N45" t="s">
         <v>23</v>
@@ -3909,24 +3907,24 @@
         <v>23</v>
       </c>
       <c r="P45" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>461</v>
+      </c>
+      <c r="R45" t="s">
         <v>458</v>
       </c>
-      <c r="Q45" t="s">
-        <v>459</v>
-      </c>
-      <c r="R45" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B46" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C46" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
@@ -3947,42 +3945,42 @@
         <v>0</v>
       </c>
       <c r="L46" t="s">
+        <v>331</v>
+      </c>
+      <c r="M46" t="s">
+        <v>332</v>
+      </c>
+      <c r="N46" t="s">
+        <v>23</v>
+      </c>
+      <c r="O46" t="s">
+        <v>23</v>
+      </c>
+      <c r="P46" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>332</v>
+      </c>
+      <c r="R46" t="s">
         <v>329</v>
-      </c>
-      <c r="M46" t="s">
-        <v>330</v>
-      </c>
-      <c r="N46" t="s">
-        <v>23</v>
-      </c>
-      <c r="O46" t="s">
-        <v>23</v>
-      </c>
-      <c r="P46" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>330</v>
-      </c>
-      <c r="R46" t="s">
-        <v>327</v>
       </c>
       <c r="S46">
         <v>50</v>
       </c>
       <c r="T46" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B47" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C47" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
@@ -4003,39 +4001,39 @@
         <v>0</v>
       </c>
       <c r="L47" t="s">
+        <v>336</v>
+      </c>
+      <c r="M47" t="s">
+        <v>337</v>
+      </c>
+      <c r="N47" t="s">
+        <v>23</v>
+      </c>
+      <c r="O47" t="s">
+        <v>23</v>
+      </c>
+      <c r="P47" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>337</v>
+      </c>
+      <c r="R47" t="s">
         <v>334</v>
-      </c>
-      <c r="M47" t="s">
-        <v>335</v>
-      </c>
-      <c r="N47" t="s">
-        <v>23</v>
-      </c>
-      <c r="O47" t="s">
-        <v>23</v>
-      </c>
-      <c r="P47" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>335</v>
-      </c>
-      <c r="R47" t="s">
-        <v>332</v>
       </c>
       <c r="S47">
         <v>51</v>
       </c>
       <c r="T47" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B48" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
@@ -4053,10 +4051,10 @@
         <v>1</v>
       </c>
       <c r="L48" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="M48" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="N48" t="s">
         <v>23</v>
@@ -4065,13 +4063,13 @@
         <v>23</v>
       </c>
       <c r="P48" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>393</v>
+      </c>
+      <c r="R48" t="s">
         <v>391</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>391</v>
-      </c>
-      <c r="R48" t="s">
-        <v>389</v>
       </c>
       <c r="S48">
         <v>64</v>
@@ -4080,12 +4078,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B49" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -4103,9 +4101,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
@@ -4123,9 +4121,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
@@ -4143,9 +4141,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
@@ -4163,9 +4161,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
@@ -4183,15 +4181,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B54" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C54" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
@@ -4212,36 +4210,36 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
+        <v>347</v>
+      </c>
+      <c r="M54" t="s">
+        <v>348</v>
+      </c>
+      <c r="N54" t="s">
+        <v>23</v>
+      </c>
+      <c r="O54" t="s">
+        <v>23</v>
+      </c>
+      <c r="P54" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>348</v>
+      </c>
+      <c r="R54" t="s">
         <v>345</v>
-      </c>
-      <c r="M54" t="s">
-        <v>346</v>
-      </c>
-      <c r="N54" t="s">
-        <v>23</v>
-      </c>
-      <c r="O54" t="s">
-        <v>23</v>
-      </c>
-      <c r="P54" t="s">
-        <v>347</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>346</v>
-      </c>
-      <c r="R54" t="s">
-        <v>343</v>
       </c>
       <c r="S54">
         <v>53</v>
       </c>
       <c r="T54" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -4259,9 +4257,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G56" t="b">
         <v>0</v>
@@ -4279,9 +4277,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F57" t="s">
         <v>50</v>
@@ -4302,39 +4300,39 @@
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="M57" t="s">
+        <v>365</v>
+      </c>
+      <c r="N57" t="s">
+        <v>23</v>
+      </c>
+      <c r="O57" t="s">
+        <v>23</v>
+      </c>
+      <c r="P57" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>365</v>
+      </c>
+      <c r="R57" t="s">
         <v>363</v>
-      </c>
-      <c r="N57" t="s">
-        <v>23</v>
-      </c>
-      <c r="O57" t="s">
-        <v>23</v>
-      </c>
-      <c r="P57" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>363</v>
-      </c>
-      <c r="R57" t="s">
-        <v>361</v>
       </c>
       <c r="S57">
         <v>57</v>
       </c>
       <c r="T57" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B58" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F58" t="s">
         <v>50</v>
@@ -4355,12 +4353,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B59" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="F59" t="s">
         <v>50</v>
@@ -4381,12 +4379,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B60" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="F60" t="s">
         <v>20</v>
@@ -4407,36 +4405,36 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="M60" t="s">
+        <v>361</v>
+      </c>
+      <c r="N60" t="s">
+        <v>23</v>
+      </c>
+      <c r="O60" t="s">
+        <v>23</v>
+      </c>
+      <c r="P60" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>361</v>
+      </c>
+      <c r="R60" t="s">
         <v>359</v>
-      </c>
-      <c r="N60" t="s">
-        <v>23</v>
-      </c>
-      <c r="O60" t="s">
-        <v>23</v>
-      </c>
-      <c r="P60" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>359</v>
-      </c>
-      <c r="R60" t="s">
-        <v>357</v>
       </c>
       <c r="S60">
         <v>56</v>
       </c>
       <c r="T60" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="G61" t="b">
         <v>0</v>
@@ -4454,12 +4452,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B62" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F62" t="s">
         <v>20</v>
@@ -4480,36 +4478,36 @@
         <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="M62" t="s">
+        <v>382</v>
+      </c>
+      <c r="N62" t="s">
+        <v>377</v>
+      </c>
+      <c r="O62" t="s">
+        <v>23</v>
+      </c>
+      <c r="P62" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>382</v>
+      </c>
+      <c r="R62" t="s">
         <v>380</v>
-      </c>
-      <c r="N62" t="s">
-        <v>375</v>
-      </c>
-      <c r="O62" t="s">
-        <v>23</v>
-      </c>
-      <c r="P62" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>380</v>
-      </c>
-      <c r="R62" t="s">
-        <v>378</v>
       </c>
       <c r="S62">
         <v>61</v>
       </c>
       <c r="T62" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -4527,15 +4525,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B64" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C64" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F64" t="s">
         <v>20</v>
@@ -4556,36 +4554,36 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
+        <v>341</v>
+      </c>
+      <c r="M64" t="s">
+        <v>342</v>
+      </c>
+      <c r="N64" t="s">
+        <v>23</v>
+      </c>
+      <c r="O64" t="s">
+        <v>23</v>
+      </c>
+      <c r="P64" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>342</v>
+      </c>
+      <c r="R64" t="s">
         <v>339</v>
-      </c>
-      <c r="M64" t="s">
-        <v>340</v>
-      </c>
-      <c r="N64" t="s">
-        <v>23</v>
-      </c>
-      <c r="O64" t="s">
-        <v>23</v>
-      </c>
-      <c r="P64" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>340</v>
-      </c>
-      <c r="R64" t="s">
-        <v>337</v>
       </c>
       <c r="S64">
         <v>52</v>
       </c>
       <c r="T64" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -4603,12 +4601,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B66" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
@@ -4626,10 +4624,10 @@
         <v>1</v>
       </c>
       <c r="L66" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="M66" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="N66" t="s">
         <v>23</v>
@@ -4638,27 +4636,27 @@
         <v>23</v>
       </c>
       <c r="P66" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="Q66" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="R66" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="S66">
         <v>59</v>
       </c>
       <c r="T66" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B67" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F67" t="s">
         <v>20</v>
@@ -4679,39 +4677,39 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="M67" t="s">
+        <v>386</v>
+      </c>
+      <c r="N67" t="s">
+        <v>377</v>
+      </c>
+      <c r="O67" t="s">
+        <v>23</v>
+      </c>
+      <c r="P67" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>386</v>
+      </c>
+      <c r="R67" t="s">
         <v>384</v>
-      </c>
-      <c r="N67" t="s">
-        <v>375</v>
-      </c>
-      <c r="O67" t="s">
-        <v>23</v>
-      </c>
-      <c r="P67" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>384</v>
-      </c>
-      <c r="R67" t="s">
-        <v>382</v>
       </c>
       <c r="S67">
         <v>62</v>
       </c>
       <c r="T67" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B68" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="F68" t="s">
         <v>50</v>
@@ -4732,9 +4730,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
@@ -4752,9 +4750,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F70" t="s">
         <v>50</v>
@@ -4775,39 +4773,39 @@
         <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="M70" t="s">
+        <v>357</v>
+      </c>
+      <c r="N70" t="s">
+        <v>23</v>
+      </c>
+      <c r="O70" t="s">
+        <v>23</v>
+      </c>
+      <c r="P70" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>357</v>
+      </c>
+      <c r="R70" t="s">
         <v>355</v>
-      </c>
-      <c r="N70" t="s">
-        <v>23</v>
-      </c>
-      <c r="O70" t="s">
-        <v>23</v>
-      </c>
-      <c r="P70" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>355</v>
-      </c>
-      <c r="R70" t="s">
-        <v>353</v>
       </c>
       <c r="S70">
         <v>55</v>
       </c>
       <c r="T70" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B71" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="F71" t="s">
         <v>50</v>
@@ -4828,12 +4826,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B72" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F72" t="s">
         <v>50</v>
@@ -4854,12 +4852,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B73" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F73" t="s">
         <v>20</v>
@@ -4880,36 +4878,36 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M73" t="s">
+        <v>353</v>
+      </c>
+      <c r="N73" t="s">
+        <v>23</v>
+      </c>
+      <c r="O73" t="s">
+        <v>23</v>
+      </c>
+      <c r="P73" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>353</v>
+      </c>
+      <c r="R73" t="s">
         <v>351</v>
-      </c>
-      <c r="N73" t="s">
-        <v>23</v>
-      </c>
-      <c r="O73" t="s">
-        <v>23</v>
-      </c>
-      <c r="P73" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>351</v>
-      </c>
-      <c r="R73" t="s">
-        <v>349</v>
       </c>
       <c r="S73">
         <v>54</v>
       </c>
       <c r="T73" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
@@ -4927,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>160</v>
       </c>
@@ -4983,7 +4981,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>188</v>
       </c>
@@ -5039,12 +5037,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B77" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
@@ -5062,15 +5060,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B78" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C78" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F78" t="s">
         <v>20</v>
@@ -5091,34 +5089,34 @@
         <v>0</v>
       </c>
       <c r="L78" t="s">
+        <v>231</v>
+      </c>
+      <c r="M78" t="s">
+        <v>232</v>
+      </c>
+      <c r="N78" t="s">
+        <v>233</v>
+      </c>
+      <c r="O78" t="s">
+        <v>23</v>
+      </c>
+      <c r="P78" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>235</v>
+      </c>
+      <c r="R78" t="s">
         <v>229</v>
-      </c>
-      <c r="M78" t="s">
-        <v>230</v>
-      </c>
-      <c r="N78" t="s">
-        <v>231</v>
-      </c>
-      <c r="O78" t="s">
-        <v>23</v>
-      </c>
-      <c r="P78" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>233</v>
-      </c>
-      <c r="R78" t="s">
-        <v>227</v>
       </c>
       <c r="S78">
         <v>33</v>
       </c>
       <c r="T78" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>208</v>
       </c>
@@ -5126,7 +5124,7 @@
         <v>209</v>
       </c>
       <c r="C79" t="s">
-        <v>536</v>
+        <v>210</v>
       </c>
       <c r="F79" t="s">
         <v>20</v>
@@ -5147,10 +5145,10 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M79" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N79" t="s">
         <v>23</v>
@@ -5159,10 +5157,10 @@
         <v>23</v>
       </c>
       <c r="P79" t="s">
-        <v>537</v>
+        <v>213</v>
       </c>
       <c r="Q79" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="R79" t="s">
         <v>209</v>
@@ -5171,18 +5169,18 @@
         <v>30</v>
       </c>
       <c r="T79" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B80" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C80" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F80" t="s">
         <v>50</v>
@@ -5203,34 +5201,34 @@
         <v>0</v>
       </c>
       <c r="L80" t="s">
+        <v>246</v>
+      </c>
+      <c r="M80" t="s">
+        <v>247</v>
+      </c>
+      <c r="N80" t="s">
+        <v>233</v>
+      </c>
+      <c r="O80" t="s">
+        <v>23</v>
+      </c>
+      <c r="P80" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>249</v>
+      </c>
+      <c r="R80" t="s">
         <v>244</v>
-      </c>
-      <c r="M80" t="s">
-        <v>245</v>
-      </c>
-      <c r="N80" t="s">
-        <v>231</v>
-      </c>
-      <c r="O80" t="s">
-        <v>23</v>
-      </c>
-      <c r="P80" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>247</v>
-      </c>
-      <c r="R80" t="s">
-        <v>242</v>
       </c>
       <c r="S80">
         <v>35</v>
       </c>
       <c r="T80" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>167</v>
       </c>
@@ -5286,15 +5284,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B82" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C82" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F82" t="s">
         <v>50</v>
@@ -5315,36 +5313,36 @@
         <v>0</v>
       </c>
       <c r="L82" t="s">
+        <v>266</v>
+      </c>
+      <c r="M82" t="s">
+        <v>267</v>
+      </c>
+      <c r="N82" t="s">
+        <v>23</v>
+      </c>
+      <c r="O82" t="s">
+        <v>23</v>
+      </c>
+      <c r="P82" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>267</v>
+      </c>
+      <c r="R82" t="s">
         <v>264</v>
-      </c>
-      <c r="M82" t="s">
-        <v>265</v>
-      </c>
-      <c r="N82" t="s">
-        <v>23</v>
-      </c>
-      <c r="O82" t="s">
-        <v>23</v>
-      </c>
-      <c r="P82" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>265</v>
-      </c>
-      <c r="R82" t="s">
-        <v>262</v>
       </c>
       <c r="S82">
         <v>38</v>
       </c>
       <c r="T82" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B83" t="s">
         <v>154</v>
@@ -5398,15 +5396,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C84" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F84" t="s">
         <v>20</v>
@@ -5427,39 +5425,39 @@
         <v>0</v>
       </c>
       <c r="L84" t="s">
+        <v>219</v>
+      </c>
+      <c r="M84" t="s">
+        <v>220</v>
+      </c>
+      <c r="N84" t="s">
+        <v>221</v>
+      </c>
+      <c r="O84" t="s">
+        <v>23</v>
+      </c>
+      <c r="P84" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>223</v>
+      </c>
+      <c r="R84" t="s">
         <v>217</v>
-      </c>
-      <c r="M84" t="s">
-        <v>218</v>
-      </c>
-      <c r="N84" t="s">
-        <v>219</v>
-      </c>
-      <c r="O84" t="s">
-        <v>23</v>
-      </c>
-      <c r="P84" t="s">
-        <v>220</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>221</v>
-      </c>
-      <c r="R84" t="s">
-        <v>215</v>
       </c>
       <c r="S84">
         <v>31</v>
       </c>
       <c r="T84" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B85" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F85" t="s">
         <v>50</v>
@@ -5480,34 +5478,34 @@
         <v>0</v>
       </c>
       <c r="L85" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="M85" t="s">
+        <v>240</v>
+      </c>
+      <c r="N85" t="s">
+        <v>233</v>
+      </c>
+      <c r="O85" t="s">
+        <v>23</v>
+      </c>
+      <c r="P85" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>242</v>
+      </c>
+      <c r="R85" t="s">
         <v>238</v>
-      </c>
-      <c r="N85" t="s">
-        <v>231</v>
-      </c>
-      <c r="O85" t="s">
-        <v>23</v>
-      </c>
-      <c r="P85" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>240</v>
-      </c>
-      <c r="R85" t="s">
-        <v>236</v>
       </c>
       <c r="S85">
         <v>34</v>
       </c>
       <c r="T85" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>194</v>
       </c>
@@ -5563,15 +5561,15 @@
         <v>187</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B87" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C87" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F87" t="s">
         <v>50</v>
@@ -5592,34 +5590,34 @@
         <v>0</v>
       </c>
       <c r="L87" t="s">
+        <v>253</v>
+      </c>
+      <c r="M87" t="s">
+        <v>254</v>
+      </c>
+      <c r="N87" t="s">
+        <v>233</v>
+      </c>
+      <c r="O87" t="s">
+        <v>23</v>
+      </c>
+      <c r="P87" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>256</v>
+      </c>
+      <c r="R87" t="s">
         <v>251</v>
-      </c>
-      <c r="M87" t="s">
-        <v>252</v>
-      </c>
-      <c r="N87" t="s">
-        <v>231</v>
-      </c>
-      <c r="O87" t="s">
-        <v>23</v>
-      </c>
-      <c r="P87" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q87" t="s">
-        <v>254</v>
-      </c>
-      <c r="R87" t="s">
-        <v>249</v>
       </c>
       <c r="S87">
         <v>36</v>
       </c>
       <c r="T87" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -5675,9 +5673,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="F89" t="s">
         <v>20</v>
@@ -5698,7 +5696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>181</v>
       </c>
@@ -5754,7 +5752,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>201</v>
       </c>
@@ -5765,7 +5763,7 @@
         <v>203</v>
       </c>
       <c r="E91" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F91" t="s">
         <v>20</v>
@@ -5813,12 +5811,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B92" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="G92" t="b">
         <v>1</v>
@@ -5836,21 +5834,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B93" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D93" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E93" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="F93" t="s">
         <v>50</v>
@@ -5871,10 +5869,10 @@
         <v>0</v>
       </c>
       <c r="L93" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="M93" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="N93" t="s">
         <v>23</v>
@@ -5883,22 +5881,22 @@
         <v>23</v>
       </c>
       <c r="P93" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="Q93" t="s">
         <v>139</v>
       </c>
       <c r="R93" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="S93">
         <v>32</v>
       </c>
       <c r="T93" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>140</v>
       </c>
@@ -5909,10 +5907,10 @@
         <v>142</v>
       </c>
       <c r="D94" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E94" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="F94" t="s">
         <v>50</v>
@@ -5960,7 +5958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>118</v>
       </c>
@@ -5971,10 +5969,10 @@
         <v>120</v>
       </c>
       <c r="D95" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E95" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
@@ -6022,7 +6020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -6033,10 +6031,10 @@
         <v>49</v>
       </c>
       <c r="D96" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E96" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="F96" t="s">
         <v>50</v>
@@ -6084,7 +6082,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>61</v>
       </c>
@@ -6095,7 +6093,7 @@
         <v>63</v>
       </c>
       <c r="E97" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F97" t="s">
         <v>20</v>
@@ -6143,7 +6141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>40</v>
       </c>
@@ -6154,7 +6152,7 @@
         <v>42</v>
       </c>
       <c r="E98" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F98" t="s">
         <v>20</v>
@@ -6202,7 +6200,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -6210,13 +6208,13 @@
         <v>113</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D99" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E99" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="F99" t="s">
         <v>50</v>
@@ -6264,12 +6262,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B100" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="G100" t="b">
         <v>0</v>
@@ -6287,12 +6285,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B101" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="G101" t="b">
         <v>0</v>
@@ -6310,12 +6308,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B102" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="G102" t="b">
         <v>0</v>
@@ -6333,9 +6331,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="G103" t="b">
         <v>0</v>
@@ -6353,12 +6351,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B104" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="G104" t="b">
         <v>0</v>
@@ -6376,9 +6374,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="G105" t="b">
         <v>0</v>
@@ -6396,7 +6394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -6407,10 +6405,10 @@
         <v>99</v>
       </c>
       <c r="D106" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E106" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F106" t="s">
         <v>20</v>
@@ -6458,7 +6456,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>108</v>
       </c>
@@ -6511,7 +6509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>104</v>
       </c>
@@ -6564,7 +6562,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>134</v>
       </c>
@@ -6575,10 +6573,10 @@
         <v>135</v>
       </c>
       <c r="D109" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E109" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="F109" t="s">
         <v>50</v>
@@ -6626,7 +6624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>55</v>
       </c>
@@ -6634,10 +6632,10 @@
         <v>56</v>
       </c>
       <c r="C110" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E110" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="F110" t="s">
         <v>20</v>
@@ -6685,7 +6683,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>34</v>
       </c>
@@ -6693,11 +6691,11 @@
         <v>35</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="F111" t="s">
         <v>20</v>
@@ -6745,7 +6743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -6756,10 +6754,10 @@
         <v>128</v>
       </c>
       <c r="D112" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E112" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F112" t="s">
         <v>50</v>
@@ -6807,7 +6805,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>75</v>
       </c>
@@ -6818,10 +6816,10 @@
         <v>77</v>
       </c>
       <c r="D113" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E113" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F113" t="s">
         <v>20</v>
@@ -6869,7 +6867,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -6877,11 +6875,11 @@
         <v>19</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="F114" t="s">
         <v>20</v>
@@ -6929,7 +6927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>68</v>
       </c>
@@ -6940,10 +6938,10 @@
         <v>70</v>
       </c>
       <c r="D115" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E115" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="F115" t="s">
         <v>20</v>
@@ -6991,7 +6989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>147</v>
       </c>
@@ -7002,7 +7000,7 @@
         <v>149</v>
       </c>
       <c r="E116" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="F116" t="s">
         <v>50</v>
@@ -7050,7 +7048,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -7061,7 +7059,7 @@
         <v>29</v>
       </c>
       <c r="E117" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="F117" t="s">
         <v>20</v>
@@ -7109,7 +7107,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -7120,10 +7118,10 @@
         <v>85</v>
       </c>
       <c r="D118" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E118" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F118" t="s">
         <v>20</v>
@@ -7171,7 +7169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>94</v>
       </c>
@@ -7224,7 +7222,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>90</v>
       </c>

</xml_diff>